<commit_message>
S'han aplicat estils a la vista d'alumnes assignats a professors.
</commit_message>
<xml_diff>
--- a/projecte_assignacio/alumnes/static/files/alumnes_ex.xlsx
+++ b/projecte_assignacio/alumnes/static/files/alumnes_ex.xlsx
@@ -511,7 +511,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Sí</t>
+          <t>SÃ­</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -525,12 +525,12 @@
       <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr">
         <is>
-          <t>[DefaultMunch(None, {'Distancia': 10.6884, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 6, 'Punt de Destí': '', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 36.2399, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Fortaleny', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 4.688, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Massanassa', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 10.6884, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 0, 'Punt de Destí': '', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 12.6795, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 5.5664, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Albal', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 0, 'Punt de Destí': '', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 5.6126000000000005, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 5.6126000000000005, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 0, 'Punt de Destí': '', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': '', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 3, 'Punt de Destí': '', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paiporta', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 5.6126000000000005, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 33.2415, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 9.9916, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': '', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 5.6126000000000005, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 3, 'Punt de Destí': '', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 12.6795, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 59.2648, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Xàtiva', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 14.767700000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 0, 'Punt de Destí': '', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 0, 'Punt de Destí': '', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 9.136899999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Mislata', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 5.6126000000000005, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 12.6795, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 5, 'Punt de Destí': '', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 8, 'Punt de Destí': '', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 4, 'Punt de Destí': '', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 14.767700000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 34.9983, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sueca', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 5.3248, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 12.3171, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 12.6795, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 17.250400000000003, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Foios', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 11, 'Punt de Destí': '', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': '', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 5.3248, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 5, 'Punt de Destí': '', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 24.8037, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Riba Roja', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 12.6795, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': '', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 5.484100000000001, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 12.6795, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 20.614900000000002, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 4.3558, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Benetusser', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 0, 'Punt de Destí': '', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 0, 'Punt de Destí': '', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 12.6795, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 4.729, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sedaví', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 20.614900000000002, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 12.3171, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 7, 'Punt de Destí': '', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 0, 'Punt de Destí': '', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': '', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 3, 'Punt de Destí': '', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 0, 'Punt de Destí': '', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': '', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': '', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 0, 'Punt de Destí': '', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 45.8185, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'Paiporta'})]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>DefaultMunch(None, {'Alumne': 'alumno01', 'Pràctica': 'COLEGIO LA INMACULADA(Pràctica 1)'})</t>
+          <t>DefaultMunch(None, {})</t>
         </is>
       </c>
     </row>
@@ -569,12 +569,12 @@
       <c r="J3" t="inlineStr"/>
       <c r="K3" t="inlineStr">
         <is>
-          <t>[DefaultMunch(None, {'Distancia': 13.6585, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 6, 'Punt de Destí': '', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 39.21, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Fortaleny', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 8.838899999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Massanassa', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 13.6585, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': '', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 9.5609, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 11.084200000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Albal', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': '', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 9.763399999999999, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 9.763399999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': '', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': '', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 3, 'Punt de Destí': '', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 8.2699, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paiporta', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 9.763399999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 28.081599999999998, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 8.0286, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': '', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 9.763399999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 3, 'Punt de Destí': '', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 9.5609, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 62.235, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Xàtiva', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 17.7379, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': '', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': '', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 4.8457, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Mislata', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 9.763399999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 9.5609, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 5, 'Punt de Destí': '', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 8, 'Punt de Destí': '', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 4, 'Punt de Destí': '', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 17.7379, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 37.9684, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sueca', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 7.937600000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 7.3922, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 9.5609, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 10.3509, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Foios', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 11, 'Punt de Destí': '', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': '', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 7.937600000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 5, 'Punt de Destí': '', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 22.5072, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Riba Roja', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 9.5609, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': '', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 10.663799999999998, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 9.5609, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 23.585, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 7.7878, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Benetusser', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': '', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': '', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 9.5609, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 6.9288, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sedaví', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 23.585, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 7.3922, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 7, 'Punt de Destí': '', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': '', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': '', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 3, 'Punt de Destí': '', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': '', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': '', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': '', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': '', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 48.7887, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'VALENCIA'})]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>DefaultMunch(None, {'Alumne': 'alumno02', 'Pràctica': 'Ahora(Pràctica 6)'})</t>
+          <t>DefaultMunch(None, {})</t>
         </is>
       </c>
     </row>
@@ -618,7 +618,7 @@
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>DefaultMunch(None, {'Alumne': 'alumno03', 'Pràctica': 'AEOL(Pràctica 2)'})</t>
+          <t>DefaultMunch(None, {})</t>
         </is>
       </c>
     </row>
@@ -662,7 +662,7 @@
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>DefaultMunch(None, {'Alumne': 'alumno04', 'Pràctica': 'AEOL(Pràctica 1)'})</t>
+          <t>DefaultMunch(None, {})</t>
         </is>
       </c>
     </row>
@@ -701,12 +701,12 @@
       <c r="J6" t="inlineStr"/>
       <c r="K6" t="inlineStr">
         <is>
-          <t>[DefaultMunch(None, {'Distancia': 13.6585, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 6, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 39.21, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Fortaleny', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 8.838899999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Massanassa', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 13.6585, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.5609, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 11.084200000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Albal', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.763399999999999, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.763399999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 3, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 8.2699, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paiporta', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.763399999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 28.081599999999998, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 8.0286, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.763399999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 3, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.5609, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 62.235, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Xàtiva', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 17.7379, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 4.8457, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Mislata', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.763399999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.5609, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 5, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 8, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 4, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 17.7379, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 37.9684, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sueca', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.937600000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.3922, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.5609, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 10.3509, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Foios', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 11, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.937600000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 5, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 22.5072, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Riba Roja', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.5609, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 10.663799999999998, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.5609, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 23.585, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.7878, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Benetusser', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.5609, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 6.9288, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sedaví', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 23.585, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.3922, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 7, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 3, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 48.7887, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'Valencia'})]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>DefaultMunch(None, {'Alumne': 'alumno05', 'Pràctica': 'Ahora(Pràctica 5)'})</t>
+          <t>DefaultMunch(None, {})</t>
         </is>
       </c>
     </row>
@@ -745,12 +745,12 @@
       <c r="J7" t="inlineStr"/>
       <c r="K7" t="inlineStr">
         <is>
-          <t>[DefaultMunch(None, {'Distancia': 71.532, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 67.56139999999999, 'Nombre de Pràctiques': 6, 'Punt de Destí': '', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 92.5077, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Fortaleny', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 70.8532, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Massanassa', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 71.532, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 67.56139999999999, 'Nombre de Pràctiques': 0, 'Punt de Destí': '', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 65.68130000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 73.0985, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Albal', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 67.56139999999999, 'Nombre de Pràctiques': 0, 'Punt de Destí': '', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 71.7777, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 67.56139999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 67.56139999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 67.56139999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 71.7777, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 67.56139999999999, 'Nombre de Pràctiques': 0, 'Punt de Destí': '', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 67.56139999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': '', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 67.56139999999999, 'Nombre de Pràctiques': 3, 'Punt de Destí': '', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 67.50389999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paiporta', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 67.56139999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 71.7777, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 60.6244, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 67.56139999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 61.9137, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 67.56139999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 67.56139999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': '', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 67.56139999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 71.7777, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 67.56139999999999, 'Nombre de Pràctiques': 3, 'Punt de Destí': '', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 65.68130000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 115.5527, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Xàtiva', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 67.8756, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 67.56139999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 67.56139999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 67.56139999999999, 'Nombre de Pràctiques': 0, 'Punt de Destí': '', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 67.56139999999999, 'Nombre de Pràctiques': 0, 'Punt de Destí': '', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 67.56139999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 65.9346, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Mislata', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 67.56139999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 71.7777, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 65.68130000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 67.56139999999999, 'Nombre de Pràctiques': 5, 'Punt de Destí': '', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 67.56139999999999, 'Nombre de Pràctiques': 8, 'Punt de Destí': '', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 67.56139999999999, 'Nombre de Pràctiques': 4, 'Punt de Destí': '', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 67.8756, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 91.26610000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sueca', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 70.7711, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 69.4528, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 65.68130000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 75.1885, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Foios', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 67.56139999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 67.56139999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 67.56139999999999, 'Nombre de Pràctiques': 11, 'Punt de Destí': '', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 67.56139999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': '', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 70.7711, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 67.56139999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 67.56139999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 67.56139999999999, 'Nombre de Pràctiques': 5, 'Punt de Destí': '', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 59.663, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Riba Roja', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 65.68130000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 67.56139999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 67.56139999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 67.56139999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 67.56139999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': '', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 62.7349, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 65.68130000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 76.8827, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 69.80210000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Benetusser', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 67.56139999999999, 'Nombre de Pràctiques': 0, 'Punt de Destí': '', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 67.56139999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 67.56139999999999, 'Nombre de Pràctiques': 0, 'Punt de Destí': '', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 65.68130000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 70.1754, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sedaví', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 67.56139999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 67.56139999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 67.56139999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 67.56139999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 67.56139999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 76.8827, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 69.4528, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 67.56139999999999, 'Nombre de Pràctiques': 7, 'Punt de Destí': '', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 67.56139999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 67.56139999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 67.56139999999999, 'Nombre de Pràctiques': 0, 'Punt de Destí': '', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 67.56139999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': '', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 67.56139999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 67.56139999999999, 'Nombre de Pràctiques': 3, 'Punt de Destí': '', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 67.56139999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 67.56139999999999, 'Nombre de Pràctiques': 0, 'Punt de Destí': '', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 67.56139999999999, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 67.56139999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': '', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 67.56139999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 67.56139999999999, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 67.56139999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': '', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 67.56139999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 67.56139999999999, 'Nombre de Pràctiques': 0, 'Punt de Destí': '', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 67.56139999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 67.56139999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 102.0864, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'Requena'})]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>DefaultMunch(None, {'Alumne': 'alumno06', 'Pràctica': 'Nexo(Pràctica 2)'})</t>
+          <t>DefaultMunch(None, {})</t>
         </is>
       </c>
     </row>
@@ -794,7 +794,7 @@
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>DefaultMunch(None, {'Alumne': 'alumno07', 'Pràctica': 'Ahora(Pràctica 4)'})</t>
+          <t>DefaultMunch(None, {})</t>
         </is>
       </c>
     </row>
@@ -833,12 +833,12 @@
       <c r="J9" t="inlineStr"/>
       <c r="K9" t="inlineStr">
         <is>
-          <t>[DefaultMunch(None, {'Distancia': 13.6585, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 6, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 39.21, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Fortaleny', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 8.838899999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Massanassa', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 13.6585, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.5609, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 11.084200000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Albal', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.763399999999999, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.763399999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 3, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 8.2699, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paiporta', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.763399999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 28.081599999999998, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 8.0286, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.763399999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 3, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.5609, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 62.235, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Xàtiva', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 17.7379, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 4.8457, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Mislata', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.763399999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.5609, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 5, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 8, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 4, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 17.7379, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 37.9684, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sueca', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.937600000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.3922, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.5609, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 10.3509, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Foios', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 11, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.937600000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 5, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 22.5072, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Riba Roja', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.5609, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 10.663799999999998, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.5609, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 23.585, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.7878, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Benetusser', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.5609, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 6.9288, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sedaví', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 23.585, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.3922, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 7, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 3, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 48.7887, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'Valencia'})]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>DefaultMunch(None, {'Alumne': 'alumno08', 'Pràctica': 'Ahora(Pràctica 3)'})</t>
+          <t>DefaultMunch(None, {})</t>
         </is>
       </c>
     </row>
@@ -877,12 +877,12 @@
       <c r="J10" t="inlineStr"/>
       <c r="K10" t="inlineStr">
         <is>
-          <t>[DefaultMunch(None, {'Distancia': 13.6585, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 6, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 39.21, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Fortaleny', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 8.838899999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Massanassa', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 13.6585, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.5609, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 11.084200000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Albal', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.763399999999999, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.763399999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 3, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 8.2699, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paiporta', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.763399999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 28.081599999999998, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 8.0286, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.763399999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 3, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.5609, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 62.235, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Xàtiva', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 17.7379, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 4.8457, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Mislata', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.763399999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.5609, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 5, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 8, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 4, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 17.7379, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 37.9684, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sueca', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.937600000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.3922, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.5609, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 10.3509, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Foios', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 11, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.937600000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 5, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 22.5072, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Riba Roja', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.5609, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 10.663799999999998, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.5609, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 23.585, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.7878, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Benetusser', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.5609, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 6.9288, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sedaví', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 23.585, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.3922, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 7, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 3, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 48.7887, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'Valencia'})]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>DefaultMunch(None, {'Alumne': 'alumno09', 'Pràctica': 'Ahora(Pràctica 2)'})</t>
+          <t>DefaultMunch(None, {})</t>
         </is>
       </c>
     </row>
@@ -926,7 +926,7 @@
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>DefaultMunch(None, {'Alumne': 'alumno10', 'Pràctica': 'Ahora(Pràctica 1)'})</t>
+          <t>DefaultMunch(None, {})</t>
         </is>
       </c>
     </row>
@@ -951,38 +951,26 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>SÃ­</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>DefaultMunch(None, {'BD': 1})</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>FCT</t>
-        </is>
-      </c>
+          <t>DefaultMunch(None, {'Backend': '4', 'Documentacion': '8', 'ERP': '8', 'Moviles': '8', 'Multiplataforma': '6', 'Robotica': '4', 'Videojuegos': '1'})</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr"/>
       <c r="H12" t="inlineStr"/>
-      <c r="I12" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="J12" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
+      <c r="I12" t="inlineStr"/>
+      <c r="J12" t="inlineStr"/>
       <c r="K12" t="inlineStr">
         <is>
-          <t>[DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 6, 'Punt de Destí': '', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 27.0358, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Fortaleny', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 7.373, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Massanassa', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 0, 'Punt de Destí': '', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 21.266099999999998, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 7.2438, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Albal', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 0, 'Punt de Destí': '', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 6.5558000000000005, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 6.5558000000000005, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 0, 'Punt de Destí': '', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 2, 'Punt de Destí': '', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 3, 'Punt de Destí': '', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 10.4937, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paiporta', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 6.5558000000000005, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 41.8281, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 18.575200000000002, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 2, 'Punt de Destí': '', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 6.5558000000000005, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 3, 'Punt de Destí': '', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 21.266099999999998, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 50.0608, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Xàtiva', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 5.144399999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 0, 'Punt de Destí': '', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 0, 'Punt de Destí': '', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 17.7205, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Mislata', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 6.5558000000000005, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 21.266099999999998, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 5, 'Punt de Destí': '', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 8, 'Punt de Destí': '', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 4, 'Punt de Destí': '', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 5.144399999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 25.7942, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sueca', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 8.857899999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 22.5564, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 21.266099999999998, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 23.5319, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Foios', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 11, 'Punt de Destí': '', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 2, 'Punt de Destí': '', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 8.857899999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 5, 'Punt de Destí': '', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 32.7965, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Riba Roja', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 21.266099999999998, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 2, 'Punt de Destí': '', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9925, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 21.266099999999998, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 11.4108, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 8.9062, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Benetusser', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 0, 'Punt de Destí': '', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 0, 'Punt de Destí': '', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 21.266099999999998, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 8.9831, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sedaví', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 11.4108, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 22.5564, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 7, 'Punt de Destí': '', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 0, 'Punt de Destí': '', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 2, 'Punt de Destí': '', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 3, 'Punt de Destí': '', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 0, 'Punt de Destí': '', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 2, 'Punt de Destí': '', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 2, 'Punt de Destí': '', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 0, 'Punt de Destí': '', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 36.6145, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'Silla'})]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>DefaultMunch(None, {'Alumne': 'alumno11', 'Pràctica': 'Atmosfera Sport(Pràctica 2)'})</t>
+          <t>DefaultMunch(None, {})</t>
         </is>
       </c>
     </row>
@@ -1021,12 +1009,12 @@
       <c r="J13" t="inlineStr"/>
       <c r="K13" t="inlineStr">
         <is>
-          <t>[DefaultMunch(None, {'Distancia': 8.6265, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776, 'Nombre de Pràctiques': 6, 'Punt de Destí': '', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 34.1779, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Fortaleny', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 1.7895, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Massanassa', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 8.6265, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776, 'Nombre de Pràctiques': 0, 'Punt de Destí': '', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 12.707, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 4.5935, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Albal', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776, 'Nombre de Pràctiques': 0, 'Punt de Destí': '', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 2.7140999999999997, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 2.7140999999999997, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776, 'Nombre de Pràctiques': 0, 'Punt de Destí': '', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776, 'Nombre de Pràctiques': 2, 'Punt de Destí': '', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776, 'Nombre de Pràctiques': 3, 'Punt de Destí': '', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 2.6365, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paiporta', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 2.7140999999999997, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 33.2689, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 10.0191, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776, 'Nombre de Pràctiques': 2, 'Punt de Destí': '', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 2.7140999999999997, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776, 'Nombre de Pràctiques': 3, 'Punt de Destí': '', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 12.707, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 57.2029, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Xàtiva', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 12.7058, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776, 'Nombre de Pràctiques': 0, 'Punt de Destí': '', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776, 'Nombre de Pràctiques': 0, 'Punt de Destí': '', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 9.164399999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Mislata', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 2.7140999999999997, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 12.707, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776, 'Nombre de Pràctiques': 5, 'Punt de Destí': '', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776, 'Nombre de Pràctiques': 8, 'Punt de Destí': '', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776, 'Nombre de Pràctiques': 4, 'Punt de Destí': '', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 12.7058, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 32.9363, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sueca', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 1.8020999999999998, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 12.7458, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 12.707, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 16.596799999999998, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Foios', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776, 'Nombre de Pràctiques': 11, 'Punt de Destí': '', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776, 'Nombre de Pràctiques': 2, 'Punt de Destí': '', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 1.8020999999999998, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776, 'Nombre de Pràctiques': 5, 'Punt de Destí': '', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 24.8312, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Riba Roja', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 12.707, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776, 'Nombre de Pràctiques': 2, 'Punt de Destí': '', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 8.5693, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 12.707, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 18.5529, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Benetusser', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776, 'Nombre de Pràctiques': 0, 'Punt de Destí': '', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776, 'Nombre de Pràctiques': 0, 'Punt de Destí': '', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 12.707, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 2.6141, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sedaví', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 18.5529, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 12.7458, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776, 'Nombre de Pràctiques': 7, 'Punt de Destí': '', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776, 'Nombre de Pràctiques': 0, 'Punt de Destí': '', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776, 'Nombre de Pràctiques': 2, 'Punt de Destí': '', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776, 'Nombre de Pràctiques': 3, 'Punt de Destí': '', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776, 'Nombre de Pràctiques': 0, 'Punt de Destí': '', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776, 'Nombre de Pràctiques': 2, 'Punt de Destí': '', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776, 'Nombre de Pràctiques': 2, 'Punt de Destí': '', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776, 'Nombre de Pràctiques': 0, 'Punt de Destí': '', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 43.7566, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'Benetusser'})]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>DefaultMunch(None, {'Alumne': 'alumno12', 'Pràctica': 'Ricardo Gomez Lara '})</t>
+          <t>DefaultMunch(None, {})</t>
         </is>
       </c>
     </row>
@@ -1065,12 +1053,12 @@
       <c r="J14" t="inlineStr"/>
       <c r="K14" t="inlineStr">
         <is>
-          <t>[DefaultMunch(None, {'Distancia': 13.950899999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 6, 'Punt de Destí': '', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 23.9937, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Fortaleny', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 20.3081, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Massanassa', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 13.950899999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 0, 'Punt de Destí': '', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 34.2012, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 20.178900000000002, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Albal', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 0, 'Punt de Destí': '', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 19.4909, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 19.4909, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 0, 'Punt de Destí': '', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 2, 'Punt de Destí': '', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 3, 'Punt de Destí': '', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 23.4287, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paiporta', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 19.4909, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 57.2663, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 31.5103, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 2, 'Punt de Destí': '', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 19.4909, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 3, 'Punt de Destí': '', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 34.2012, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 35.7939, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Xàtiva', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 15.867700000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 0, 'Punt de Destí': '', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 0, 'Punt de Destí': '', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 30.6556, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Mislata', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 19.4909, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 34.2012, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 5, 'Punt de Destí': '', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 8, 'Punt de Destí': '', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 4, 'Punt de Destí': '', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 15.867700000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 21.3029, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sueca', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 21.792900000000003, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 35.4914, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 34.2012, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 36.467, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Foios', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 11, 'Punt de Destí': '', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 2, 'Punt de Destí': '', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 21.792900000000003, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 5, 'Punt de Destí': '', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 41.643699999999995, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Riba Roja', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 34.2012, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 2, 'Punt de Destí': '', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 25.6662, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 34.2012, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 7.9038, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 21.8412, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Benetusser', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 0, 'Punt de Destí': '', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 0, 'Punt de Destí': '', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 34.2012, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 21.9181, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sedaví', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 7.9038, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 35.4914, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 7, 'Punt de Destí': '', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 0, 'Punt de Destí': '', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 2, 'Punt de Destí': '', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 3, 'Punt de Destí': '', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 0, 'Punt de Destí': '', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 2, 'Punt de Destí': '', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 2, 'Punt de Destí': '', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 0, 'Punt de Destí': '', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 33.5724, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'Alginet'})]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>DefaultMunch(None, {'Alumne': 'alumno13', 'Pràctica': 'Red902(Pràctica 2)'})</t>
+          <t>DefaultMunch(None, {})</t>
         </is>
       </c>
     </row>
@@ -1109,12 +1097,12 @@
       <c r="J15" t="inlineStr"/>
       <c r="K15" t="inlineStr">
         <is>
-          <t>[DefaultMunch(None, {'Distancia': 13.950899999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 6, 'Punt de Destí': '', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 23.9937, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Fortaleny', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 20.3081, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Massanassa', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 13.950899999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 0, 'Punt de Destí': '', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 34.2012, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 20.178900000000002, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Albal', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 0, 'Punt de Destí': '', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 19.4909, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 19.4909, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 0, 'Punt de Destí': '', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 2, 'Punt de Destí': '', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 3, 'Punt de Destí': '', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 23.4287, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paiporta', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 19.4909, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 57.2663, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 31.5103, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 2, 'Punt de Destí': '', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 19.4909, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 3, 'Punt de Destí': '', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 34.2012, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 35.7939, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Xàtiva', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 15.867700000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 0, 'Punt de Destí': '', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 0, 'Punt de Destí': '', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 30.6556, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Mislata', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 19.4909, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 34.2012, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 5, 'Punt de Destí': '', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 8, 'Punt de Destí': '', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 4, 'Punt de Destí': '', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 15.867700000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 21.3029, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sueca', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 21.792900000000003, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 35.4914, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 34.2012, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 36.467, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Foios', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 11, 'Punt de Destí': '', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 2, 'Punt de Destí': '', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 21.792900000000003, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 5, 'Punt de Destí': '', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 41.643699999999995, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Riba Roja', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 34.2012, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 2, 'Punt de Destí': '', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 25.6662, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 34.2012, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 7.9038, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 21.8412, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Benetusser', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 0, 'Punt de Destí': '', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 0, 'Punt de Destí': '', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 34.2012, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 21.9181, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sedaví', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 7.9038, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 35.4914, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 7, 'Punt de Destí': '', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 0, 'Punt de Destí': '', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 2, 'Punt de Destí': '', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 3, 'Punt de Destí': '', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 0, 'Punt de Destí': '', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 2, 'Punt de Destí': '', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 2, 'Punt de Destí': '', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 0, 'Punt de Destí': '', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 33.5724, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'Alginet'})]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>DefaultMunch(None, {'Alumne': 'alumno14', 'Pràctica': 'Red902(Pràctica 1)'})</t>
+          <t>DefaultMunch(None, {})</t>
         </is>
       </c>
     </row>
@@ -1153,12 +1141,12 @@
       <c r="J16" t="inlineStr"/>
       <c r="K16" t="inlineStr">
         <is>
-          <t>[DefaultMunch(None, {'Distancia': 6.1035, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2912, 'Nombre de Pràctiques': 6, 'Punt de Destí': '', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 31.6549, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Fortaleny', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 1.2002000000000002, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Massanassa', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 6.1035, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2912, 'Nombre de Pràctiques': 0, 'Punt de Destí': '', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 15.2222, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 2.0949, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Albal', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2912, 'Nombre de Pràctiques': 0, 'Punt de Destí': '', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2912, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2912, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2912, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2912, 'Nombre de Pràctiques': 0, 'Punt de Destí': '', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2912, 'Nombre de Pràctiques': 2, 'Punt de Destí': '', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2912, 'Nombre de Pràctiques': 3, 'Punt de Destí': '', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 5.1517, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paiporta', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2912, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 35.784099999999995, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2912, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 12.5343, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2912, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2912, 'Nombre de Pràctiques': 2, 'Punt de Destí': '', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2912, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2912, 'Nombre de Pràctiques': 3, 'Punt de Destí': '', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 15.2222, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 54.6799, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Xàtiva', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 10.182799999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2912, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2912, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2912, 'Nombre de Pràctiques': 0, 'Punt de Destí': '', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2912, 'Nombre de Pràctiques': 0, 'Punt de Destí': '', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2912, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 11.6796, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Mislata', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2912, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 15.2222, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2912, 'Nombre de Pràctiques': 5, 'Punt de Destí': '', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2912, 'Nombre de Pràctiques': 8, 'Punt de Destí': '', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2912, 'Nombre de Pràctiques': 4, 'Punt de Destí': '', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 10.182799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 30.4133, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sueca', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 3.3274, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 15.261, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 15.2222, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 19.112, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Foios', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2912, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2912, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2912, 'Nombre de Pràctiques': 11, 'Punt de Destí': '', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2912, 'Nombre de Pràctiques': 2, 'Punt de Destí': '', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 3.3274, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2912, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2912, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2912, 'Nombre de Pràctiques': 5, 'Punt de Destí': '', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 27.346400000000003, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Riba Roja', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 15.2222, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2912, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2912, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2912, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2912, 'Nombre de Pràctiques': 2, 'Punt de Destí': '', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 10.5417, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 15.2222, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 16.0299, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 2.7334, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Benetusser', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2912, 'Nombre de Pràctiques': 0, 'Punt de Destí': '', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2912, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2912, 'Nombre de Pràctiques': 0, 'Punt de Destí': '', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 15.2222, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 4.2168, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sedaví', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2912, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2912, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2912, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2912, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2912, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 16.0299, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 15.261, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2912, 'Nombre de Pràctiques': 7, 'Punt de Destí': '', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2912, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2912, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2912, 'Nombre de Pràctiques': 0, 'Punt de Destí': '', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2912, 'Nombre de Pràctiques': 2, 'Punt de Destí': '', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2912, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2912, 'Nombre de Pràctiques': 3, 'Punt de Destí': '', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2912, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2912, 'Nombre de Pràctiques': 0, 'Punt de Destí': '', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2912, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2912, 'Nombre de Pràctiques': 2, 'Punt de Destí': '', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2912, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2912, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2912, 'Nombre de Pràctiques': 2, 'Punt de Destí': '', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2912, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2912, 'Nombre de Pràctiques': 0, 'Punt de Destí': '', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2912, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2912, 'Nombre de Pràctiques': 1, 'Punt de Destí': '', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 41.233599999999996, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'Catarroja'})]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>DefaultMunch(None, {'Alumne': 'alumno15', 'Pràctica': 'Cesumin(Pràctica 1)'})</t>
+          <t>DefaultMunch(None, {})</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
El TFG ja s'ha presentat.
</commit_message>
<xml_diff>
--- a/projecte_assignacio/alumnes/static/files/alumnes_ex.xlsx
+++ b/projecte_assignacio/alumnes/static/files/alumnes_ex.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L16"/>
+  <dimension ref="A1:L61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -511,7 +511,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>SÃ­</t>
+          <t>Si</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -525,12 +525,12 @@
       <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[DefaultMunch(None, {'Distancia': 10.6884, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 6, 'Punt de Destí': 'Valencia', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 36.2399, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Fortaleny', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 4.6883, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Massanassa', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 10.6884, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Valencia', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 12.6795, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 5.5664, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Albal', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 33.2415, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 5.6128, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 9.9916, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 5.6128, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 5.3247, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 12.6795, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'València', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paiporta', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 5.6128, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 33.2415, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 9.9916, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 33.136199999999995, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Algemesí', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 5.3247, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 12.6795, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 5.6128, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 370.2797, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Pozuelo de Alarcón', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 12.6795, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 59.2648, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Xàtiva', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 14.767700000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 14.767700000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 32.4708, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Benisanó', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 33.3842, 'Nombre de Pràctiques': 1, 'Punt de Destí': "L'Alcúdia", 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 9.136899999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Mislata', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 5.484100000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 5.6128, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 12.6795, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 12.6795, 'Nombre de Pràctiques': 5, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 8, 'Punt de Destí': 'València', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 4, 'Punt de Destí': 'València', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 14.767700000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 34.9983, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sueca', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 5.3247, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 12.3171, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 12.6795, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 17.250400000000003, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Foios', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 6.9689, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Alaquas', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 11, 'Punt de Destí': 'València', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 5.3247, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 5, 'Punt de Destí': 'València', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 24.8687, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Riba Roja', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 12.6795, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 10.6884, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 968.8234, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 5.484100000000001, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 12.6795, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 20.614900000000002, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 4.3557, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Benetusser', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 170.9496, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Elche', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 12.6795, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 4.7298, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sedaví', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 20.614900000000002, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 12.3171, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 27.6094, 'Nombre de Pràctiques': 7, 'Punt de Destí': 'Rafelbunyol', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 20.614900000000002, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 34.5298, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Guadassuar', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 66.7536, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Gandía', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 66.7536, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Gandía', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'València', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 5.484100000000001, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 12.6795, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 14.767700000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 374.057, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Montcada i Reixac', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 12.6795, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 968.8234, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'Paiporta'})]</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>DefaultMunch(None, {})</t>
+          <t>DefaultMunch(None, {'Alumne': 'alumno01', 'Pràctica': 'COLEGIO LA INMACULADA(Pràctica 1)'})</t>
         </is>
       </c>
     </row>
@@ -555,7 +555,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>SÃ­</t>
+          <t>Si</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -569,12 +569,12 @@
       <c r="J3" t="inlineStr"/>
       <c r="K3" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[DefaultMunch(None, {'Distancia': 13.6585, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 6, 'Punt de Destí': 'Valencia', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 39.21, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Fortaleny', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 8.8391, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Massanassa', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 13.6585, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Valencia', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 11.0844, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Albal', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 28.0815, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 9.7637, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 8.0286, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 9.7637, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 7.937600000000001, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'València', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 8.2699, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paiporta', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 9.7637, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 28.0815, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 8.0286, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 36.1064, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Algemesí', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 7.937600000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 9.7637, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 367.69440000000003, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Pozuelo de Alarcón', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 62.235, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Xàtiva', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 17.7379, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 17.7379, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 27.3108, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Benisanó', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 36.3544, 'Nombre de Pràctiques': 1, 'Punt de Destí': "L'Alcúdia", 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 4.8457, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Mislata', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 10.663799999999998, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 9.7637, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 5, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 8, 'Punt de Destí': 'València', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 4, 'Punt de Destí': 'València', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 17.7379, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 37.9684, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sueca', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 7.937600000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 7.3887, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 10.3529, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Foios', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 10.22, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Alaquas', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 11, 'Punt de Destí': 'València', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 7.937600000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 5, 'Punt de Destí': 'València', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 22.5721, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Riba Roja', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 13.6585, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Silla', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 966.2381, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 10.663799999999998, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 23.585, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 7.7878, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Benetusser', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 173.9197, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Elche', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 6.9288, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sedaví', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 23.585, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 7.3887, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 19.881400000000003, 'Nombre de Pràctiques': 7, 'Punt de Destí': 'Rafelbunyol', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 23.585, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 37.499900000000004, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Guadassuar', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 69.7237, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Gandía', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 69.7237, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Gandía', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'València', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 10.663799999999998, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 17.7379, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 361.05379999999997, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Montcada i Reixac', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'VALENCIA'}), DefaultMunch(None, {'Distancia': 966.2381, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'VALENCIA'})]</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>DefaultMunch(None, {})</t>
+          <t>DefaultMunch(None, {'Alumne': 'alumno02', 'Pràctica': 'YMANT(Pràctica 1)'})</t>
         </is>
       </c>
     </row>
@@ -594,7 +594,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>AlgemesÃ­</t>
+          <t>Algemesi</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -613,12 +613,12 @@
       <c r="J4" t="inlineStr"/>
       <c r="K4" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[DefaultMunch(None, {'Distancia': 23.3551, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 35.9315, 'Nombre de Pràctiques': 6, 'Punt de Destí': 'Valencia', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 12.055, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Fortaleny', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 29.7122, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Massanassa', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 23.3551, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 35.9315, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Valencia', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 43.2173, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 29.583, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Albal', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 66.6484, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 28.895, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 35.9315, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 35.9315, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 40.5264, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 28.895, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 30.809, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 43.2173, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 35.9315, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'València', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 33.276199999999996, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paiporta', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 35.9315, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 28.895, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 66.6484, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 35.9315, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 40.5264, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Algemesí', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 30.809, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 43.2173, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 28.895, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 389.9939, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Pozuelo de Alarcón', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 43.2173, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 33.8352, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Xàtiva', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 25.2359, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 35.9315, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 25.2359, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 35.9315, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 65.87769999999999, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Benisanó', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 7.87, 'Nombre de Pràctiques': 1, 'Punt de Destí': "L'Alcúdia", 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 39.671699999999994, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Mislata', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 35.048199999999994, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 28.895, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 43.2173, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 43.2173, 'Nombre de Pràctiques': 5, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 35.9315, 'Nombre de Pràctiques': 8, 'Punt de Destí': 'València', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 35.9315, 'Nombre de Pràctiques': 4, 'Punt de Destí': 'València', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 25.2359, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 12.5734, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sueca', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 30.809, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 44.5076, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 43.2173, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 45.485, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Foios', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 37.517199999999995, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Alaquas', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 35.9315, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 35.9315, 'Nombre de Pràctiques': 11, 'Punt de Destí': 'València', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 35.9315, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 30.809, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 35.9315, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 35.9315, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 35.9315, 'Nombre de Pràctiques': 5, 'Punt de Destí': 'València', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 51.085300000000004, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Riba Roja', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 43.2173, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 35.9315, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 35.9315, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 23.3551, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 946.8343000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 35.048199999999994, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 43.2173, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 13.41, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 30.8573, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Benetusser', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 145.5199, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Elche', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 35.9315, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 35.9315, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 43.2173, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 30.9342, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sedaví', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 35.9315, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 35.9315, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 35.9315, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 35.9315, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 35.9315, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 13.41, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 44.5076, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 65.7825, 'Nombre de Pràctiques': 7, 'Punt de Destí': 'Rafelbunyol', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 35.9315, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 13.41, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 4.868, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Guadassuar', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 39.7578, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Gandía', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 39.7578, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Gandía', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 35.9315, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'València', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 35.9315, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 35.048199999999994, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 35.9315, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 35.9315, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 35.9315, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 35.9315, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 43.2173, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 25.2359, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 35.9315, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 405.7919, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Montcada i Reixac', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 43.2173, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 946.8343000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'Algemesi'})]</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>DefaultMunch(None, {})</t>
+          <t>DefaultMunch(None, {'Alumne': 'alumno03', 'Pràctica': 'Disai Automoción(Pràctica 1)'})</t>
         </is>
       </c>
     </row>
@@ -638,12 +638,12 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>AlaquÃ s</t>
+          <t>Alaquas</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>SÃ­</t>
+          <t>Si</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -657,12 +657,12 @@
       <c r="J5" t="inlineStr"/>
       <c r="K5" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[DefaultMunch(None, {'Distancia': 16.0995, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Alaquas'}), DefaultMunch(None, {'Distancia': 9.1359, 'Nombre de Pràctiques': 6, 'Punt de Destí': 'Valencia', 'Punt de Partida': 'Alaquas'}), DefaultMunch(None, {'Distancia': 41.280699999999996, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Fortaleny', 'Punt de Partida': 'Alaquas'}), DefaultMunch(None, {'Distancia': 11.0385, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Massanassa', 'Punt de Partida': 'Alaquas'}), DefaultMunch(None, {'Distancia': 16.0995, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Alaquas'}), DefaultMunch(None, {'Distancia': 9.1359, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Valencia', 'Punt de Partida': 'Alaquas'}), DefaultMunch(None, {'Distancia': 7.9505, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Alaquas'}), DefaultMunch(None, {'Distancia': 11.221200000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Albal', 'Punt de Partida': 'Alaquas'}), DefaultMunch(None, {'Distancia': 31.613599999999998, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'Alaquas'}), DefaultMunch(None, {'Distancia': 11.963, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Alaquas'}), DefaultMunch(None, {'Distancia': 9.1359, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Alaquas'}), DefaultMunch(None, {'Distancia': 9.1359, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Alaquas'}), DefaultMunch(None, {'Distancia': 4.2501999999999995, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'Alaquas'}), DefaultMunch(None, {'Distancia': 11.963, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Alaquas'}), DefaultMunch(None, {'Distancia': 10.956100000000001, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Alaquas'}), DefaultMunch(None, {'Distancia': 7.9505, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Alaquas'}), DefaultMunch(None, {'Distancia': 9.1359, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'València', 'Punt de Partida': 'Alaquas'}), DefaultMunch(None, {'Distancia': 7.331300000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paiporta', 'Punt de Partida': 'Alaquas'}), DefaultMunch(None, {'Distancia': 9.1359, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Alaquas'}), DefaultMunch(None, {'Distancia': 11.963, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Alaquas'}), DefaultMunch(None, {'Distancia': 31.613599999999998, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'Alaquas'}), DefaultMunch(None, {'Distancia': 9.1359, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Alaquas'}), DefaultMunch(None, {'Distancia': 4.2501999999999995, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'Alaquas'}), DefaultMunch(None, {'Distancia': 38.177099999999996, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Algemesí', 'Punt de Partida': 'Alaquas'}), DefaultMunch(None, {'Distancia': 10.956100000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Alaquas'}), DefaultMunch(None, {'Distancia': 7.9505, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Alaquas'}), DefaultMunch(None, {'Distancia': 11.963, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Alaquas'}), DefaultMunch(None, {'Distancia': 362.014, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Pozuelo de Alarcón', 'Punt de Partida': 'Alaquas'}), DefaultMunch(None, {'Distancia': 7.9505, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Alaquas'}), DefaultMunch(None, {'Distancia': 64.6759, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Xàtiva', 'Punt de Partida': 'Alaquas'}), DefaultMunch(None, {'Distancia': 16.6486, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Alaquas'}), DefaultMunch(None, {'Distancia': 9.1359, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Alaquas'}), DefaultMunch(None, {'Distancia': 16.6486, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Alaquas'}), DefaultMunch(None, {'Distancia': 9.1359, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Alaquas'}), DefaultMunch(None, {'Distancia': 30.843, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Benisanó', 'Punt de Partida': 'Alaquas'}), DefaultMunch(None, {'Distancia': 38.795300000000005, 'Nombre de Pràctiques': 1, 'Punt de Destí': "L'Alcúdia", 'Punt de Partida': 'Alaquas'}), DefaultMunch(None, {'Distancia': 7.5091, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Mislata', 'Punt de Partida': 'Alaquas'}), DefaultMunch(None, {'Distancia': 3.1399, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Alaquas'}), DefaultMunch(None, {'Distancia': 11.963, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Alaquas'}), DefaultMunch(None, {'Distancia': 7.9505, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Alaquas'}), DefaultMunch(None, {'Distancia': 7.9505, 'Nombre de Pràctiques': 5, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Alaquas'}), DefaultMunch(None, {'Distancia': 9.1359, 'Nombre de Pràctiques': 8, 'Punt de Destí': 'València', 'Punt de Partida': 'Alaquas'}), DefaultMunch(None, {'Distancia': 9.1359, 'Nombre de Pràctiques': 4, 'Punt de Destí': 'València', 'Punt de Partida': 'Alaquas'}), DefaultMunch(None, {'Distancia': 16.6486, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Alaquas'}), DefaultMunch(None, {'Distancia': 40.0391, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sueca', 'Punt de Partida': 'Alaquas'}), DefaultMunch(None, {'Distancia': 10.956100000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Alaquas'}), DefaultMunch(None, {'Distancia': 12.341899999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Alaquas'}), DefaultMunch(None, {'Distancia': 7.9505, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Alaquas'}), DefaultMunch(None, {'Distancia': 16.763099999999998, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Foios', 'Punt de Partida': 'Alaquas'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Alaquas', 'Punt de Partida': 'Alaquas'}), DefaultMunch(None, {'Distancia': 9.1359, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Alaquas'}), DefaultMunch(None, {'Distancia': 9.1359, 'Nombre de Pràctiques': 11, 'Punt de Destí': 'València', 'Punt de Partida': 'Alaquas'}), DefaultMunch(None, {'Distancia': 9.1359, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Alaquas'}), DefaultMunch(None, {'Distancia': 10.956100000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Alaquas'}), DefaultMunch(None, {'Distancia': 9.1359, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Alaquas'}), DefaultMunch(None, {'Distancia': 9.1359, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Alaquas'}), DefaultMunch(None, {'Distancia': 9.1359, 'Nombre de Pràctiques': 5, 'Punt de Destí': 'València', 'Punt de Partida': 'Alaquas'}), DefaultMunch(None, {'Distancia': 17.2001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Riba Roja', 'Punt de Partida': 'Alaquas'}), DefaultMunch(None, {'Distancia': 7.9505, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Alaquas'}), DefaultMunch(None, {'Distancia': 9.1359, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Alaquas'}), DefaultMunch(None, {'Distancia': 9.1359, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Alaquas'}), DefaultMunch(None, {'Distancia': 16.0995, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Alaquas'}), DefaultMunch(None, {'Distancia': 960.5577, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'Alaquas'}), DefaultMunch(None, {'Distancia': 3.1399, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Alaquas'}), DefaultMunch(None, {'Distancia': 7.9505, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Alaquas'}), DefaultMunch(None, {'Distancia': 25.6557, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Alaquas'}), DefaultMunch(None, {'Distancia': 9.9871, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Benetusser', 'Punt de Partida': 'Alaquas'}), DefaultMunch(None, {'Distancia': 176.3606, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Elche', 'Punt de Partida': 'Alaquas'}), DefaultMunch(None, {'Distancia': 9.1359, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Alaquas'}), DefaultMunch(None, {'Distancia': 9.1359, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Alaquas'}), DefaultMunch(None, {'Distancia': 7.9505, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Alaquas'}), DefaultMunch(None, {'Distancia': 10.3612, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sedaví', 'Punt de Partida': 'Alaquas'}), DefaultMunch(None, {'Distancia': 9.1359, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Alaquas'}), DefaultMunch(None, {'Distancia': 9.1359, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Alaquas'}), DefaultMunch(None, {'Distancia': 9.1359, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Alaquas'}), DefaultMunch(None, {'Distancia': 9.1359, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Alaquas'}), DefaultMunch(None, {'Distancia': 9.1359, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Alaquas'}), DefaultMunch(None, {'Distancia': 25.6557, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Alaquas'}), DefaultMunch(None, {'Distancia': 12.341899999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Alaquas'}), DefaultMunch(None, {'Distancia': 29.6459, 'Nombre de Pràctiques': 7, 'Punt de Destí': 'Rafelbunyol', 'Punt de Partida': 'Alaquas'}), DefaultMunch(None, {'Distancia': 9.1359, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Alaquas'}), DefaultMunch(None, {'Distancia': 25.6557, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Alaquas'}), DefaultMunch(None, {'Distancia': 39.9409, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Guadassuar', 'Punt de Partida': 'Alaquas'}), DefaultMunch(None, {'Distancia': 71.7944, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Gandía', 'Punt de Partida': 'Alaquas'}), DefaultMunch(None, {'Distancia': 71.7944, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Gandía', 'Punt de Partida': 'Alaquas'}), DefaultMunch(None, {'Distancia': 9.1359, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'València', 'Punt de Partida': 'Alaquas'}), DefaultMunch(None, {'Distancia': 9.1359, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Alaquas'}), DefaultMunch(None, {'Distancia': 3.1399, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Alaquas'}), DefaultMunch(None, {'Distancia': 9.1359, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Alaquas'}), DefaultMunch(None, {'Distancia': 9.1359, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Alaquas'}), DefaultMunch(None, {'Distancia': 9.1359, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Alaquas'}), DefaultMunch(None, {'Distancia': 9.1359, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Alaquas'}), DefaultMunch(None, {'Distancia': 7.9505, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Alaquas'}), DefaultMunch(None, {'Distancia': 16.6486, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Alaquas'}), DefaultMunch(None, {'Distancia': 9.1359, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Alaquas'}), DefaultMunch(None, {'Distancia': 369.6553, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Montcada i Reixac', 'Punt de Partida': 'Alaquas'}), DefaultMunch(None, {'Distancia': 7.9505, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Alaquas'}), DefaultMunch(None, {'Distancia': 960.5577, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'Alaquas'})]</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>DefaultMunch(None, {})</t>
+          <t>DefaultMunch(None, {'Alumne': 'alumno04', 'Pràctica': 'Jumping in the Virtual System(Pràctica 1)'})</t>
         </is>
       </c>
     </row>
@@ -687,7 +687,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>SÃ­</t>
+          <t>Si</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -701,12 +701,12 @@
       <c r="J6" t="inlineStr"/>
       <c r="K6" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[DefaultMunch(None, {'Distancia': 13.6585, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 6, 'Punt de Destí': 'Valencia', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 39.21, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Fortaleny', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 8.8391, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Massanassa', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 13.6585, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Valencia', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 11.0844, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Albal', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 28.0815, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.7637, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 8.0286, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.7637, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.937600000000001, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 8.2699, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paiporta', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.7637, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 28.0815, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 8.0286, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 36.1064, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Algemesí', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.937600000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.7637, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 367.69440000000003, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Pozuelo de Alarcón', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 62.235, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Xàtiva', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 17.7379, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 17.7379, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 27.3108, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Benisanó', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 36.3544, 'Nombre de Pràctiques': 1, 'Punt de Destí': "L'Alcúdia", 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 4.8457, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Mislata', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 10.663799999999998, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.7637, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 5, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 8, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 4, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 17.7379, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 37.9684, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sueca', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.937600000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.3887, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 10.3529, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Foios', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 10.22, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Alaquas', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 11, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.937600000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 5, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 22.5721, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Riba Roja', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 13.6585, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 966.2381, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 10.663799999999998, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 23.585, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.7878, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Benetusser', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 173.9197, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Elche', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 6.9288, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sedaví', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 23.585, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.3887, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 19.881400000000003, 'Nombre de Pràctiques': 7, 'Punt de Destí': 'Rafelbunyol', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 23.585, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 37.499900000000004, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Guadassuar', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 69.7237, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Gandía', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 69.7237, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Gandía', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 10.663799999999998, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 17.7379, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 361.05379999999997, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Montcada i Reixac', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 966.2381, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'Valencia'})]</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>DefaultMunch(None, {})</t>
+          <t>DefaultMunch(None, {'Alumne': 'alumno05', 'Pràctica': 'Onestic(Pràctica 1)'})</t>
         </is>
       </c>
     </row>
@@ -745,12 +745,12 @@
       <c r="J7" t="inlineStr"/>
       <c r="K7" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[DefaultMunch(None, {'Distancia': 71.532, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 67.56139999999999, 'Nombre de Pràctiques': 6, 'Punt de Destí': 'Valencia', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 92.5077, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Fortaleny', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 70.8534, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Massanassa', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 71.532, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 67.56139999999999, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Valencia', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 65.68130000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 73.0987, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Albal', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 60.6259, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 71.77789999999999, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 67.56139999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 67.56139999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 61.9137, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 71.77789999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 70.7711, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 65.68130000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 67.56139999999999, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'València', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 67.50389999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paiporta', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 67.56139999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 71.77789999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 60.6259, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 67.56139999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 61.9137, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 89.4041, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Algemesí', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 70.7711, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 65.68130000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 71.77789999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 300.9108, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Pozuelo de Alarcón', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 65.68130000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 115.5527, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Xàtiva', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 67.8756, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 67.56139999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 67.8756, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 67.56139999999999, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 61.4647, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Benisanó', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 89.6721, 'Nombre de Pràctiques': 1, 'Punt de Destí': "L'Alcúdia", 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 65.9345, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Mislata', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 62.7349, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 71.77789999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 65.68130000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 65.68130000000001, 'Nombre de Pràctiques': 5, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 67.56139999999999, 'Nombre de Pràctiques': 8, 'Punt de Destí': 'València', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 67.56139999999999, 'Nombre de Pràctiques': 4, 'Punt de Destí': 'València', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 67.8756, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 91.26610000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sueca', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 70.7711, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 69.4528, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 65.68130000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 75.1885, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Foios', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 61.5154, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Alaquas', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 67.56139999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 67.56139999999999, 'Nombre de Pràctiques': 11, 'Punt de Destí': 'València', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 67.56139999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 70.7711, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 67.56139999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 67.56139999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 67.56139999999999, 'Nombre de Pràctiques': 5, 'Punt de Destí': 'València', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 59.6629, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Riba Roja', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 65.68130000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 67.56139999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 67.56139999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 71.532, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 899.4545, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 62.7349, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 65.68130000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 76.8827, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 69.80210000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Benetusser', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 170.1181, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Elche', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 67.56139999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 67.56139999999999, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 65.68130000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 70.1762, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sedaví', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 67.56139999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 67.56139999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 67.56139999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 67.56139999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 67.56139999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 76.8827, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 69.4528, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 79.8415, 'Nombre de Pràctiques': 7, 'Punt de Destí': 'Rafelbunyol', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 67.56139999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 76.8827, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 90.8177, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Guadassuar', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 123.0215, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Gandía', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 123.0215, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Gandía', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 67.56139999999999, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'València', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 67.56139999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 62.7349, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 67.56139999999999, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 67.56139999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 67.56139999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 67.56139999999999, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 65.68130000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 67.8756, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 67.56139999999999, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 419.8509, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Montcada i Reixac', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 65.68130000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Requena'}), DefaultMunch(None, {'Distancia': 899.4545, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'Requena'})]</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>DefaultMunch(None, {})</t>
+          <t>DefaultMunch(None, {'Alumne': 'alumno06', 'Pràctica': 'Nexo(Pràctica 1)'})</t>
         </is>
       </c>
     </row>
@@ -770,7 +770,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>AlgemesÃ­</t>
+          <t>Algemesi</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -789,12 +789,12 @@
       <c r="J8" t="inlineStr"/>
       <c r="K8" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[DefaultMunch(None, {'Distancia': 23.3551, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 35.9315, 'Nombre de Pràctiques': 6, 'Punt de Destí': 'Valencia', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 12.055, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Fortaleny', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 29.7122, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Massanassa', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 23.3551, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 35.9315, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Valencia', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 43.2173, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 29.583, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Albal', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 66.6484, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 28.895, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 35.9315, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 35.9315, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 40.5264, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 28.895, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 30.809, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 43.2173, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 35.9315, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'València', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 33.276199999999996, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paiporta', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 35.9315, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 28.895, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 66.6484, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 35.9315, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 40.5264, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Algemesí', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 30.809, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 43.2173, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 28.895, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 389.9939, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Pozuelo de Alarcón', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 43.2173, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 33.8352, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Xàtiva', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 25.2359, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 35.9315, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 25.2359, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 35.9315, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 65.87769999999999, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Benisanó', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 7.87, 'Nombre de Pràctiques': 1, 'Punt de Destí': "L'Alcúdia", 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 39.671699999999994, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Mislata', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 35.048199999999994, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 28.895, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 43.2173, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 43.2173, 'Nombre de Pràctiques': 5, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 35.9315, 'Nombre de Pràctiques': 8, 'Punt de Destí': 'València', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 35.9315, 'Nombre de Pràctiques': 4, 'Punt de Destí': 'València', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 25.2359, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 12.5734, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sueca', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 30.809, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 44.5076, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 43.2173, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 45.485, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Foios', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 37.517199999999995, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Alaquas', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 35.9315, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 35.9315, 'Nombre de Pràctiques': 11, 'Punt de Destí': 'València', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 35.9315, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 30.809, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 35.9315, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 35.9315, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 35.9315, 'Nombre de Pràctiques': 5, 'Punt de Destí': 'València', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 51.085300000000004, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Riba Roja', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 43.2173, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 35.9315, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 35.9315, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 23.3551, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 946.8343000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 35.048199999999994, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 43.2173, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 13.41, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 30.8573, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Benetusser', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 145.5199, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Elche', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 35.9315, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 35.9315, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 43.2173, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 30.9342, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sedaví', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 35.9315, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 35.9315, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 35.9315, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 35.9315, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 35.9315, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 13.41, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 44.5076, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 65.7825, 'Nombre de Pràctiques': 7, 'Punt de Destí': 'Rafelbunyol', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 35.9315, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 13.41, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 4.868, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Guadassuar', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 39.7578, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Gandía', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 39.7578, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Gandía', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 35.9315, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'València', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 35.9315, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 35.048199999999994, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 35.9315, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 35.9315, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 35.9315, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 35.9315, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 43.2173, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 25.2359, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 35.9315, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 405.7919, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Montcada i Reixac', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 43.2173, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Algemesi'}), DefaultMunch(None, {'Distancia': 946.8343000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'Algemesi'})]</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>DefaultMunch(None, {})</t>
+          <t>DefaultMunch(None, {'Alumne': 'alumno07', 'Pràctica': 'AiCOM Software(Pràctica 1)'})</t>
         </is>
       </c>
     </row>
@@ -833,12 +833,12 @@
       <c r="J9" t="inlineStr"/>
       <c r="K9" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[DefaultMunch(None, {'Distancia': 13.6585, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 6, 'Punt de Destí': 'Valencia', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 39.21, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Fortaleny', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 8.8391, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Massanassa', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 13.6585, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Valencia', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 11.0844, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Albal', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 28.0815, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.7637, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 8.0286, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.7637, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.937600000000001, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 8.2699, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paiporta', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.7637, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 28.0815, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 8.0286, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 36.1064, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Algemesí', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.937600000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.7637, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 367.69440000000003, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Pozuelo de Alarcón', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 62.235, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Xàtiva', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 17.7379, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 17.7379, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 27.3108, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Benisanó', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 36.3544, 'Nombre de Pràctiques': 1, 'Punt de Destí': "L'Alcúdia", 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 4.8457, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Mislata', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 10.663799999999998, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.7637, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 5, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 8, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 4, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 17.7379, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 37.9684, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sueca', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.937600000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.3887, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 10.3529, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Foios', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 10.22, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Alaquas', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 11, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.937600000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 5, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 22.5721, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Riba Roja', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 13.6585, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 966.2381, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 10.663799999999998, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 23.585, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.7878, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Benetusser', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 173.9197, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Elche', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 6.9288, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sedaví', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 23.585, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.3887, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 19.881400000000003, 'Nombre de Pràctiques': 7, 'Punt de Destí': 'Rafelbunyol', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 23.585, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 37.499900000000004, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Guadassuar', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 69.7237, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Gandía', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 69.7237, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Gandía', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 10.663799999999998, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 17.7379, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 361.05379999999997, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Montcada i Reixac', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 966.2381, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'Valencia'})]</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>DefaultMunch(None, {})</t>
+          <t>DefaultMunch(None, {'Alumne': 'alumno08', 'Pràctica': 'Indenova(Pràctica 4)'})</t>
         </is>
       </c>
     </row>
@@ -877,12 +877,12 @@
       <c r="J10" t="inlineStr"/>
       <c r="K10" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[DefaultMunch(None, {'Distancia': 13.6585, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 6, 'Punt de Destí': 'Valencia', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 39.21, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Fortaleny', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 8.8391, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Massanassa', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 13.6585, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Valencia', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 11.0844, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Albal', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 28.0815, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.7637, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 8.0286, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.7637, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.937600000000001, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 8.2699, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paiporta', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.7637, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 28.0815, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 8.0286, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 36.1064, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Algemesí', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.937600000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.7637, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 367.69440000000003, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Pozuelo de Alarcón', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 62.235, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Xàtiva', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 17.7379, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 17.7379, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 27.3108, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Benisanó', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 36.3544, 'Nombre de Pràctiques': 1, 'Punt de Destí': "L'Alcúdia", 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 4.8457, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Mislata', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 10.663799999999998, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.7637, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 5, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 8, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 4, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 17.7379, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 37.9684, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sueca', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.937600000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.3887, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 10.3529, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Foios', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 10.22, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Alaquas', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 11, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.937600000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 5, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 22.5721, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Riba Roja', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 13.6585, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 966.2381, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 10.663799999999998, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 23.585, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.7878, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Benetusser', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 173.9197, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Elche', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 6.9288, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sedaví', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 23.585, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.3887, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 19.881400000000003, 'Nombre de Pràctiques': 7, 'Punt de Destí': 'Rafelbunyol', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 23.585, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 37.499900000000004, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Guadassuar', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 69.7237, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Gandía', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 69.7237, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Gandía', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 10.663799999999998, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 17.7379, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 361.05379999999997, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Montcada i Reixac', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 966.2381, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'Valencia'})]</t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>DefaultMunch(None, {})</t>
+          <t>DefaultMunch(None, {'Alumne': 'alumno09', 'Pràctica': 'Laberit (proyecto academy)(Pràctica 1)'})</t>
         </is>
       </c>
     </row>
@@ -902,7 +902,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>BenetÃºsser</t>
+          <t>Benetusser</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -921,12 +921,12 @@
       <c r="J11" t="inlineStr"/>
       <c r="K11" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[DefaultMunch(None, {'Distancia': 8.6265, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776800000000001, 'Nombre de Pràctiques': 6, 'Punt de Destí': 'Valencia', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 34.1779, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Fortaleny', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 1.7895, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Massanassa', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 8.6265, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776800000000001, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Valencia', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 12.707, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 4.5936, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Albal', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 33.2689, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 2.7140999999999997, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776800000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776800000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 10.0191, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 2.7140999999999997, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 1.8020999999999998, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 12.707, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776800000000001, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'València', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 2.6365, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paiporta', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776800000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 2.7140999999999997, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 33.2689, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776800000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 10.0191, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 31.0743, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Algemesí', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 1.8020999999999998, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 12.707, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 2.7140999999999997, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 370.3071, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Pozuelo de Alarcón', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 12.707, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 57.2029, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Xàtiva', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 12.7058, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776800000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 12.7058, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776800000000001, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 32.4983, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Benisanó', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 31.3223, 'Nombre de Pràctiques': 1, 'Punt de Destí': "L'Alcúdia", 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 9.164399999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Mislata', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 8.5693, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 2.7140999999999997, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 12.707, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 12.707, 'Nombre de Pràctiques': 5, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776800000000001, 'Nombre de Pràctiques': 8, 'Punt de Destí': 'València', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776800000000001, 'Nombre de Pràctiques': 4, 'Punt de Destí': 'València', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 12.7058, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 32.9363, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sueca', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 1.8020999999999998, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 12.7466, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 12.707, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 16.5976, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Foios', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 9.2968, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Alaquas', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776800000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776800000000001, 'Nombre de Pràctiques': 11, 'Punt de Destí': 'València', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776800000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 1.8020999999999998, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776800000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776800000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776800000000001, 'Nombre de Pràctiques': 5, 'Punt de Destí': 'València', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 24.896099999999997, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Riba Roja', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 12.707, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776800000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776800000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 8.6265, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 968.8508, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 8.5693, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 12.707, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 18.5529, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Benetusser', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 168.8876, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Elche', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776800000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776800000000001, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 12.707, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 2.6135, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sedaví', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776800000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776800000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776800000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776800000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776800000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 18.5529, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 12.7466, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 26.4115, 'Nombre de Pràctiques': 7, 'Punt de Destí': 'Rafelbunyol', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776800000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 18.5529, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 32.4678, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Guadassuar', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 64.6917, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Gandía', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 64.6917, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Gandía', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776800000000001, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'València', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776800000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 8.5693, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776800000000001, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776800000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776800000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776800000000001, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 12.707, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 12.7058, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776800000000001, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 367.5839, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Montcada i Reixac', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 12.707, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 968.8508, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'Benetusser'})]</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>DefaultMunch(None, {})</t>
+          <t>DefaultMunch(None, {'Alumne': 'alumno10', 'Pràctica': 'Snollocer(Pràctica 1)'})</t>
         </is>
       </c>
     </row>
@@ -951,7 +951,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>SÃ­</t>
+          <t>Si</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -965,12 +965,12 @@
       <c r="J12" t="inlineStr"/>
       <c r="K12" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 6, 'Punt de Destí': 'Valencia', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 27.0358, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Fortaleny', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 7.373, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Massanassa', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Valencia', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 21.266099999999998, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 6.5287, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Albal', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 41.8281, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 5.8407, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 18.575200000000002, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 5.8407, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 8.857899999999999, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 21.266099999999998, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 9.7786, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paiporta', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 5.8407, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 41.8281, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 18.575200000000002, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 23.9322, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Algemesí', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 8.857899999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 21.266099999999998, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 5.8407, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 371.7647, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Pozuelo de Alarcón', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 21.266099999999998, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 50.0608, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Xàtiva', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 5.144399999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 5.144399999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 41.0574, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Benisanó', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 24.1802, 'Nombre de Pràctiques': 1, 'Punt de Destí': "L'Alcúdia", 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 17.7205, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Mislata', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.2774, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 5.8407, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 21.266099999999998, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 21.266099999999998, 'Nombre de Pràctiques': 5, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 8, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 4, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 5.144399999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 25.7942, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sueca', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 8.857899999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 22.5564, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 21.266099999999998, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 23.533900000000003, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Foios', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 15.6059, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Alaquas', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 11, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 8.857899999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 5, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 32.856, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Riba Roja', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 21.266099999999998, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 970.3084, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.2774, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 21.266099999999998, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 11.4108, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 8.9062, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Benetusser', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 161.7455, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Elche', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 21.266099999999998, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 8.9831, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sedaví', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 11.4108, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 22.5564, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 32.553, 'Nombre de Pràctiques': 7, 'Punt de Destí': 'Rafelbunyol', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 11.4108, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 25.3257, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Guadassuar', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 57.5496, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Gandía', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 57.5496, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Gandía', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.2774, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 21.266099999999998, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 5.144399999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 373.7255, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Montcada i Reixac', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 21.266099999999998, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 970.3084, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'Silla'})]</t>
         </is>
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>DefaultMunch(None, {})</t>
+          <t>DefaultMunch(None, {'Alumne': 'alumno11', 'Pràctica': 'Atmosfera Sport(Pràctica 2)'})</t>
         </is>
       </c>
     </row>
@@ -1009,12 +1009,12 @@
       <c r="J13" t="inlineStr"/>
       <c r="K13" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[DefaultMunch(None, {'Distancia': 8.6265, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776800000000001, 'Nombre de Pràctiques': 6, 'Punt de Destí': 'Valencia', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 34.1779, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Fortaleny', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 1.7895, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Massanassa', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 8.6265, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776800000000001, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Valencia', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 12.707, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 4.5936, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Albal', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 33.2689, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 2.7140999999999997, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776800000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776800000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 10.0191, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 2.7140999999999997, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 1.8020999999999998, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 12.707, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776800000000001, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'València', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 2.6365, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paiporta', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776800000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 2.7140999999999997, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 33.2689, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776800000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 10.0191, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 31.0743, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Algemesí', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 1.8020999999999998, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 12.707, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 2.7140999999999997, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 370.3071, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Pozuelo de Alarcón', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 12.707, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 57.2029, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Xàtiva', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 12.7058, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776800000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 12.7058, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776800000000001, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 32.4983, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Benisanó', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 31.3223, 'Nombre de Pràctiques': 1, 'Punt de Destí': "L'Alcúdia", 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 9.164399999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Mislata', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 8.5693, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 2.7140999999999997, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 12.707, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 12.707, 'Nombre de Pràctiques': 5, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776800000000001, 'Nombre de Pràctiques': 8, 'Punt de Destí': 'València', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776800000000001, 'Nombre de Pràctiques': 4, 'Punt de Destí': 'València', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 12.7058, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 32.9363, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sueca', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 1.8020999999999998, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 12.7466, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 12.707, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 16.5976, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Foios', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 9.2968, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Alaquas', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776800000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776800000000001, 'Nombre de Pràctiques': 11, 'Punt de Destí': 'València', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776800000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 1.8020999999999998, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776800000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776800000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776800000000001, 'Nombre de Pràctiques': 5, 'Punt de Destí': 'València', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 24.896099999999997, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Riba Roja', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 12.707, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776800000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776800000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 8.6265, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 968.8508, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 8.5693, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 12.707, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 18.5529, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Benetusser', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 168.8876, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Elche', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776800000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776800000000001, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 12.707, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 2.6135, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sedaví', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776800000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776800000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776800000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776800000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776800000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 18.5529, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 12.7466, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 26.4115, 'Nombre de Pràctiques': 7, 'Punt de Destí': 'Rafelbunyol', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776800000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 18.5529, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 32.4678, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Guadassuar', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 64.6917, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Gandía', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 64.6917, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Gandía', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776800000000001, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'València', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776800000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 8.5693, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776800000000001, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776800000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776800000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776800000000001, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 12.707, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 12.7058, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776800000000001, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 367.5839, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Montcada i Reixac', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 12.707, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 968.8508, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'Benetusser'})]</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>DefaultMunch(None, {})</t>
+          <t>DefaultMunch(None, {'Alumne': 'alumno12', 'Pràctica': 'Ricardo Gomez Lara '})</t>
         </is>
       </c>
     </row>
@@ -1039,7 +1039,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>SÃ­</t>
+          <t>Si</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -1053,12 +1053,12 @@
       <c r="J14" t="inlineStr"/>
       <c r="K14" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[DefaultMunch(None, {'Distancia': 13.950899999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 6, 'Punt de Destí': 'Valencia', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 23.9937, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Fortaleny', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 20.3081, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Massanassa', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 13.950899999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Valencia', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 34.2012, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 20.178900000000002, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Albal', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 57.2663, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 19.4909, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 31.5103, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 19.4909, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 21.792900000000003, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 34.2012, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 24.260099999999998, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paiporta', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 19.4909, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 57.2663, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 31.5103, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 10.4673, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Algemesí', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 21.792900000000003, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 34.2012, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 19.4909, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 380.61190000000005, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Pozuelo de Alarcón', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 34.2012, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 35.7939, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Xàtiva', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 15.867700000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 15.867700000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 56.495599999999996, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Benisanó', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 9.9133, 'Nombre de Pràctiques': 1, 'Punt de Destí': "L'Alcúdia", 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 30.6556, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Mislata', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 25.6662, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 19.4909, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 34.2012, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 34.2012, 'Nombre de Pràctiques': 5, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 8, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 4, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 15.867700000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 21.3029, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sueca', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 21.792900000000003, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 35.4914, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 34.2012, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 36.468900000000005, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Foios', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 28.135099999999998, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Alaquas', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 11, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 21.792900000000003, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 5, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 41.703199999999995, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Riba Roja', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 34.2012, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 13.950899999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 948.793, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 25.6662, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 34.2012, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 7.9038, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 21.8412, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Benetusser', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 147.4786, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Elche', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 34.2012, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 21.9181, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sedaví', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 7.9038, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 35.4914, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 56.400400000000005, 'Nombre de Pràctiques': 7, 'Punt de Destí': 'Rafelbunyol', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 7.9038, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 11.0588, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Guadassuar', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 48.4726, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Gandía', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 48.4726, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Gandía', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 25.6662, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 34.2012, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 15.867700000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 396.40979999999996, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Montcada i Reixac', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 34.2012, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 948.793, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'Alginet'})]</t>
         </is>
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>DefaultMunch(None, {})</t>
+          <t>DefaultMunch(None, {'Alumne': 'alumno13', 'Pràctica': 'Geinfor(Pràctica 1)'})</t>
         </is>
       </c>
     </row>
@@ -1097,12 +1097,12 @@
       <c r="J15" t="inlineStr"/>
       <c r="K15" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[DefaultMunch(None, {'Distancia': 13.950899999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 6, 'Punt de Destí': 'Valencia', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 23.9937, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Fortaleny', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 20.3081, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Massanassa', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 13.950899999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Valencia', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 34.2012, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 20.178900000000002, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Albal', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 57.2663, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 19.4909, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 31.5103, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 19.4909, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 21.792900000000003, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 34.2012, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 24.260099999999998, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paiporta', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 19.4909, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 57.2663, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 31.5103, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 10.4673, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Algemesí', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 21.792900000000003, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 34.2012, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 19.4909, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 380.61190000000005, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Pozuelo de Alarcón', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 34.2012, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 35.7939, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Xàtiva', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 15.867700000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 15.867700000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 56.495599999999996, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Benisanó', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 9.9133, 'Nombre de Pràctiques': 1, 'Punt de Destí': "L'Alcúdia", 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 30.6556, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Mislata', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 25.6662, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 19.4909, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 34.2012, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 34.2012, 'Nombre de Pràctiques': 5, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 8, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 4, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 15.867700000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 21.3029, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sueca', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 21.792900000000003, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 35.4914, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 34.2012, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 36.468900000000005, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Foios', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 28.135099999999998, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Alaquas', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 11, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 21.792900000000003, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 5, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 41.703199999999995, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Riba Roja', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 34.2012, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 13.950899999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 948.793, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 25.6662, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 34.2012, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 7.9038, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 21.8412, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Benetusser', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 147.4786, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Elche', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 34.2012, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 21.9181, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sedaví', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 7.9038, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 35.4914, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 56.400400000000005, 'Nombre de Pràctiques': 7, 'Punt de Destí': 'Rafelbunyol', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 7.9038, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 11.0588, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Guadassuar', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 48.4726, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Gandía', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 48.4726, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Gandía', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 25.6662, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 34.2012, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 15.867700000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 396.40979999999996, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Montcada i Reixac', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 34.2012, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 948.793, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'Alginet'})]</t>
         </is>
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>DefaultMunch(None, {})</t>
+          <t>DefaultMunch(None, {'Alumne': 'alumno14', 'Pràctica': 'EtraMufrep(Pràctica 1)'})</t>
         </is>
       </c>
     </row>
@@ -1141,12 +1141,1992 @@
       <c r="J16" t="inlineStr"/>
       <c r="K16" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[DefaultMunch(None, {'Distancia': 6.1035, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 6, 'Punt de Destí': 'Valencia', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 31.6549, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Fortaleny', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 1.2002000000000002, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Massanassa', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 6.1035, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Valencia', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 15.222700000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 2.0949, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Albal', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 35.7846, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 12.534799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 3.3274, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 15.222700000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 5.1522, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paiporta', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 35.7846, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 12.534799999999999, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 28.551299999999998, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Algemesí', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 3.3274, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 15.222700000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 372.8228, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Pozuelo de Alarcón', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 15.222700000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 54.6799, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Xàtiva', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 10.182799999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 10.182799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 35.014, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Benisanó', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 28.7993, 'Nombre de Pràctiques': 1, 'Punt de Destí': "L'Alcúdia", 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 11.6801, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Mislata', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 10.5417, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 15.222700000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 15.222700000000001, 'Nombre de Pràctiques': 5, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 8, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 4, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 10.182799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 30.4133, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sueca', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 3.3274, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 15.2623, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 15.222700000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 19.1133, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Foios', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 12.8701, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Alaquas', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 11, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 3.3274, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 5, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 27.4118, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Riba Roja', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 15.222700000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 6.1035, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 971.3665, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 10.5417, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 15.222700000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 16.0299, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 2.7334, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Benetusser', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 166.3646, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Elche', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 15.222700000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 4.2168, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sedaví', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 16.0299, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 15.2623, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 28.9272, 'Nombre de Pràctiques': 7, 'Punt de Destí': 'Rafelbunyol', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 16.0299, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 29.9449, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Guadassuar', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 62.168699999999994, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Gandía', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 62.168699999999994, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Gandía', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 10.5417, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 15.222700000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 10.182799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 370.0997, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Montcada i Reixac', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 15.222700000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 971.3665, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'Catarroja'})]</t>
         </is>
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>DefaultMunch(None, {})</t>
+          <t>DefaultMunch(None, {'Alumne': 'alumno15', 'Pràctica': 'Arrocerias Pons(Pràctica 2)'})</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>alumno16</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>DAW</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Picassent</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Backend': '9', 'Devops': '9', 'Disenyador': '8', 'Documentacion': '9', 'Frontend': '8', 'Fullstack': '9', 'Moviles': '8'})</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr"/>
+      <c r="H17" t="inlineStr"/>
+      <c r="I17" t="inlineStr"/>
+      <c r="J17" t="inlineStr"/>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>[DefaultMunch(None, {'Distancia': 5.1371, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 18.2363, 'Nombre de Pràctiques': 6, 'Punt de Destí': 'Valencia', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 27.827099999999998, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Fortaleny', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 11.629100000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Massanassa', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 5.1371, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 18.2363, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Valencia', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 25.5222, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 9.295, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Albal', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 45.2917, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 8.607, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 18.2363, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 18.2363, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 22.8313, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 8.607, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 13.1139, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 25.5222, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 18.2363, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'València', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 12.5449, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paiporta', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 18.2363, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 8.607, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 45.2917, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 18.2363, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 22.8313, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 24.7234, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Algemesí', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 13.1139, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 25.5222, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 8.607, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 368.6373, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Pozuelo de Alarcón', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 25.5222, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 50.8544, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Xàtiva', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 18.2363, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 18.2363, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 44.521, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Benisanó', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 24.9738, 'Nombre de Pràctiques': 1, 'Punt de Destí': "L'Alcúdia", 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 21.9765, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Mislata', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 13.691600000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 8.607, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 25.5222, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 25.5222, 'Nombre de Pràctiques': 5, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 18.2363, 'Nombre de Pràctiques': 8, 'Punt de Destí': 'València', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 18.2363, 'Nombre de Pràctiques': 4, 'Punt de Destí': 'València', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 26.5854, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sueca', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 13.1139, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 26.8124, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 25.5222, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 27.789900000000003, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Foios', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 16.1605, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Alaquas', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 18.2363, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 18.2363, 'Nombre de Pràctiques': 11, 'Punt de Destí': 'València', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 18.2363, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 13.1139, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 18.2363, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 18.2363, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 18.2363, 'Nombre de Pràctiques': 5, 'Punt de Destí': 'València', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 29.7286, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Riba Roja', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 25.5222, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 18.2363, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 18.2363, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 5.1371, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 967.181, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 13.691600000000001, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 25.5222, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 12.2021, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 13.1622, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Benetusser', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 162.53910000000002, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Elche', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 18.2363, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 18.2363, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 25.5222, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 13.2391, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sedaví', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 18.2363, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 18.2363, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 18.2363, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 18.2363, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 18.2363, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 12.2021, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 26.8124, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 44.4258, 'Nombre de Pràctiques': 7, 'Punt de Destí': 'Rafelbunyol', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 18.2363, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 12.2021, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 26.1193, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Guadassuar', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 58.3408, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Gandía', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 58.3408, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Gandía', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 18.2363, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'València', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 18.2363, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 13.691600000000001, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 18.2363, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 18.2363, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 18.2363, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 18.2363, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 25.5222, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 18.2363, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 384.4352, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Montcada i Reixac', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 25.5222, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 967.181, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'Picassent'})]</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Alumne': 'alumno16', 'Pràctica': 'RECAMBIOS VICAMP, S.L(Pràctica 1)'})</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>alumno17</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>DAW</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Catarroja</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Si</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Backend': '10', 'Devops': '6', 'Disenyador': '7', 'Documentacion': '4', 'Frontend': '8', 'Fullstack': '9', 'Moviles': '3'})</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr"/>
+      <c r="H18" t="inlineStr"/>
+      <c r="I18" t="inlineStr"/>
+      <c r="J18" t="inlineStr"/>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>[DefaultMunch(None, {'Distancia': 6.1035, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 6, 'Punt de Destí': 'Valencia', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 31.6549, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Fortaleny', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 1.2002000000000002, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Massanassa', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 6.1035, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Valencia', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 15.222700000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 2.0949, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Albal', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 35.7846, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 12.534799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 3.3274, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 15.222700000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 5.1522, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paiporta', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 35.7846, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 12.534799999999999, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 28.551299999999998, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Algemesí', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 3.3274, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 15.222700000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 372.8228, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Pozuelo de Alarcón', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 15.222700000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 54.6799, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Xàtiva', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 10.182799999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 10.182799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 35.014, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Benisanó', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 28.7993, 'Nombre de Pràctiques': 1, 'Punt de Destí': "L'Alcúdia", 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 11.6801, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Mislata', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 10.5417, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 15.222700000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 15.222700000000001, 'Nombre de Pràctiques': 5, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 8, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 4, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 10.182799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 30.4133, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sueca', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 3.3274, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 15.2623, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 15.222700000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 19.1133, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Foios', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 12.8701, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Alaquas', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 11, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 3.3274, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 5, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 27.4118, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Riba Roja', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 15.222700000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 6.1035, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 971.3665, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 10.5417, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 15.222700000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 16.0299, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 2.7334, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Benetusser', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 166.3646, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Elche', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 15.222700000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 4.2168, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sedaví', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 16.0299, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 15.2623, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 28.9272, 'Nombre de Pràctiques': 7, 'Punt de Destí': 'Rafelbunyol', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 16.0299, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 29.9449, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Guadassuar', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 62.168699999999994, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Gandía', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 62.168699999999994, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Gandía', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 10.5417, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 15.222700000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 10.182799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 370.0997, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Montcada i Reixac', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 15.222700000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 971.3665, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'Catarroja'})]</t>
+        </is>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Alumne': 'alumno17', 'Pràctica': 'Cesumin(Pràctica 1)'})</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>alumno18</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>DAW</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Valencia</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Backend': '8', 'Devops': '3', 'Disenyador': '2', 'Documentacion': '2', 'Frontend': '4', 'Fullstack': '8', 'Moviles': '5'})</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr"/>
+      <c r="H19" t="inlineStr"/>
+      <c r="I19" t="inlineStr"/>
+      <c r="J19" t="inlineStr"/>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>[DefaultMunch(None, {'Distancia': 13.6585, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 6, 'Punt de Destí': 'Valencia', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 39.21, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Fortaleny', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 8.8391, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Massanassa', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 13.6585, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Valencia', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 11.0844, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Albal', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 28.0815, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.7637, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 8.0286, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.7637, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.937600000000001, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 8.2699, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paiporta', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.7637, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 28.0815, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 8.0286, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 36.1064, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Algemesí', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.937600000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.7637, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 367.69440000000003, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Pozuelo de Alarcón', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 62.235, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Xàtiva', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 17.7379, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 17.7379, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 27.3108, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Benisanó', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 36.3544, 'Nombre de Pràctiques': 1, 'Punt de Destí': "L'Alcúdia", 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 4.8457, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Mislata', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 10.663799999999998, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.7637, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 5, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 8, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 4, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 17.7379, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 37.9684, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sueca', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.937600000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.3887, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 10.3529, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Foios', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 10.22, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Alaquas', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 11, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.937600000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 5, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 22.5721, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Riba Roja', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 13.6585, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 966.2381, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 10.663799999999998, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 23.585, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.7878, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Benetusser', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 173.9197, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Elche', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 6.9288, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sedaví', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 23.585, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.3887, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 19.881400000000003, 'Nombre de Pràctiques': 7, 'Punt de Destí': 'Rafelbunyol', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 23.585, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 37.499900000000004, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Guadassuar', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 69.7237, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Gandía', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 69.7237, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Gandía', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 10.663799999999998, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 17.7379, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 361.05379999999997, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Montcada i Reixac', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 966.2381, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'Valencia'})]</t>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Alumne': 'alumno18', 'Pràctica': 'Indra // Minsait(Pràctica 4)'})</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>alumno19</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>DAW</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Albal</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Si</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Backend': '10', 'Devops': '5', 'Disenyador': '8', 'Documentacion': '1', 'Frontend': '10', 'Fullstack': '10', 'Moviles': '10'})</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr"/>
+      <c r="H20" t="inlineStr"/>
+      <c r="I20" t="inlineStr"/>
+      <c r="J20" t="inlineStr"/>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>[DefaultMunch(None, {'Distancia': 5.904, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 6, 'Punt de Destí': 'Valencia', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 31.4555, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Fortaleny', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 3.7565, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Massanassa', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 5.904, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Valencia', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 16.428099999999997, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Albal', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 36.9901, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 2.3773, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 13.7403, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 2.3773, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 5.59, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 16.428099999999997, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 6.3576999999999995, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paiporta', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 2.3773, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 36.9901, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 13.7403, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 28.3518, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Algemesí', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 5.59, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 16.428099999999997, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 2.3773, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 374.0283, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Pozuelo de Alarcón', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 16.428099999999997, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 54.4804, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Xàtiva', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 9.9833, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 9.9833, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 36.2194, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Benisanó', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 28.5998, 'Nombre de Pràctiques': 1, 'Punt de Destí': "L'Alcúdia", 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 12.8855, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Mislata', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 8.44, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 2.3773, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 16.428099999999997, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 16.428099999999997, 'Nombre de Pràctiques': 5, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 8, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 4, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 9.9833, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 30.2138, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sueca', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 5.59, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 16.4677, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 16.428099999999997, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 20.3187, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Foios', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.7685, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Alaquas', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 11, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 5.59, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 5, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 28.6172, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Riba Roja', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 16.428099999999997, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 5.904, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 972.572, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 8.44, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 16.428099999999997, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 15.8304, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 4.996, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Benetusser', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 166.1651, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Elche', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 16.428099999999997, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 7.253100000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sedaví', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 15.8304, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 16.4677, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 30.1327, 'Nombre de Pràctiques': 7, 'Punt de Destí': 'Rafelbunyol', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 15.8304, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 29.7454, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Guadassuar', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 61.969199999999994, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Gandía', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 61.969199999999994, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Gandía', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 8.44, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 16.428099999999997, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 9.9833, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 371.3051, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Montcada i Reixac', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 16.428099999999997, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 972.572, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'Albal'})]</t>
+        </is>
+      </c>
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Alumne': 'alumno19', 'Pràctica': 'Electrodomesticos Llacer(Pràctica 2)'})</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>alumno20</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>DAW</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Sollana</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Backend': '7', 'Devops': '7', 'Disenyador': '10', 'Documentacion': '1', 'Frontend': '10', 'Fullstack': '7', 'Moviles': '7'})</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr"/>
+      <c r="H21" t="inlineStr"/>
+      <c r="I21" t="inlineStr"/>
+      <c r="J21" t="inlineStr"/>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>[DefaultMunch(None, {'Distancia': 15.9393, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 28.9037, 'Nombre de Pràctiques': 6, 'Punt de Destí': 'Valencia', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 13.506, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Fortaleny', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 22.2965, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Massanassa', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 15.9393, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 28.9037, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Valencia', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 36.1896, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 22.1673, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Albal', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 59.2326, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 21.4793, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 28.9037, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 28.9037, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 33.4987, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 21.4793, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 23.781299999999998, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 36.1896, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 28.9037, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'València', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 26.2484, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paiporta', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 28.9037, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 21.4793, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 59.2326, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 28.9037, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 33.4987, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 15.0618, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Algemesí', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 23.781299999999998, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 36.1896, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 21.4793, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 382.57820000000004, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Pozuelo de Alarcón', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 36.1896, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 46.8598, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Xàtiva', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 17.8201, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 28.9037, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 17.8201, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 28.9037, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 58.4619, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Benisanó', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 20.979200000000002, 'Nombre de Pràctiques': 1, 'Punt de Destí': "L'Alcúdia", 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 32.6439, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Mislata', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 27.6325, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 21.4793, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 36.1896, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 36.1896, 'Nombre de Pràctiques': 5, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 28.9037, 'Nombre de Pràctiques': 8, 'Punt de Destí': 'València', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 28.9037, 'Nombre de Pràctiques': 4, 'Punt de Destí': 'València', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 17.8201, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 12.2644, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sueca', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 23.781299999999998, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 37.479800000000004, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 36.1896, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 38.457300000000004, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Foios', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 30.1014, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Alaquas', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 28.9037, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 28.9037, 'Nombre de Pràctiques': 11, 'Punt de Destí': 'València', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 28.9037, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 23.781299999999998, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 28.9037, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 28.9037, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 28.9037, 'Nombre de Pràctiques': 5, 'Punt de Destí': 'València', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 43.6695, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Riba Roja', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 36.1896, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 28.9037, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 28.9037, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 15.9393, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 981.1219, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 27.6325, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 36.1896, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 5.4293000000000005, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 23.8296, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Benetusser', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 158.5445, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Elche', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 28.9037, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 28.9037, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 36.1896, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 23.9065, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sedaví', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 28.9037, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 28.9037, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 28.9037, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 28.9037, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 28.9037, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 5.4293000000000005, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 37.479800000000004, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 58.366699999999994, 'Nombre de Pràctiques': 7, 'Punt de Destí': 'Rafelbunyol', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 28.9037, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 5.4293000000000005, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 19.6719, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Guadassuar', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 42.441199999999995, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Gandía', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 42.441199999999995, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Gandía', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 28.9037, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'València', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 28.9037, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 27.6325, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 28.9037, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 28.9037, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 28.9037, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 28.9037, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 36.1896, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 17.8201, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 28.9037, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 398.37609999999995, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Montcada i Reixac', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 36.1896, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 981.1219, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'Sollana'})]</t>
+        </is>
+      </c>
+      <c r="L21" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Alumne': 'alumno20', 'Pràctica': 'Walkerpark(Pràctica 1)'})</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>alumno21</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>DAW</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Carcaixent</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Si</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Backend': '10', 'Devops': '7', 'Disenyador': '5', 'Documentacion': '1', 'Frontend': '5', 'Fullstack': '5', 'Moviles': '1 '})</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr"/>
+      <c r="H22" t="inlineStr"/>
+      <c r="I22" t="inlineStr"/>
+      <c r="J22" t="inlineStr"/>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>[DefaultMunch(None, {'Distancia': 34.293099999999995, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Carcaixent'}), DefaultMunch(None, {'Distancia': 47.2576, 'Nombre de Pràctiques': 6, 'Punt de Destí': 'Valencia', 'Punt de Partida': 'Carcaixent'}), DefaultMunch(None, {'Distancia': 18.9595, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Fortaleny', 'Punt de Partida': 'Carcaixent'}), DefaultMunch(None, {'Distancia': 40.6503, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Massanassa', 'Punt de Partida': 'Carcaixent'}), DefaultMunch(None, {'Distancia': 34.293099999999995, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Carcaixent'}), DefaultMunch(None, {'Distancia': 47.2576, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Valencia', 'Punt de Partida': 'Carcaixent'}), DefaultMunch(None, {'Distancia': 54.5434, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Carcaixent'}), DefaultMunch(None, {'Distancia': 40.5211, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Albal', 'Punt de Partida': 'Carcaixent'}), DefaultMunch(None, {'Distancia': 77.6085, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'Carcaixent'}), DefaultMunch(None, {'Distancia': 39.8331, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Carcaixent'}), DefaultMunch(None, {'Distancia': 47.2576, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Carcaixent'}), DefaultMunch(None, {'Distancia': 47.2576, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Carcaixent'}), DefaultMunch(None, {'Distancia': 51.8525, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'Carcaixent'}), DefaultMunch(None, {'Distancia': 39.8331, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Carcaixent'}), DefaultMunch(None, {'Distancia': 42.1352, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Carcaixent'}), DefaultMunch(None, {'Distancia': 54.5434, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Carcaixent'}), DefaultMunch(None, {'Distancia': 47.2576, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'València', 'Punt de Partida': 'Carcaixent'}), DefaultMunch(None, {'Distancia': 44.6023, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paiporta', 'Punt de Partida': 'Carcaixent'}), DefaultMunch(None, {'Distancia': 47.2576, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Carcaixent'}), DefaultMunch(None, {'Distancia': 39.8331, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Carcaixent'}), DefaultMunch(None, {'Distancia': 77.6085, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'Carcaixent'}), DefaultMunch(None, {'Distancia': 47.2576, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Carcaixent'}), DefaultMunch(None, {'Distancia': 51.8525, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'Carcaixent'}), DefaultMunch(None, {'Distancia': 10.7684, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Algemesí', 'Punt de Partida': 'Carcaixent'}), DefaultMunch(None, {'Distancia': 42.1352, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Carcaixent'}), DefaultMunch(None, {'Distancia': 54.5434, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Carcaixent'}), DefaultMunch(None, {'Distancia': 39.8331, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Carcaixent'}), DefaultMunch(None, {'Distancia': 400.9541, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Pozuelo de Alarcón', 'Punt de Partida': 'Carcaixent'}), DefaultMunch(None, {'Distancia': 54.5434, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Carcaixent'}), DefaultMunch(None, {'Distancia': 19.518099999999997, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Xàtiva', 'Punt de Partida': 'Carcaixent'}), DefaultMunch(None, {'Distancia': 36.209900000000005, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Carcaixent'}), DefaultMunch(None, {'Distancia': 47.2576, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Carcaixent'}), DefaultMunch(None, {'Distancia': 36.209900000000005, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Carcaixent'}), DefaultMunch(None, {'Distancia': 47.2576, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Carcaixent'}), DefaultMunch(None, {'Distancia': 76.8378, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Benisanó', 'Punt de Partida': 'Carcaixent'}), DefaultMunch(None, {'Distancia': 13.2639, 'Nombre de Pràctiques': 1, 'Punt de Destí': "L'Alcúdia", 'Punt de Partida': 'Carcaixent'}), DefaultMunch(None, {'Distancia': 50.997800000000005, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Mislata', 'Punt de Partida': 'Carcaixent'}), DefaultMunch(None, {'Distancia': 46.0084, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Carcaixent'}), DefaultMunch(None, {'Distancia': 39.8331, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Carcaixent'}), DefaultMunch(None, {'Distancia': 54.5434, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Carcaixent'}), DefaultMunch(None, {'Distancia': 54.5434, 'Nombre de Pràctiques': 5, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Carcaixent'}), DefaultMunch(None, {'Distancia': 47.2576, 'Nombre de Pràctiques': 8, 'Punt de Destí': 'València', 'Punt de Partida': 'Carcaixent'}), DefaultMunch(None, {'Distancia': 47.2576, 'Nombre de Pràctiques': 4, 'Punt de Destí': 'València', 'Punt de Partida': 'Carcaixent'}), DefaultMunch(None, {'Distancia': 36.209900000000005, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Carcaixent'}), DefaultMunch(None, {'Distancia': 19.6814, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sueca', 'Punt de Partida': 'Carcaixent'}), DefaultMunch(None, {'Distancia': 42.1352, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Carcaixent'}), DefaultMunch(None, {'Distancia': 55.8337, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Carcaixent'}), DefaultMunch(None, {'Distancia': 54.5434, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Carcaixent'}), DefaultMunch(None, {'Distancia': 56.811099999999996, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Foios', 'Punt de Partida': 'Carcaixent'}), DefaultMunch(None, {'Distancia': 48.4773, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Alaquas', 'Punt de Partida': 'Carcaixent'}), DefaultMunch(None, {'Distancia': 47.2576, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Carcaixent'}), DefaultMunch(None, {'Distancia': 47.2576, 'Nombre de Pràctiques': 11, 'Punt de Destí': 'València', 'Punt de Partida': 'Carcaixent'}), DefaultMunch(None, {'Distancia': 47.2576, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Carcaixent'}), DefaultMunch(None, {'Distancia': 42.1352, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Carcaixent'}), DefaultMunch(None, {'Distancia': 47.2576, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Carcaixent'}), DefaultMunch(None, {'Distancia': 47.2576, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Carcaixent'}), DefaultMunch(None, {'Distancia': 47.2576, 'Nombre de Pràctiques': 5, 'Punt de Destí': 'València', 'Punt de Partida': 'Carcaixent'}), DefaultMunch(None, {'Distancia': 62.0454, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Riba Roja', 'Punt de Partida': 'Carcaixent'}), DefaultMunch(None, {'Distancia': 54.5434, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Carcaixent'}), DefaultMunch(None, {'Distancia': 47.2576, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Carcaixent'}), DefaultMunch(None, {'Distancia': 47.2576, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Carcaixent'}), DefaultMunch(None, {'Distancia': 34.293099999999995, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Carcaixent'}), DefaultMunch(None, {'Distancia': 936.6451999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'Carcaixent'}), DefaultMunch(None, {'Distancia': 46.0084, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Carcaixent'}), DefaultMunch(None, {'Distancia': 54.5434, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Carcaixent'}), DefaultMunch(None, {'Distancia': 24.8101, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Carcaixent'}), DefaultMunch(None, {'Distancia': 42.1835, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Benetusser', 'Punt de Partida': 'Carcaixent'}), DefaultMunch(None, {'Distancia': 135.33089999999999, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Elche', 'Punt de Partida': 'Carcaixent'}), DefaultMunch(None, {'Distancia': 47.2576, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Carcaixent'}), DefaultMunch(None, {'Distancia': 47.2576, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Carcaixent'}), DefaultMunch(None, {'Distancia': 54.5434, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Carcaixent'}), DefaultMunch(None, {'Distancia': 42.2603, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sedaví', 'Punt de Partida': 'Carcaixent'}), DefaultMunch(None, {'Distancia': 47.2576, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Carcaixent'}), DefaultMunch(None, {'Distancia': 47.2576, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Carcaixent'}), DefaultMunch(None, {'Distancia': 47.2576, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Carcaixent'}), DefaultMunch(None, {'Distancia': 47.2576, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Carcaixent'}), DefaultMunch(None, {'Distancia': 47.2576, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Carcaixent'}), DefaultMunch(None, {'Distancia': 24.8101, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Carcaixent'}), DefaultMunch(None, {'Distancia': 55.8337, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Carcaixent'}), DefaultMunch(None, {'Distancia': 76.74260000000001, 'Nombre de Pràctiques': 7, 'Punt de Destí': 'Rafelbunyol', 'Punt de Partida': 'Carcaixent'}), DefaultMunch(None, {'Distancia': 47.2576, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Carcaixent'}), DefaultMunch(None, {'Distancia': 24.8101, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Carcaixent'}), DefaultMunch(None, {'Distancia': 10.4368, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Guadassuar', 'Punt de Partida': 'Carcaixent'}), DefaultMunch(None, {'Distancia': 35.8797, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Gandía', 'Punt de Partida': 'Carcaixent'}), DefaultMunch(None, {'Distancia': 35.8797, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Gandía', 'Punt de Partida': 'Carcaixent'}), DefaultMunch(None, {'Distancia': 47.2576, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'València', 'Punt de Partida': 'Carcaixent'}), DefaultMunch(None, {'Distancia': 47.2576, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Carcaixent'}), DefaultMunch(None, {'Distancia': 46.0084, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Carcaixent'}), DefaultMunch(None, {'Distancia': 47.2576, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Carcaixent'}), DefaultMunch(None, {'Distancia': 47.2576, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Carcaixent'}), DefaultMunch(None, {'Distancia': 47.2576, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Carcaixent'}), DefaultMunch(None, {'Distancia': 47.2576, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Carcaixent'}), DefaultMunch(None, {'Distancia': 54.5434, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Carcaixent'}), DefaultMunch(None, {'Distancia': 36.209900000000005, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Carcaixent'}), DefaultMunch(None, {'Distancia': 47.2576, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Carcaixent'}), DefaultMunch(None, {'Distancia': 416.752, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Montcada i Reixac', 'Punt de Partida': 'Carcaixent'}), DefaultMunch(None, {'Distancia': 54.5434, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Carcaixent'}), DefaultMunch(None, {'Distancia': 936.6451999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'Carcaixent'})]</t>
+        </is>
+      </c>
+      <c r="L22" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Alumne': 'alumno21', 'Pràctica': 'AiCOM Software(Pràctica 3)'})</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>alumno22</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>DAW</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Albal</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Si</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Backend': '6', 'Devops': '6', 'Disenyador': '8', 'Documentacion': '6', 'Frontend': '7', 'Fullstack': '7', 'Moviles': '6'})</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr"/>
+      <c r="H23" t="inlineStr"/>
+      <c r="I23" t="inlineStr"/>
+      <c r="J23" t="inlineStr"/>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>[DefaultMunch(None, {'Distancia': 5.904, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 6, 'Punt de Destí': 'Valencia', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 31.4555, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Fortaleny', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 3.7565, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Massanassa', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 5.904, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Valencia', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 16.428099999999997, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Albal', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 36.9901, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 2.3773, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 13.7403, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 2.3773, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 5.59, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 16.428099999999997, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 6.3576999999999995, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paiporta', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 2.3773, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 36.9901, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 13.7403, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 28.3518, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Algemesí', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 5.59, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 16.428099999999997, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 2.3773, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 374.0283, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Pozuelo de Alarcón', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 16.428099999999997, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 54.4804, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Xàtiva', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 9.9833, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 9.9833, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 36.2194, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Benisanó', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 28.5998, 'Nombre de Pràctiques': 1, 'Punt de Destí': "L'Alcúdia", 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 12.8855, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Mislata', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 8.44, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 2.3773, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 16.428099999999997, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 16.428099999999997, 'Nombre de Pràctiques': 5, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 8, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 4, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 9.9833, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 30.2138, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sueca', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 5.59, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 16.4677, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 16.428099999999997, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 20.3187, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Foios', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.7685, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Alaquas', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 11, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 5.59, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 5, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 28.6172, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Riba Roja', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 16.428099999999997, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 5.904, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 972.572, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 8.44, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 16.428099999999997, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 15.8304, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 4.996, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Benetusser', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 166.1651, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Elche', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 16.428099999999997, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 7.253100000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sedaví', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 15.8304, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 16.4677, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 30.1327, 'Nombre de Pràctiques': 7, 'Punt de Destí': 'Rafelbunyol', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 15.8304, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 29.7454, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Guadassuar', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 61.969199999999994, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Gandía', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 61.969199999999994, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Gandía', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 8.44, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 16.428099999999997, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 9.9833, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 371.3051, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Montcada i Reixac', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 16.428099999999997, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 972.572, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'Albal'})]</t>
+        </is>
+      </c>
+      <c r="L23" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Alumne': 'alumno22', 'Pràctica': 'DYNAMIZATIC(Pràctica 2)'})</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>alumno23</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>DAW</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Valencia</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Si</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Backend': '10', 'Devops': '8', 'Disenyador': '8', 'Documentacion': '8', 'Frontend': '8', 'Fullstack': '7', 'Moviles': '6'})</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr"/>
+      <c r="H24" t="inlineStr"/>
+      <c r="I24" t="inlineStr"/>
+      <c r="J24" t="inlineStr"/>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>[DefaultMunch(None, {'Distancia': 13.6585, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 6, 'Punt de Destí': 'Valencia', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 39.21, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Fortaleny', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 8.8391, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Massanassa', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 13.6585, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Valencia', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 11.0844, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Albal', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 28.0815, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.7637, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 8.0286, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.7637, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.937600000000001, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 8.2699, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paiporta', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.7637, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 28.0815, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 8.0286, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 36.1064, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Algemesí', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.937600000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.7637, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 367.69440000000003, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Pozuelo de Alarcón', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 62.235, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Xàtiva', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 17.7379, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 17.7379, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 27.3108, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Benisanó', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 36.3544, 'Nombre de Pràctiques': 1, 'Punt de Destí': "L'Alcúdia", 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 4.8457, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Mislata', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 10.663799999999998, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.7637, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 5, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 8, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 4, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 17.7379, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 37.9684, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sueca', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.937600000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.3887, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 10.3529, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Foios', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 10.22, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Alaquas', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 11, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.937600000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 5, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 22.5721, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Riba Roja', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 13.6585, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 966.2381, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 10.663799999999998, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 23.585, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.7878, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Benetusser', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 173.9197, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Elche', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 6.9288, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sedaví', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 23.585, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.3887, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 19.881400000000003, 'Nombre de Pràctiques': 7, 'Punt de Destí': 'Rafelbunyol', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 23.585, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 37.499900000000004, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Guadassuar', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 69.7237, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Gandía', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 69.7237, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Gandía', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 10.663799999999998, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 17.7379, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 361.05379999999997, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Montcada i Reixac', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 966.2381, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'Valencia'})]</t>
+        </is>
+      </c>
+      <c r="L24" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Alumne': 'alumno23', 'Pràctica': 'COLBA TECHNOLOGIES(Pràctica 3)'})</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>alumno24</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>DAW</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Picassent</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Backend': '9', 'Devops': '8', 'Disenyador': '8', 'Documentacion': '6', 'Frontend': '9', 'Fullstack': '10', 'Moviles': '8'})</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr"/>
+      <c r="H25" t="inlineStr"/>
+      <c r="I25" t="inlineStr"/>
+      <c r="J25" t="inlineStr"/>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>[DefaultMunch(None, {'Distancia': 5.1371, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 18.2363, 'Nombre de Pràctiques': 6, 'Punt de Destí': 'Valencia', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 27.827099999999998, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Fortaleny', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 11.629100000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Massanassa', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 5.1371, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 18.2363, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Valencia', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 25.5222, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 9.295, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Albal', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 45.2917, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 8.607, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 18.2363, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 18.2363, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 22.8313, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 8.607, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 13.1139, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 25.5222, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 18.2363, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'València', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 12.5449, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paiporta', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 18.2363, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 8.607, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 45.2917, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 18.2363, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 22.8313, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 24.7234, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Algemesí', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 13.1139, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 25.5222, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 8.607, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 368.6373, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Pozuelo de Alarcón', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 25.5222, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 50.8544, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Xàtiva', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 18.2363, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 18.2363, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 44.521, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Benisanó', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 24.9738, 'Nombre de Pràctiques': 1, 'Punt de Destí': "L'Alcúdia", 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 21.9765, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Mislata', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 13.691600000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 8.607, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 25.5222, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 25.5222, 'Nombre de Pràctiques': 5, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 18.2363, 'Nombre de Pràctiques': 8, 'Punt de Destí': 'València', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 18.2363, 'Nombre de Pràctiques': 4, 'Punt de Destí': 'València', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 26.5854, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sueca', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 13.1139, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 26.8124, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 25.5222, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 27.789900000000003, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Foios', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 16.1605, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Alaquas', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 18.2363, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 18.2363, 'Nombre de Pràctiques': 11, 'Punt de Destí': 'València', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 18.2363, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 13.1139, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 18.2363, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 18.2363, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 18.2363, 'Nombre de Pràctiques': 5, 'Punt de Destí': 'València', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 29.7286, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Riba Roja', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 25.5222, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 18.2363, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 18.2363, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 5.1371, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 967.181, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 13.691600000000001, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 25.5222, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 12.2021, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 13.1622, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Benetusser', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 162.53910000000002, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Elche', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 18.2363, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 18.2363, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 25.5222, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 13.2391, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sedaví', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 18.2363, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 18.2363, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 18.2363, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 18.2363, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 18.2363, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 12.2021, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 26.8124, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 44.4258, 'Nombre de Pràctiques': 7, 'Punt de Destí': 'Rafelbunyol', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 18.2363, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 12.2021, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 26.1193, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Guadassuar', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 58.3408, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Gandía', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 58.3408, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Gandía', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 18.2363, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'València', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 18.2363, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 13.691600000000001, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 18.2363, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 18.2363, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 18.2363, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 18.2363, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 25.5222, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 18.2363, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 384.4352, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Montcada i Reixac', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 25.5222, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 967.181, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'Picassent'})]</t>
+        </is>
+      </c>
+      <c r="L25" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Alumne': 'alumno24', 'Pràctica': 'FIX technology(Pràctica 1)'})</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>alumno25</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>DAW</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Valencia</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>Si</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Backend': '9', 'Devops': '1', 'Disenyador': '9', 'Documentacion': '1', 'Frontend': '9', 'Fullstack': '9', 'Moviles': '1'})</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr"/>
+      <c r="H26" t="inlineStr"/>
+      <c r="I26" t="inlineStr"/>
+      <c r="J26" t="inlineStr"/>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>[DefaultMunch(None, {'Distancia': 13.6585, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 6, 'Punt de Destí': 'Valencia', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 39.21, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Fortaleny', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 8.8391, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Massanassa', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 13.6585, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Valencia', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 11.0844, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Albal', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 28.0815, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.7637, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 8.0286, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.7637, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.937600000000001, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 8.2699, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paiporta', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.7637, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 28.0815, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 8.0286, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 36.1064, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Algemesí', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.937600000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.7637, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 367.69440000000003, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Pozuelo de Alarcón', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 62.235, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Xàtiva', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 17.7379, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 17.7379, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 27.3108, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Benisanó', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 36.3544, 'Nombre de Pràctiques': 1, 'Punt de Destí': "L'Alcúdia", 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 4.8457, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Mislata', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 10.663799999999998, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.7637, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 5, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 8, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 4, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 17.7379, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 37.9684, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sueca', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.937600000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.3887, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 10.3529, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Foios', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 10.22, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Alaquas', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 11, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.937600000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 5, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 22.5721, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Riba Roja', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 13.6585, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 966.2381, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 10.663799999999998, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 23.585, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.7878, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Benetusser', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 173.9197, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Elche', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 6.9288, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sedaví', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 23.585, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.3887, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 19.881400000000003, 'Nombre de Pràctiques': 7, 'Punt de Destí': 'Rafelbunyol', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 23.585, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 37.499900000000004, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Guadassuar', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 69.7237, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Gandía', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 69.7237, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Gandía', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 10.663799999999998, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 17.7379, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 361.05379999999997, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Montcada i Reixac', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 966.2381, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'Valencia'})]</t>
+        </is>
+      </c>
+      <c r="L26" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Alumne': 'alumno25', 'Pràctica': 'Trigeasport(Pràctica 1)'})</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>alumno26</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>DAW</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Albal</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>Si</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Backend': '2', 'Devops': '9', 'Disenyador': '2', 'Documentacion': '7', 'Frontend': '9', 'Fullstack': '8', 'Moviles': '5'})</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr"/>
+      <c r="H27" t="inlineStr"/>
+      <c r="I27" t="inlineStr"/>
+      <c r="J27" t="inlineStr"/>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t>[DefaultMunch(None, {'Distancia': 5.904, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 6, 'Punt de Destí': 'Valencia', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 31.4555, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Fortaleny', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 3.7565, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Massanassa', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 5.904, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Valencia', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 16.428099999999997, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Albal', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 36.9901, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 2.3773, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 13.7403, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 2.3773, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 5.59, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 16.428099999999997, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 6.3576999999999995, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paiporta', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 2.3773, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 36.9901, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 13.7403, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 28.3518, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Algemesí', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 5.59, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 16.428099999999997, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 2.3773, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 374.0283, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Pozuelo de Alarcón', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 16.428099999999997, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 54.4804, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Xàtiva', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 9.9833, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 9.9833, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 36.2194, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Benisanó', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 28.5998, 'Nombre de Pràctiques': 1, 'Punt de Destí': "L'Alcúdia", 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 12.8855, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Mislata', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 8.44, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 2.3773, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 16.428099999999997, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 16.428099999999997, 'Nombre de Pràctiques': 5, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 8, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 4, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 9.9833, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 30.2138, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sueca', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 5.59, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 16.4677, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 16.428099999999997, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 20.3187, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Foios', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.7685, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Alaquas', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 11, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 5.59, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 5, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 28.6172, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Riba Roja', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 16.428099999999997, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 5.904, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 972.572, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 8.44, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 16.428099999999997, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 15.8304, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 4.996, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Benetusser', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 166.1651, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Elche', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 16.428099999999997, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 7.253100000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sedaví', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 15.8304, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 16.4677, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 30.1327, 'Nombre de Pràctiques': 7, 'Punt de Destí': 'Rafelbunyol', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 15.8304, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 29.7454, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Guadassuar', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 61.969199999999994, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Gandía', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 61.969199999999994, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Gandía', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 8.44, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 16.428099999999997, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 9.9833, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 371.3051, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Montcada i Reixac', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 16.428099999999997, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 972.572, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'Albal'})]</t>
+        </is>
+      </c>
+      <c r="L27" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Alumne': 'alumno26', 'Pràctica': 'Informática Alfafar S.L.(Pràctica 1)'})</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>alumno27</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>DAW</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Silla</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>Si</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Backend': '7', 'Devops': '2', 'Disenyador': '10', 'Documentacion': '8', 'Frontend': '7', 'Fullstack': '4', 'Moviles': '6'})</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr"/>
+      <c r="H28" t="inlineStr"/>
+      <c r="I28" t="inlineStr"/>
+      <c r="J28" t="inlineStr"/>
+      <c r="K28" t="inlineStr">
+        <is>
+          <t>[DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 6, 'Punt de Destí': 'Valencia', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 27.0358, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Fortaleny', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 7.373, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Massanassa', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Valencia', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 21.266099999999998, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 6.5287, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Albal', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 41.8281, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 5.8407, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 18.575200000000002, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 5.8407, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 8.857899999999999, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 21.266099999999998, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 9.7786, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paiporta', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 5.8407, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 41.8281, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 18.575200000000002, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 23.9322, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Algemesí', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 8.857899999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 21.266099999999998, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 5.8407, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 371.7647, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Pozuelo de Alarcón', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 21.266099999999998, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 50.0608, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Xàtiva', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 5.144399999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 5.144399999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 41.0574, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Benisanó', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 24.1802, 'Nombre de Pràctiques': 1, 'Punt de Destí': "L'Alcúdia", 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 17.7205, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Mislata', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.2774, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 5.8407, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 21.266099999999998, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 21.266099999999998, 'Nombre de Pràctiques': 5, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 8, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 4, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 5.144399999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 25.7942, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sueca', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 8.857899999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 22.5564, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 21.266099999999998, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 23.533900000000003, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Foios', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 15.6059, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Alaquas', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 11, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 8.857899999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 5, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 32.856, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Riba Roja', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 21.266099999999998, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 970.3084, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.2774, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 21.266099999999998, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 11.4108, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 8.9062, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Benetusser', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 161.7455, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Elche', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 21.266099999999998, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 8.9831, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sedaví', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 11.4108, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 22.5564, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 32.553, 'Nombre de Pràctiques': 7, 'Punt de Destí': 'Rafelbunyol', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 11.4108, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 25.3257, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Guadassuar', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 57.5496, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Gandía', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 57.5496, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Gandía', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.2774, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 21.266099999999998, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 5.144399999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 373.7255, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Montcada i Reixac', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 21.266099999999998, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 970.3084, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'Silla'})]</t>
+        </is>
+      </c>
+      <c r="L28" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Alumne': 'alumno27', 'Pràctica': 'Osmofilter(Pràctica 1)'})</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>alumno28</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>DAW</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Valencia</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>Si</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Backend': '6', 'Devops': '8', 'Disenyador': '4', 'Documentacion': '4', 'Frontend': '7', 'Fullstack': '8', 'Moviles': '9'})</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr"/>
+      <c r="H29" t="inlineStr"/>
+      <c r="I29" t="inlineStr"/>
+      <c r="J29" t="inlineStr"/>
+      <c r="K29" t="inlineStr">
+        <is>
+          <t>[DefaultMunch(None, {'Distancia': 13.6585, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 6, 'Punt de Destí': 'Valencia', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 39.21, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Fortaleny', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 8.8391, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Massanassa', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 13.6585, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Valencia', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 11.0844, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Albal', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 28.0815, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.7637, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 8.0286, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.7637, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.937600000000001, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 8.2699, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paiporta', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.7637, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 28.0815, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 8.0286, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 36.1064, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Algemesí', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.937600000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.7637, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 367.69440000000003, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Pozuelo de Alarcón', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 62.235, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Xàtiva', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 17.7379, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 17.7379, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 27.3108, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Benisanó', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 36.3544, 'Nombre de Pràctiques': 1, 'Punt de Destí': "L'Alcúdia", 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 4.8457, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Mislata', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 10.663799999999998, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.7637, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 5, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 8, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 4, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 17.7379, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 37.9684, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sueca', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.937600000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.3887, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 10.3529, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Foios', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 10.22, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Alaquas', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 11, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.937600000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 5, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 22.5721, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Riba Roja', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 13.6585, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 966.2381, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 10.663799999999998, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 23.585, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.7878, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Benetusser', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 173.9197, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Elche', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 6.9288, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sedaví', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 23.585, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.3887, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 19.881400000000003, 'Nombre de Pràctiques': 7, 'Punt de Destí': 'Rafelbunyol', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 23.585, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 37.499900000000004, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Guadassuar', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 69.7237, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Gandía', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 69.7237, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Gandía', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 10.663799999999998, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 17.7379, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 361.05379999999997, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Montcada i Reixac', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 966.2381, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'Valencia'})]</t>
+        </is>
+      </c>
+      <c r="L29" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Alumne': 'alumno28', 'Pràctica': 'Indenova(Pràctica 5)'})</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>alumno29</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>DAW</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>Benetusser</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>Si</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Backend': '2', 'Devops': '9', 'Disenyador': '1', 'Documentacion': '2', 'Frontend': '4', 'Fullstack': '6', 'Moviles': '3'})</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr"/>
+      <c r="H30" t="inlineStr"/>
+      <c r="I30" t="inlineStr"/>
+      <c r="J30" t="inlineStr"/>
+      <c r="K30" t="inlineStr">
+        <is>
+          <t>[DefaultMunch(None, {'Distancia': 8.6265, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776800000000001, 'Nombre de Pràctiques': 6, 'Punt de Destí': 'Valencia', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 34.1779, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Fortaleny', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 1.7895, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Massanassa', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 8.6265, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776800000000001, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Valencia', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 12.707, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 4.5936, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Albal', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 33.2689, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 2.7140999999999997, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776800000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776800000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 10.0191, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 2.7140999999999997, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 1.8020999999999998, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 12.707, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776800000000001, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'València', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 2.6365, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paiporta', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776800000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 2.7140999999999997, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 33.2689, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776800000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 10.0191, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 31.0743, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Algemesí', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 1.8020999999999998, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 12.707, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 2.7140999999999997, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 370.3071, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Pozuelo de Alarcón', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 12.707, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 57.2029, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Xàtiva', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 12.7058, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776800000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 12.7058, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776800000000001, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 32.4983, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Benisanó', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 31.3223, 'Nombre de Pràctiques': 1, 'Punt de Destí': "L'Alcúdia", 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 9.164399999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Mislata', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 8.5693, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 2.7140999999999997, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 12.707, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 12.707, 'Nombre de Pràctiques': 5, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776800000000001, 'Nombre de Pràctiques': 8, 'Punt de Destí': 'València', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776800000000001, 'Nombre de Pràctiques': 4, 'Punt de Destí': 'València', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 12.7058, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 32.9363, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sueca', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 1.8020999999999998, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 12.7466, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 12.707, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 16.5976, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Foios', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 9.2968, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Alaquas', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776800000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776800000000001, 'Nombre de Pràctiques': 11, 'Punt de Destí': 'València', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776800000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 1.8020999999999998, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776800000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776800000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776800000000001, 'Nombre de Pràctiques': 5, 'Punt de Destí': 'València', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 24.896099999999997, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Riba Roja', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 12.707, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776800000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776800000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 8.6265, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 968.8508, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 8.5693, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 12.707, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 18.5529, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Benetusser', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 168.8876, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Elche', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776800000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776800000000001, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 12.707, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 2.6135, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sedaví', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776800000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776800000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776800000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776800000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776800000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 18.5529, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 12.7466, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 26.4115, 'Nombre de Pràctiques': 7, 'Punt de Destí': 'Rafelbunyol', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776800000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 18.5529, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 32.4678, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Guadassuar', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 64.6917, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Gandía', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 64.6917, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Gandía', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776800000000001, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'València', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776800000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 8.5693, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776800000000001, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776800000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776800000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776800000000001, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 12.707, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 12.7058, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 6.776800000000001, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 367.5839, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Montcada i Reixac', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 12.707, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Benetusser'}), DefaultMunch(None, {'Distancia': 968.8508, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'Benetusser'})]</t>
+        </is>
+      </c>
+      <c r="L30" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Alumne': 'alumno29', 'Pràctica': 'Informática Alfafar S.L.(Pràctica 2)'})</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>alumno30</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>DAW</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>Catarroja</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Backend': '5', 'Devops': '2', 'Disenyador': '5', 'Documentacion': '6', 'Frontend': '4', 'Fullstack': '8', 'Moviles': '2'})</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr"/>
+      <c r="H31" t="inlineStr"/>
+      <c r="I31" t="inlineStr"/>
+      <c r="J31" t="inlineStr"/>
+      <c r="K31" t="inlineStr">
+        <is>
+          <t>[DefaultMunch(None, {'Distancia': 6.1035, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 6, 'Punt de Destí': 'Valencia', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 31.6549, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Fortaleny', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 1.2002000000000002, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Massanassa', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 6.1035, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Valencia', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 15.222700000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 2.0949, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Albal', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 35.7846, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 12.534799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 3.3274, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 15.222700000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 5.1522, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paiporta', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 35.7846, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 12.534799999999999, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 28.551299999999998, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Algemesí', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 3.3274, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 15.222700000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 372.8228, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Pozuelo de Alarcón', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 15.222700000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 54.6799, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Xàtiva', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 10.182799999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 10.182799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 35.014, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Benisanó', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 28.7993, 'Nombre de Pràctiques': 1, 'Punt de Destí': "L'Alcúdia", 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 11.6801, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Mislata', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 10.5417, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 15.222700000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 15.222700000000001, 'Nombre de Pràctiques': 5, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 8, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 4, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 10.182799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 30.4133, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sueca', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 3.3274, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 15.2623, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 15.222700000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 19.1133, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Foios', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 12.8701, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Alaquas', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 11, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 3.3274, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 5, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 27.4118, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Riba Roja', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 15.222700000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 6.1035, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 971.3665, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 10.5417, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 15.222700000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 16.0299, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 2.7334, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Benetusser', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 166.3646, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Elche', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 15.222700000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 4.2168, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sedaví', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 16.0299, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 15.2623, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 28.9272, 'Nombre de Pràctiques': 7, 'Punt de Destí': 'Rafelbunyol', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 16.0299, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 29.9449, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Guadassuar', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 62.168699999999994, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Gandía', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 62.168699999999994, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Gandía', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 10.5417, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 15.222700000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 10.182799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 370.0997, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Montcada i Reixac', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 15.222700000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 971.3665, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'Catarroja'})]</t>
+        </is>
+      </c>
+      <c r="L31" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Alumne': 'alumno30', 'Pràctica': 'Grupo Bonatel(Pràctica 1)'})</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>alumno31</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>ASIR</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>Valencia</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>Si</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Auditor': '8', 'BD': '8', 'Ciberseguridad': '10', 'Consultor': '8', 'Hardware': '7', 'HelpDesk': '9', 'Monitorizador': '10', 'Redes': '8', 'Sistemas': '10'})</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr"/>
+      <c r="H32" t="inlineStr"/>
+      <c r="I32" t="inlineStr"/>
+      <c r="J32" t="inlineStr"/>
+      <c r="K32" t="inlineStr">
+        <is>
+          <t>[DefaultMunch(None, {'Distancia': 13.6585, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 6, 'Punt de Destí': 'Valencia', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 39.21, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Fortaleny', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 8.8391, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Massanassa', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 13.6585, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Valencia', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 11.0844, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Albal', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 28.0815, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.7637, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 8.0286, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.7637, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.937600000000001, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 8.2699, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paiporta', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.7637, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 28.0815, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 8.0286, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 36.1064, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Algemesí', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.937600000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.7637, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 367.69440000000003, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Pozuelo de Alarcón', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 62.235, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Xàtiva', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 17.7379, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 17.7379, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 27.3108, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Benisanó', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 36.3544, 'Nombre de Pràctiques': 1, 'Punt de Destí': "L'Alcúdia", 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 4.8457, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Mislata', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 10.663799999999998, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.7637, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 5, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 8, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 4, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 17.7379, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 37.9684, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sueca', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.937600000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.3887, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 10.3529, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Foios', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 10.22, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Alaquas', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 11, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.937600000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 5, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 22.5721, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Riba Roja', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 13.6585, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 966.2381, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 10.663799999999998, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 23.585, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.7878, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Benetusser', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 173.9197, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Elche', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 6.9288, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sedaví', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 23.585, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.3887, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 19.881400000000003, 'Nombre de Pràctiques': 7, 'Punt de Destí': 'Rafelbunyol', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 23.585, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 37.499900000000004, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Guadassuar', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 69.7237, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Gandía', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 69.7237, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Gandía', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 10.663799999999998, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 17.7379, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 361.05379999999997, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Montcada i Reixac', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 966.2381, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'Valencia'})]</t>
+        </is>
+      </c>
+      <c r="L32" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Alumne': 'alumno31', 'Pràctica': 'ISECO(Pràctica 3)'})</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>alumno32</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>ASIR</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>Sueca</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>Si</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Auditor': '9', 'BD': '8', 'Ciberseguridad': '6', 'Consultor': '9', 'Hardware': '10', 'HelpDesk': '4', 'Monitorizador': '10', 'Redes': '8', 'Sistemas': '10'})</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr"/>
+      <c r="H33" t="inlineStr"/>
+      <c r="I33" t="inlineStr"/>
+      <c r="J33" t="inlineStr"/>
+      <c r="K33" t="inlineStr">
+        <is>
+          <t>[DefaultMunch(None, {'Distancia': 23.7486, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Sueca'}), DefaultMunch(None, {'Distancia': 36.713, 'Nombre de Pràctiques': 6, 'Punt de Destí': 'Valencia', 'Punt de Partida': 'Sueca'}), DefaultMunch(None, {'Distancia': 3.0088000000000004, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Fortaleny', 'Punt de Partida': 'Sueca'}), DefaultMunch(None, {'Distancia': 30.105700000000002, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Massanassa', 'Punt de Partida': 'Sueca'}), DefaultMunch(None, {'Distancia': 23.7486, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Sueca'}), DefaultMunch(None, {'Distancia': 36.713, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Valencia', 'Punt de Partida': 'Sueca'}), DefaultMunch(None, {'Distancia': 43.9989, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Sueca'}), DefaultMunch(None, {'Distancia': 29.9765, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Albal', 'Punt de Partida': 'Sueca'}), DefaultMunch(None, {'Distancia': 67.0419, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'Sueca'}), DefaultMunch(None, {'Distancia': 29.2885, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Sueca'}), DefaultMunch(None, {'Distancia': 36.713, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Sueca'}), DefaultMunch(None, {'Distancia': 36.713, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Sueca'}), DefaultMunch(None, {'Distancia': 41.307900000000004, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'Sueca'}), DefaultMunch(None, {'Distancia': 29.2885, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Sueca'}), DefaultMunch(None, {'Distancia': 31.5906, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Sueca'}), DefaultMunch(None, {'Distancia': 43.9989, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Sueca'}), DefaultMunch(None, {'Distancia': 36.713, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'València', 'Punt de Partida': 'Sueca'}), DefaultMunch(None, {'Distancia': 34.0577, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paiporta', 'Punt de Partida': 'Sueca'}), DefaultMunch(None, {'Distancia': 36.713, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Sueca'}), DefaultMunch(None, {'Distancia': 29.2885, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Sueca'}), DefaultMunch(None, {'Distancia': 67.0419, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'Sueca'}), DefaultMunch(None, {'Distancia': 36.713, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Sueca'}), DefaultMunch(None, {'Distancia': 41.307900000000004, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'Sueca'}), DefaultMunch(None, {'Distancia': 12.5595, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Algemesí', 'Punt de Partida': 'Sueca'}), DefaultMunch(None, {'Distancia': 31.5906, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Sueca'}), DefaultMunch(None, {'Distancia': 43.9989, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Sueca'}), DefaultMunch(None, {'Distancia': 29.2885, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Sueca'}), DefaultMunch(None, {'Distancia': 390.3875, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Pozuelo de Alarcón', 'Punt de Partida': 'Sueca'}), DefaultMunch(None, {'Distancia': 43.9989, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Sueca'}), DefaultMunch(None, {'Distancia': 38.3182, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Xàtiva', 'Punt de Partida': 'Sueca'}), DefaultMunch(None, {'Distancia': 25.6294, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Sueca'}), DefaultMunch(None, {'Distancia': 36.713, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Sueca'}), DefaultMunch(None, {'Distancia': 25.6294, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Sueca'}), DefaultMunch(None, {'Distancia': 36.713, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Sueca'}), DefaultMunch(None, {'Distancia': 66.2712, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Benisanó', 'Punt de Partida': 'Sueca'}), DefaultMunch(None, {'Distancia': 22.6687, 'Nombre de Pràctiques': 1, 'Punt de Destí': "L'Alcúdia", 'Punt de Partida': 'Sueca'}), DefaultMunch(None, {'Distancia': 40.453199999999995, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Mislata', 'Punt de Partida': 'Sueca'}), DefaultMunch(None, {'Distancia': 35.4418, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Sueca'}), DefaultMunch(None, {'Distancia': 29.2885, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Sueca'}), DefaultMunch(None, {'Distancia': 43.9989, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Sueca'}), DefaultMunch(None, {'Distancia': 43.9989, 'Nombre de Pràctiques': 5, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Sueca'}), DefaultMunch(None, {'Distancia': 36.713, 'Nombre de Pràctiques': 8, 'Punt de Destí': 'València', 'Punt de Partida': 'Sueca'}), DefaultMunch(None, {'Distancia': 36.713, 'Nombre de Pràctiques': 4, 'Punt de Destí': 'València', 'Punt de Partida': 'Sueca'}), DefaultMunch(None, {'Distancia': 25.6294, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Sueca'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sueca', 'Punt de Partida': 'Sueca'}), DefaultMunch(None, {'Distancia': 31.5906, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Sueca'}), DefaultMunch(None, {'Distancia': 45.2891, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Sueca'}), DefaultMunch(None, {'Distancia': 43.9989, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Sueca'}), DefaultMunch(None, {'Distancia': 46.2666, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Foios', 'Punt de Partida': 'Sueca'}), DefaultMunch(None, {'Distancia': 37.9107, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Alaquas', 'Punt de Partida': 'Sueca'}), DefaultMunch(None, {'Distancia': 36.713, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Sueca'}), DefaultMunch(None, {'Distancia': 36.713, 'Nombre de Pràctiques': 11, 'Punt de Destí': 'València', 'Punt de Partida': 'Sueca'}), DefaultMunch(None, {'Distancia': 36.713, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Sueca'}), DefaultMunch(None, {'Distancia': 31.5906, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Sueca'}), DefaultMunch(None, {'Distancia': 36.713, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Sueca'}), DefaultMunch(None, {'Distancia': 36.713, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Sueca'}), DefaultMunch(None, {'Distancia': 36.713, 'Nombre de Pràctiques': 5, 'Punt de Destí': 'València', 'Punt de Partida': 'Sueca'}), DefaultMunch(None, {'Distancia': 51.4788, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Riba Roja', 'Punt de Partida': 'Sueca'}), DefaultMunch(None, {'Distancia': 43.9989, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Sueca'}), DefaultMunch(None, {'Distancia': 36.713, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Sueca'}), DefaultMunch(None, {'Distancia': 36.713, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Sueca'}), DefaultMunch(None, {'Distancia': 23.7486, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Sueca'}), DefaultMunch(None, {'Distancia': 988.9312, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'Sueca'}), DefaultMunch(None, {'Distancia': 35.4418, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Sueca'}), DefaultMunch(None, {'Distancia': 43.9989, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Sueca'}), DefaultMunch(None, {'Distancia': 18.207099999999997, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Sueca'}), DefaultMunch(None, {'Distancia': 31.638900000000003, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Benetusser', 'Punt de Partida': 'Sueca'}), DefaultMunch(None, {'Distancia': 155.0193, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Elche', 'Punt de Partida': 'Sueca'}), DefaultMunch(None, {'Distancia': 36.713, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Sueca'}), DefaultMunch(None, {'Distancia': 36.713, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Sueca'}), DefaultMunch(None, {'Distancia': 43.9989, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Sueca'}), DefaultMunch(None, {'Distancia': 31.715799999999998, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sedaví', 'Punt de Partida': 'Sueca'}), DefaultMunch(None, {'Distancia': 36.713, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Sueca'}), DefaultMunch(None, {'Distancia': 36.713, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Sueca'}), DefaultMunch(None, {'Distancia': 36.713, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Sueca'}), DefaultMunch(None, {'Distancia': 36.713, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Sueca'}), DefaultMunch(None, {'Distancia': 36.713, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Sueca'}), DefaultMunch(None, {'Distancia': 18.207099999999997, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Sueca'}), DefaultMunch(None, {'Distancia': 45.2891, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Sueca'}), DefaultMunch(None, {'Distancia': 66.176, 'Nombre de Pràctiques': 7, 'Punt de Destí': 'Rafelbunyol', 'Punt de Partida': 'Sueca'}), DefaultMunch(None, {'Distancia': 36.713, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Sueca'}), DefaultMunch(None, {'Distancia': 18.207099999999997, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Sueca'}), DefaultMunch(None, {'Distancia': 18.4972, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Guadassuar', 'Punt de Partida': 'Sueca'}), DefaultMunch(None, {'Distancia': 31.9642, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Gandía', 'Punt de Partida': 'Sueca'}), DefaultMunch(None, {'Distancia': 31.9642, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Gandía', 'Punt de Partida': 'Sueca'}), DefaultMunch(None, {'Distancia': 36.713, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'València', 'Punt de Partida': 'Sueca'}), DefaultMunch(None, {'Distancia': 36.713, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Sueca'}), DefaultMunch(None, {'Distancia': 35.4418, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Sueca'}), DefaultMunch(None, {'Distancia': 36.713, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Sueca'}), DefaultMunch(None, {'Distancia': 36.713, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Sueca'}), DefaultMunch(None, {'Distancia': 36.713, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Sueca'}), DefaultMunch(None, {'Distancia': 36.713, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Sueca'}), DefaultMunch(None, {'Distancia': 43.9989, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Sueca'}), DefaultMunch(None, {'Distancia': 25.6294, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Sueca'}), DefaultMunch(None, {'Distancia': 36.713, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Sueca'}), DefaultMunch(None, {'Distancia': 406.1854, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Montcada i Reixac', 'Punt de Partida': 'Sueca'}), DefaultMunch(None, {'Distancia': 43.9989, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Sueca'}), DefaultMunch(None, {'Distancia': 988.9312, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'Sueca'})]</t>
+        </is>
+      </c>
+      <c r="L33" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Alumne': 'alumno32', 'Pràctica': 'Infordinadors(Pràctica 1)'})</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>alumno33</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>ASIR</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>Albal</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>Si</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Auditor': '7', 'BD': '10', 'Ciberseguridad': '9', 'Consultor': '7', 'Hardware': '7', 'HelpDesk': '6', 'Monitorizador': '7', 'Redes': '8', 'Sistemas': '10'})</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr"/>
+      <c r="H34" t="inlineStr"/>
+      <c r="I34" t="inlineStr"/>
+      <c r="J34" t="inlineStr"/>
+      <c r="K34" t="inlineStr">
+        <is>
+          <t>[DefaultMunch(None, {'Distancia': 5.904, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 6, 'Punt de Destí': 'Valencia', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 31.4555, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Fortaleny', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 3.7565, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Massanassa', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 5.904, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Valencia', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 16.428099999999997, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Albal', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 36.9901, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 2.3773, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 13.7403, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 2.3773, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 5.59, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 16.428099999999997, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 6.3576999999999995, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paiporta', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 2.3773, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 36.9901, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 13.7403, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 28.3518, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Algemesí', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 5.59, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 16.428099999999997, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 2.3773, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 374.0283, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Pozuelo de Alarcón', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 16.428099999999997, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 54.4804, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Xàtiva', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 9.9833, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 9.9833, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 36.2194, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Benisanó', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 28.5998, 'Nombre de Pràctiques': 1, 'Punt de Destí': "L'Alcúdia", 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 12.8855, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Mislata', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 8.44, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 2.3773, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 16.428099999999997, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 16.428099999999997, 'Nombre de Pràctiques': 5, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 8, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 4, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 9.9833, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 30.2138, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sueca', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 5.59, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 16.4677, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 16.428099999999997, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 20.3187, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Foios', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.7685, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Alaquas', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 11, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 5.59, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 5, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 28.6172, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Riba Roja', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 16.428099999999997, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 5.904, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 972.572, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 8.44, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 16.428099999999997, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 15.8304, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 4.996, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Benetusser', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 166.1651, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Elche', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 16.428099999999997, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 7.253100000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sedaví', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 15.8304, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 16.4677, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 30.1327, 'Nombre de Pràctiques': 7, 'Punt de Destí': 'Rafelbunyol', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 15.8304, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 29.7454, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Guadassuar', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 61.969199999999994, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Gandía', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 61.969199999999994, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Gandía', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 8.44, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 16.428099999999997, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 9.9833, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 371.3051, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Montcada i Reixac', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 16.428099999999997, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 972.572, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'Albal'})]</t>
+        </is>
+      </c>
+      <c r="L34" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Alumne': 'alumno33', 'Pràctica': 'Media'})</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>alumno34</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>ASIR</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>Valencia</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>Si</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Auditor': '2', 'BD': '2', 'Ciberseguridad': '4', 'Consultor': '3', 'Hardware': '4', 'HelpDesk': '2', 'Monitorizador': '3', 'Redes': '1', 'Sistemas': '3'})</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr"/>
+      <c r="H35" t="inlineStr"/>
+      <c r="I35" t="inlineStr"/>
+      <c r="J35" t="inlineStr"/>
+      <c r="K35" t="inlineStr">
+        <is>
+          <t>[DefaultMunch(None, {'Distancia': 13.6585, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 6, 'Punt de Destí': 'Valencia', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 39.21, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Fortaleny', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 8.8391, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Massanassa', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 13.6585, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Valencia', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 11.0844, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Albal', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 28.0815, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.7637, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 8.0286, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.7637, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.937600000000001, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 8.2699, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paiporta', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.7637, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 28.0815, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 8.0286, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 36.1064, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Algemesí', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.937600000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.7637, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 367.69440000000003, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Pozuelo de Alarcón', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 62.235, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Xàtiva', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 17.7379, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 17.7379, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 27.3108, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Benisanó', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 36.3544, 'Nombre de Pràctiques': 1, 'Punt de Destí': "L'Alcúdia", 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 4.8457, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Mislata', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 10.663799999999998, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.7637, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 5, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 8, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 4, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 17.7379, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 37.9684, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sueca', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.937600000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.3887, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 10.3529, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Foios', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 10.22, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Alaquas', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 11, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.937600000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 5, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 22.5721, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Riba Roja', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 13.6585, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 966.2381, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 10.663799999999998, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 23.585, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.7878, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Benetusser', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 173.9197, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Elche', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 6.9288, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sedaví', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 23.585, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.3887, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 19.881400000000003, 'Nombre de Pràctiques': 7, 'Punt de Destí': 'Rafelbunyol', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 23.585, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 37.499900000000004, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Guadassuar', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 69.7237, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Gandía', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 69.7237, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Gandía', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 10.663799999999998, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 17.7379, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 361.05379999999997, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Montcada i Reixac', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 966.2381, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'Valencia'})]</t>
+        </is>
+      </c>
+      <c r="L35" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Alumne': 'alumno34', 'Pràctica': 'Ahora(Pràctica 4)'})</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>alumno35</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>ASIR</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>La pobla de Vallbona</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>Si</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Auditor': '7', 'BD': '8', 'Ciberseguridad': '8', 'Consultor': '7', 'Hardware': '8', 'HelpDesk': '7', 'Monitorizador': '6', 'Redes': '6', 'Sistemas': '9'})</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr"/>
+      <c r="H36" t="inlineStr"/>
+      <c r="I36" t="inlineStr"/>
+      <c r="J36" t="inlineStr"/>
+      <c r="K36" t="inlineStr">
+        <is>
+          <t>[DefaultMunch(None, {'Distancia': 35.314800000000005, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'La pobla de Vallbona'}), DefaultMunch(None, {'Distancia': 22.1695, 'Nombre de Pràctiques': 6, 'Punt de Destí': 'Valencia', 'Punt de Partida': 'La pobla de Vallbona'}), DefaultMunch(None, {'Distancia': 63.2846, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Fortaleny', 'Punt de Partida': 'La pobla de Vallbona'}), DefaultMunch(None, {'Distancia': 27.679599999999997, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Massanassa', 'Punt de Partida': 'La pobla de Vallbona'}), DefaultMunch(None, {'Distancia': 35.314800000000005, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'La pobla de Vallbona'}), DefaultMunch(None, {'Distancia': 22.1695, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Valencia', 'Punt de Partida': 'La pobla de Vallbona'}), DefaultMunch(None, {'Distancia': 16.390700000000002, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'La pobla de Vallbona'}), DefaultMunch(None, {'Distancia': 29.9249, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Albal', 'Punt de Partida': 'La pobla de Vallbona'}), DefaultMunch(None, {'Distancia': 5.5652, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'La pobla de Vallbona'}), DefaultMunch(None, {'Distancia': 28.604200000000002, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'La pobla de Vallbona'}), DefaultMunch(None, {'Distancia': 22.1695, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'La pobla de Vallbona'}), DefaultMunch(None, {'Distancia': 22.1695, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'La pobla de Vallbona'}), DefaultMunch(None, {'Distancia': 20.0334, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'La pobla de Vallbona'}), DefaultMunch(None, {'Distancia': 28.604200000000002, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'La pobla de Vallbona'}), DefaultMunch(None, {'Distancia': 27.5973, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'La pobla de Vallbona'}), DefaultMunch(None, {'Distancia': 16.390700000000002, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'La pobla de Vallbona'}), DefaultMunch(None, {'Distancia': 22.1695, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'València', 'Punt de Partida': 'La pobla de Vallbona'}), DefaultMunch(None, {'Distancia': 26.3733, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paiporta', 'Punt de Partida': 'La pobla de Vallbona'}), DefaultMunch(None, {'Distancia': 22.1695, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'La pobla de Vallbona'}), DefaultMunch(None, {'Distancia': 28.604200000000002, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'La pobla de Vallbona'}), DefaultMunch(None, {'Distancia': 5.5652, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'La pobla de Vallbona'}), DefaultMunch(None, {'Distancia': 22.1695, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'La pobla de Vallbona'}), DefaultMunch(None, {'Distancia': 20.0334, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'La pobla de Vallbona'}), DefaultMunch(None, {'Distancia': 60.181, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Algemesí', 'Punt de Partida': 'La pobla de Vallbona'}), DefaultMunch(None, {'Distancia': 27.5973, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'La pobla de Vallbona'}), DefaultMunch(None, {'Distancia': 16.390700000000002, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'La pobla de Vallbona'}), DefaultMunch(None, {'Distancia': 28.604200000000002, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'La pobla de Vallbona'}), DefaultMunch(None, {'Distancia': 361.64959999999996, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Pozuelo de Alarcón', 'Punt de Partida': 'La pobla de Vallbona'}), DefaultMunch(None, {'Distancia': 16.390700000000002, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'La pobla de Vallbona'}), DefaultMunch(None, {'Distancia': 86.3296, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Xàtiva', 'Punt de Partida': 'La pobla de Vallbona'}), DefaultMunch(None, {'Distancia': 38.6525, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'La pobla de Vallbona'}), DefaultMunch(None, {'Distancia': 22.1695, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'La pobla de Vallbona'}), DefaultMunch(None, {'Distancia': 38.6525, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'La pobla de Vallbona'}), DefaultMunch(None, {'Distancia': 22.1695, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'La pobla de Vallbona'}), DefaultMunch(None, {'Distancia': 3.3224, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Benisanó', 'Punt de Partida': 'La pobla de Vallbona'}), DefaultMunch(None, {'Distancia': 60.449, 'Nombre de Pràctiques': 1, 'Punt de Destí': "L'Alcúdia", 'Punt de Partida': 'La pobla de Vallbona'}), DefaultMunch(None, {'Distancia': 21.7321, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Mislata', 'Punt de Partida': 'La pobla de Vallbona'}), DefaultMunch(None, {'Distancia': 27.0966, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'La pobla de Vallbona'}), DefaultMunch(None, {'Distancia': 28.604200000000002, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'La pobla de Vallbona'}), DefaultMunch(None, {'Distancia': 16.390700000000002, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'La pobla de Vallbona'}), DefaultMunch(None, {'Distancia': 16.390700000000002, 'Nombre de Pràctiques': 5, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'La pobla de Vallbona'}), DefaultMunch(None, {'Distancia': 22.1695, 'Nombre de Pràctiques': 8, 'Punt de Destí': 'València', 'Punt de Partida': 'La pobla de Vallbona'}), DefaultMunch(None, {'Distancia': 22.1695, 'Nombre de Pràctiques': 4, 'Punt de Destí': 'València', 'Punt de Partida': 'La pobla de Vallbona'}), DefaultMunch(None, {'Distancia': 38.6525, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'La pobla de Vallbona'}), DefaultMunch(None, {'Distancia': 62.043, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sueca', 'Punt de Partida': 'La pobla de Vallbona'}), DefaultMunch(None, {'Distancia': 27.5973, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'La pobla de Vallbona'}), DefaultMunch(None, {'Distancia': 17.217299999999998, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'La pobla de Vallbona'}), DefaultMunch(None, {'Distancia': 16.390700000000002, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'La pobla de Vallbona'}), DefaultMunch(None, {'Distancia': 30.973200000000002, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Foios', 'Punt de Partida': 'La pobla de Vallbona'}), DefaultMunch(None, {'Distancia': 25.2483, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Alaquas', 'Punt de Partida': 'La pobla de Vallbona'}), DefaultMunch(None, {'Distancia': 22.1695, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'La pobla de Vallbona'}), DefaultMunch(None, {'Distancia': 22.1695, 'Nombre de Pràctiques': 11, 'Punt de Destí': 'València', 'Punt de Partida': 'La pobla de Vallbona'}), DefaultMunch(None, {'Distancia': 22.1695, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'La pobla de Vallbona'}), DefaultMunch(None, {'Distancia': 27.5973, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'La pobla de Vallbona'}), DefaultMunch(None, {'Distancia': 22.1695, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'La pobla de Vallbona'}), DefaultMunch(None, {'Distancia': 22.1695, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'La pobla de Vallbona'}), DefaultMunch(None, {'Distancia': 22.1695, 'Nombre de Pràctiques': 5, 'Punt de Destí': 'València', 'Punt de Partida': 'La pobla de Vallbona'}), DefaultMunch(None, {'Distancia': 7.2779, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Riba Roja', 'Punt de Partida': 'La pobla de Vallbona'}), DefaultMunch(None, {'Distancia': 16.390700000000002, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'La pobla de Vallbona'}), DefaultMunch(None, {'Distancia': 22.1695, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'La pobla de Vallbona'}), DefaultMunch(None, {'Distancia': 22.1695, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'La pobla de Vallbona'}), DefaultMunch(None, {'Distancia': 35.314800000000005, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Silla', 'Punt de Partida': 'La pobla de Vallbona'}), DefaultMunch(None, {'Distancia': 960.1933, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'La pobla de Vallbona'}), DefaultMunch(None, {'Distancia': 27.0966, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'La pobla de Vallbona'}), DefaultMunch(None, {'Distancia': 16.390700000000002, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'La pobla de Vallbona'}), DefaultMunch(None, {'Distancia': 47.6596, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'La pobla de Vallbona'}), DefaultMunch(None, {'Distancia': 26.6283, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Benetusser', 'Punt de Partida': 'La pobla de Vallbona'}), DefaultMunch(None, {'Distancia': 198.0143, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Elche', 'Punt de Partida': 'La pobla de Vallbona'}), DefaultMunch(None, {'Distancia': 22.1695, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'La pobla de Vallbona'}), DefaultMunch(None, {'Distancia': 22.1695, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'La pobla de Vallbona'}), DefaultMunch(None, {'Distancia': 16.390700000000002, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'La pobla de Vallbona'}), DefaultMunch(None, {'Distancia': 27.0024, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sedaví', 'Punt de Partida': 'La pobla de Vallbona'}), DefaultMunch(None, {'Distancia': 22.1695, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'La pobla de Vallbona'}), DefaultMunch(None, {'Distancia': 22.1695, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'La pobla de Vallbona'}), DefaultMunch(None, {'Distancia': 22.1695, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'La pobla de Vallbona'}), DefaultMunch(None, {'Distancia': 22.1695, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'La pobla de Vallbona'}), DefaultMunch(None, {'Distancia': 22.1695, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'La pobla de Vallbona'}), DefaultMunch(None, {'Distancia': 47.6596, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'La pobla de Vallbona'}), DefaultMunch(None, {'Distancia': 17.217299999999998, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'La pobla de Vallbona'}), DefaultMunch(None, {'Distancia': 27.2815, 'Nombre de Pràctiques': 7, 'Punt de Destí': 'Rafelbunyol', 'Punt de Partida': 'La pobla de Vallbona'}), DefaultMunch(None, {'Distancia': 22.1695, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'La pobla de Vallbona'}), DefaultMunch(None, {'Distancia': 47.6596, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'La pobla de Vallbona'}), DefaultMunch(None, {'Distancia': 61.5945, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Guadassuar', 'Punt de Partida': 'La pobla de Vallbona'}), DefaultMunch(None, {'Distancia': 93.7983, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Gandía', 'Punt de Partida': 'La pobla de Vallbona'}), DefaultMunch(None, {'Distancia': 93.7983, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Gandía', 'Punt de Partida': 'La pobla de Vallbona'}), DefaultMunch(None, {'Distancia': 22.1695, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'València', 'Punt de Partida': 'La pobla de Vallbona'}), DefaultMunch(None, {'Distancia': 22.1695, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'La pobla de Vallbona'}), DefaultMunch(None, {'Distancia': 27.0966, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'La pobla de Vallbona'}), DefaultMunch(None, {'Distancia': 22.1695, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'La pobla de Vallbona'}), DefaultMunch(None, {'Distancia': 22.1695, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'La pobla de Vallbona'}), DefaultMunch(None, {'Distancia': 22.1695, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'La pobla de Vallbona'}), DefaultMunch(None, {'Distancia': 22.1695, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'La pobla de Vallbona'}), DefaultMunch(None, {'Distancia': 16.390700000000002, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'La pobla de Vallbona'}), DefaultMunch(None, {'Distancia': 38.6525, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'La pobla de Vallbona'}), DefaultMunch(None, {'Distancia': 22.1695, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'La pobla de Vallbona'}), DefaultMunch(None, {'Distancia': 367.2908, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Montcada i Reixac', 'Punt de Partida': 'La pobla de Vallbona'}), DefaultMunch(None, {'Distancia': 16.390700000000002, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'La pobla de Vallbona'}), DefaultMunch(None, {'Distancia': 960.1933, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'La pobla de Vallbona'})]</t>
+        </is>
+      </c>
+      <c r="L36" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Alumne': 'alumno35', 'Pràctica': 'Consultoria Informática JAM, S.L.(Pràctica 1)'})</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>alumno36</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>ASIR</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>Sollana</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>Si</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Auditor': '7', 'BD': '7', 'Ciberseguridad': '7', 'Consultor': '7', 'Hardware': '7', 'HelpDesk': '7', 'Monitorizador': '7', 'Redes': '7', 'Sistemas': '7'})</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr"/>
+      <c r="H37" t="inlineStr"/>
+      <c r="I37" t="inlineStr"/>
+      <c r="J37" t="inlineStr"/>
+      <c r="K37" t="inlineStr">
+        <is>
+          <t>[DefaultMunch(None, {'Distancia': 15.9393, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 28.9037, 'Nombre de Pràctiques': 6, 'Punt de Destí': 'Valencia', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 13.506, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Fortaleny', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 22.2965, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Massanassa', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 15.9393, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 28.9037, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Valencia', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 36.1896, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 22.1673, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Albal', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 59.2326, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 21.4793, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 28.9037, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 28.9037, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 33.4987, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 21.4793, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 23.781299999999998, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 36.1896, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 28.9037, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'València', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 26.2484, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paiporta', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 28.9037, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 21.4793, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 59.2326, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 28.9037, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 33.4987, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 15.0618, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Algemesí', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 23.781299999999998, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 36.1896, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 21.4793, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 382.57820000000004, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Pozuelo de Alarcón', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 36.1896, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 46.8598, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Xàtiva', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 17.8201, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 28.9037, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 17.8201, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 28.9037, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 58.4619, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Benisanó', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 20.979200000000002, 'Nombre de Pràctiques': 1, 'Punt de Destí': "L'Alcúdia", 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 32.6439, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Mislata', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 27.6325, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 21.4793, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 36.1896, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 36.1896, 'Nombre de Pràctiques': 5, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 28.9037, 'Nombre de Pràctiques': 8, 'Punt de Destí': 'València', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 28.9037, 'Nombre de Pràctiques': 4, 'Punt de Destí': 'València', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 17.8201, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 12.2644, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sueca', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 23.781299999999998, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 37.479800000000004, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 36.1896, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 38.457300000000004, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Foios', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 30.1014, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Alaquas', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 28.9037, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 28.9037, 'Nombre de Pràctiques': 11, 'Punt de Destí': 'València', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 28.9037, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 23.781299999999998, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 28.9037, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 28.9037, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 28.9037, 'Nombre de Pràctiques': 5, 'Punt de Destí': 'València', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 43.6695, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Riba Roja', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 36.1896, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 28.9037, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 28.9037, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 15.9393, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 981.1219, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 27.6325, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 36.1896, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 5.4293000000000005, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 23.8296, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Benetusser', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 158.5445, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Elche', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 28.9037, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 28.9037, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 36.1896, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 23.9065, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sedaví', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 28.9037, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 28.9037, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 28.9037, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 28.9037, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 28.9037, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 5.4293000000000005, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 37.479800000000004, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 58.366699999999994, 'Nombre de Pràctiques': 7, 'Punt de Destí': 'Rafelbunyol', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 28.9037, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 5.4293000000000005, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 19.6719, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Guadassuar', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 42.441199999999995, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Gandía', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 42.441199999999995, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Gandía', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 28.9037, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'València', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 28.9037, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 27.6325, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 28.9037, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 28.9037, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 28.9037, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 28.9037, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 36.1896, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 17.8201, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 28.9037, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 398.37609999999995, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Montcada i Reixac', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 36.1896, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 981.1219, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'Sollana'})]</t>
+        </is>
+      </c>
+      <c r="L37" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Alumne': 'alumno36', 'Pràctica': 'Red902(Pràctica 1)'})</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>alumno37</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>ASIR</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>L'Olleria</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>Si</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Auditor': '10', 'BD': '9', 'Ciberseguridad': '10', 'Consultor': '10', 'Hardware': '8', 'HelpDesk': '8', 'Monitorizador': '9', 'Redes': '9', 'Sistemas': '9'})</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr"/>
+      <c r="H38" t="inlineStr"/>
+      <c r="I38" t="inlineStr"/>
+      <c r="J38" t="inlineStr"/>
+      <c r="K38" t="inlineStr">
+        <is>
+          <t>[DefaultMunch(None, {'Distancia': 62.0908, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': "L'Olleria"}), DefaultMunch(None, {'Distancia': 75.0552, 'Nombre de Pràctiques': 6, 'Punt de Destí': 'Valencia', 'Punt de Partida': "L'Olleria"}), DefaultMunch(None, {'Distancia': 55.172, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Fortaleny', 'Punt de Partida': "L'Olleria"}), DefaultMunch(None, {'Distancia': 68.44789999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Massanassa', 'Punt de Partida': "L'Olleria"}), DefaultMunch(None, {'Distancia': 62.0908, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': "L'Olleria"}), DefaultMunch(None, {'Distancia': 75.0552, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Valencia', 'Punt de Partida': "L'Olleria"}), DefaultMunch(None, {'Distancia': 82.341, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': "L'Olleria"}), DefaultMunch(None, {'Distancia': 68.31869999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Albal', 'Punt de Partida': "L'Olleria"}), DefaultMunch(None, {'Distancia': 105.40610000000001, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Lliria', 'Punt de Partida': "L'Olleria"}), DefaultMunch(None, {'Distancia': 67.63069999999999, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Catarroja', 'Punt de Partida': "L'Olleria"}), DefaultMunch(None, {'Distancia': 75.0552, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': "L'Olleria"}), DefaultMunch(None, {'Distancia': 75.0552, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': "L'Olleria"}), DefaultMunch(None, {'Distancia': 79.65010000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': "L'Olleria"}), DefaultMunch(None, {'Distancia': 67.63069999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': "L'Olleria"}), DefaultMunch(None, {'Distancia': 69.9328, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Alfafar', 'Punt de Partida': "L'Olleria"}), DefaultMunch(None, {'Distancia': 82.341, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': "L'Olleria"}), DefaultMunch(None, {'Distancia': 75.0552, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'València', 'Punt de Partida': "L'Olleria"}), DefaultMunch(None, {'Distancia': 72.39989999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paiporta', 'Punt de Partida': "L'Olleria"}), DefaultMunch(None, {'Distancia': 75.0552, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': "L'Olleria"}), DefaultMunch(None, {'Distancia': 67.63069999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': "L'Olleria"}), DefaultMunch(None, {'Distancia': 105.40610000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Lliria', 'Punt de Partida': "L'Olleria"}), DefaultMunch(None, {'Distancia': 75.0552, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': "L'Olleria"}), DefaultMunch(None, {'Distancia': 79.65010000000001, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': "L'Olleria"}), DefaultMunch(None, {'Distancia': 46.489, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Algemesí', 'Punt de Partida': "L'Olleria"}), DefaultMunch(None, {'Distancia': 69.9328, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': "L'Olleria"}), DefaultMunch(None, {'Distancia': 82.341, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': "L'Olleria"}), DefaultMunch(None, {'Distancia': 67.63069999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Catarroja', 'Punt de Partida': "L'Olleria"}), DefaultMunch(None, {'Distancia': 404.0675, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Pozuelo de Alarcón', 'Punt de Partida': "L'Olleria"}), DefaultMunch(None, {'Distancia': 82.341, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': "L'Olleria"}), DefaultMunch(None, {'Distancia': 16.4962, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Xàtiva', 'Punt de Partida': "L'Olleria"}), DefaultMunch(None, {'Distancia': 64.0076, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Picassent', 'Punt de Partida': "L'Olleria"}), DefaultMunch(None, {'Distancia': 75.0552, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': "L'Olleria"}), DefaultMunch(None, {'Distancia': 64.0076, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': "L'Olleria"}), DefaultMunch(None, {'Distancia': 75.0552, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': "L'Olleria"}), DefaultMunch(None, {'Distancia': 104.6355, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Benisanó', 'Punt de Partida': "L'Olleria"}), DefaultMunch(None, {'Distancia': 39.6941, 'Nombre de Pràctiques': 1, 'Punt de Destí': "L'Alcúdia", 'Punt de Partida': "L'Olleria"}), DefaultMunch(None, {'Distancia': 78.7954, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Mislata', 'Punt de Partida': "L'Olleria"}), DefaultMunch(None, {'Distancia': 73.806, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Torrent', 'Punt de Partida': "L'Olleria"}), DefaultMunch(None, {'Distancia': 67.63069999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': "L'Olleria"}), DefaultMunch(None, {'Distancia': 82.341, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': "L'Olleria"}), DefaultMunch(None, {'Distancia': 82.341, 'Nombre de Pràctiques': 5, 'Punt de Destí': 'Paterna', 'Punt de Partida': "L'Olleria"}), DefaultMunch(None, {'Distancia': 75.0552, 'Nombre de Pràctiques': 8, 'Punt de Destí': 'València', 'Punt de Partida': "L'Olleria"}), DefaultMunch(None, {'Distancia': 75.0552, 'Nombre de Pràctiques': 4, 'Punt de Destí': 'València', 'Punt de Partida': "L'Olleria"}), DefaultMunch(None, {'Distancia': 64.0076, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': "L'Olleria"}), DefaultMunch(None, {'Distancia': 55.8939, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sueca', 'Punt de Partida': "L'Olleria"}), DefaultMunch(None, {'Distancia': 69.9328, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': "L'Olleria"}), DefaultMunch(None, {'Distancia': 83.6313, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': "L'Olleria"}), DefaultMunch(None, {'Distancia': 82.341, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': "L'Olleria"}), DefaultMunch(None, {'Distancia': 84.6088, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Foios', 'Punt de Partida': "L'Olleria"}), DefaultMunch(None, {'Distancia': 76.275, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Alaquas', 'Punt de Partida': "L'Olleria"}), DefaultMunch(None, {'Distancia': 75.0552, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': "L'Olleria"}), DefaultMunch(None, {'Distancia': 75.0552, 'Nombre de Pràctiques': 11, 'Punt de Destí': 'València', 'Punt de Partida': "L'Olleria"}), DefaultMunch(None, {'Distancia': 75.0552, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': "L'Olleria"}), DefaultMunch(None, {'Distancia': 69.9328, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': "L'Olleria"}), DefaultMunch(None, {'Distancia': 75.0552, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': "L'Olleria"}), DefaultMunch(None, {'Distancia': 75.0552, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': "L'Olleria"}), DefaultMunch(None, {'Distancia': 75.0552, 'Nombre de Pràctiques': 5, 'Punt de Destí': 'València', 'Punt de Partida': "L'Olleria"}), DefaultMunch(None, {'Distancia': 89.843, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Riba Roja', 'Punt de Partida': "L'Olleria"}), DefaultMunch(None, {'Distancia': 82.341, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': "L'Olleria"}), DefaultMunch(None, {'Distancia': 75.0552, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': "L'Olleria"}), DefaultMunch(None, {'Distancia': 75.0552, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': "L'Olleria"}), DefaultMunch(None, {'Distancia': 62.0908, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Silla', 'Punt de Partida': "L'Olleria"}), DefaultMunch(None, {'Distancia': 929.154, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Madrid', 'Punt de Partida': "L'Olleria"}), DefaultMunch(None, {'Distancia': 73.806, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Torrent', 'Punt de Partida': "L'Olleria"}), DefaultMunch(None, {'Distancia': 82.341, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': "L'Olleria"}), DefaultMunch(None, {'Distancia': 56.0381, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': "L'Olleria"}), DefaultMunch(None, {'Distancia': 69.98110000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Benetusser', 'Punt de Partida': "L'Olleria"}), DefaultMunch(None, {'Distancia': 113.6443, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Elche', 'Punt de Partida': "L'Olleria"}), DefaultMunch(None, {'Distancia': 75.0552, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': "L'Olleria"}), DefaultMunch(None, {'Distancia': 75.0552, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': "L'Olleria"}), DefaultMunch(None, {'Distancia': 82.341, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': "L'Olleria"}), DefaultMunch(None, {'Distancia': 70.058, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sedaví', 'Punt de Partida': "L'Olleria"}), DefaultMunch(None, {'Distancia': 75.0552, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': "L'Olleria"}), DefaultMunch(None, {'Distancia': 75.0552, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': "L'Olleria"}), DefaultMunch(None, {'Distancia': 75.0552, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': "L'Olleria"}), DefaultMunch(None, {'Distancia': 75.0552, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': "L'Olleria"}), DefaultMunch(None, {'Distancia': 75.0552, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': "L'Olleria"}), DefaultMunch(None, {'Distancia': 56.0381, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': "L'Olleria"}), DefaultMunch(None, {'Distancia': 83.6313, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': "L'Olleria"}), DefaultMunch(None, {'Distancia': 104.5402, 'Nombre de Pràctiques': 7, 'Punt de Destí': 'Rafelbunyol', 'Punt de Partida': "L'Olleria"}), DefaultMunch(None, {'Distancia': 75.0552, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': "L'Olleria"}), DefaultMunch(None, {'Distancia': 56.0381, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Almussafes', 'Punt de Partida': "L'Olleria"}), DefaultMunch(None, {'Distancia': 41.5949, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Guadassuar', 'Punt de Partida': "L'Olleria"}), DefaultMunch(None, {'Distancia': 41.7994, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Gandía', 'Punt de Partida': "L'Olleria"}), DefaultMunch(None, {'Distancia': 41.7994, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Gandía', 'Punt de Partida': "L'Olleria"}), DefaultMunch(None, {'Distancia': 75.0552, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'València', 'Punt de Partida': "L'Olleria"}), DefaultMunch(None, {'Distancia': 75.0552, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': "L'Olleria"}), DefaultMunch(None, {'Distancia': 73.806, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Torrent', 'Punt de Partida': "L'Olleria"}), DefaultMunch(None, {'Distancia': 75.0552, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': "L'Olleria"}), DefaultMunch(None, {'Distancia': 75.0552, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': "L'Olleria"}), DefaultMunch(None, {'Distancia': 75.0552, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': "L'Olleria"}), DefaultMunch(None, {'Distancia': 75.0552, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': "L'Olleria"}), DefaultMunch(None, {'Distancia': 82.341, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': "L'Olleria"}), DefaultMunch(None, {'Distancia': 64.0076, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': "L'Olleria"}), DefaultMunch(None, {'Distancia': 75.0552, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': "L'Olleria"}), DefaultMunch(None, {'Distancia': 444.5496, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Montcada i Reixac', 'Punt de Partida': "L'Olleria"}), DefaultMunch(None, {'Distancia': 82.341, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': "L'Olleria"}), DefaultMunch(None, {'Distancia': 929.154, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Madrid', 'Punt de Partida': "L'Olleria"})]</t>
+        </is>
+      </c>
+      <c r="L38" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Alumne': 'alumno37', 'Pràctica': 'ESORIANO(Pràctica 1)'})</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="n">
+        <v>37</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>alumno38</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>ASIR</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>Albal</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>Si</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Auditor': '2', 'BD': '7', 'Ciberseguridad': '5', 'Consultor': '3', 'Hardware': '1', 'HelpDesk': '9', 'Monitorizador': '4', 'Redes': '1', 'Sistemas': '3'})</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr"/>
+      <c r="H39" t="inlineStr"/>
+      <c r="I39" t="inlineStr"/>
+      <c r="J39" t="inlineStr"/>
+      <c r="K39" t="inlineStr">
+        <is>
+          <t>[DefaultMunch(None, {'Distancia': 5.904, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 6, 'Punt de Destí': 'Valencia', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 31.4555, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Fortaleny', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 3.7565, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Massanassa', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 5.904, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Valencia', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 16.428099999999997, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Albal', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 36.9901, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 2.3773, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 13.7403, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 2.3773, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 5.59, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 16.428099999999997, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 6.3576999999999995, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paiporta', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 2.3773, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 36.9901, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 13.7403, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 28.3518, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Algemesí', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 5.59, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 16.428099999999997, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 2.3773, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 374.0283, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Pozuelo de Alarcón', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 16.428099999999997, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 54.4804, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Xàtiva', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 9.9833, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 9.9833, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 36.2194, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Benisanó', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 28.5998, 'Nombre de Pràctiques': 1, 'Punt de Destí': "L'Alcúdia", 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 12.8855, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Mislata', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 8.44, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 2.3773, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 16.428099999999997, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 16.428099999999997, 'Nombre de Pràctiques': 5, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 8, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 4, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 9.9833, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 30.2138, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sueca', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 5.59, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 16.4677, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 16.428099999999997, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 20.3187, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Foios', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.7685, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Alaquas', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 11, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 5.59, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 5, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 28.6172, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Riba Roja', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 16.428099999999997, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 5.904, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 972.572, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 8.44, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 16.428099999999997, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 15.8304, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 4.996, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Benetusser', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 166.1651, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Elche', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 16.428099999999997, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 7.253100000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sedaví', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 15.8304, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 16.4677, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 30.1327, 'Nombre de Pràctiques': 7, 'Punt de Destí': 'Rafelbunyol', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 15.8304, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 29.7454, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Guadassuar', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 61.969199999999994, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Gandía', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 61.969199999999994, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Gandía', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 8.44, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 16.428099999999997, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 9.9833, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 371.3051, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Montcada i Reixac', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 16.428099999999997, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 972.572, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'Albal'})]</t>
+        </is>
+      </c>
+      <c r="L39" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Alumne': 'alumno38', 'Pràctica': 'Electrodomesticos Llacer(Pràctica 1)'})</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>alumno39</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>ASIR</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>Valencia</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>Si</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Auditor': '1', 'BD': '2', 'Ciberseguridad': '1', 'Consultor': '2', 'Hardware': '1', 'HelpDesk': '1', 'Monitorizador': '1', 'Redes': '2', 'Sistemas': '2'})</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr"/>
+      <c r="H40" t="inlineStr"/>
+      <c r="I40" t="inlineStr"/>
+      <c r="J40" t="inlineStr"/>
+      <c r="K40" t="inlineStr">
+        <is>
+          <t>[DefaultMunch(None, {'Distancia': 13.6585, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 6, 'Punt de Destí': 'Valencia', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 39.21, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Fortaleny', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 8.8391, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Massanassa', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 13.6585, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Valencia', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 11.0844, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Albal', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 28.0815, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.7637, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 8.0286, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.7637, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.937600000000001, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 8.2699, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paiporta', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.7637, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 28.0815, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 8.0286, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 36.1064, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Algemesí', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.937600000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.7637, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 367.69440000000003, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Pozuelo de Alarcón', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 62.235, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Xàtiva', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 17.7379, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 17.7379, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 27.3108, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Benisanó', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 36.3544, 'Nombre de Pràctiques': 1, 'Punt de Destí': "L'Alcúdia", 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 4.8457, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Mislata', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 10.663799999999998, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.7637, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 5, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 8, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 4, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 17.7379, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 37.9684, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sueca', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.937600000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.3887, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 10.3529, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Foios', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 10.22, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Alaquas', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 11, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.937600000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 5, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 22.5721, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Riba Roja', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 13.6585, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 966.2381, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 10.663799999999998, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 23.585, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.7878, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Benetusser', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 173.9197, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Elche', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 6.9288, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sedaví', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 23.585, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.3887, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 19.881400000000003, 'Nombre de Pràctiques': 7, 'Punt de Destí': 'Rafelbunyol', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 23.585, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 37.499900000000004, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Guadassuar', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 69.7237, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Gandía', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 69.7237, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Gandía', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 10.663799999999998, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 17.7379, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 361.05379999999997, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Montcada i Reixac', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 966.2381, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'Valencia'})]</t>
+        </is>
+      </c>
+      <c r="L40" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Alumne': 'alumno39', 'Pràctica': 'PANTALLAX, S.L.(Pràctica 1)'})</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>alumno40</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>ASIR</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>Catarroja</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>Si</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Auditor': '7', 'BD': '7', 'Ciberseguridad': '9', 'Consultor': '7', 'Hardware': '3', 'HelpDesk': '3', 'Monitorizador': '7', 'Redes': '6', 'Sistemas': '7'})</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr"/>
+      <c r="H41" t="inlineStr"/>
+      <c r="I41" t="inlineStr"/>
+      <c r="J41" t="inlineStr"/>
+      <c r="K41" t="inlineStr">
+        <is>
+          <t>[DefaultMunch(None, {'Distancia': 6.1035, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 6, 'Punt de Destí': 'Valencia', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 31.6549, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Fortaleny', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 1.2002000000000002, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Massanassa', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 6.1035, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Valencia', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 15.222700000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 2.0949, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Albal', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 35.7846, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 12.534799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 3.3274, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 15.222700000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 5.1522, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paiporta', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 35.7846, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 12.534799999999999, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 28.551299999999998, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Algemesí', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 3.3274, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 15.222700000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 372.8228, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Pozuelo de Alarcón', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 15.222700000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 54.6799, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Xàtiva', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 10.182799999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 10.182799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 35.014, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Benisanó', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 28.7993, 'Nombre de Pràctiques': 1, 'Punt de Destí': "L'Alcúdia", 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 11.6801, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Mislata', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 10.5417, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 15.222700000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 15.222700000000001, 'Nombre de Pràctiques': 5, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 8, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 4, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 10.182799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 30.4133, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sueca', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 3.3274, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 15.2623, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 15.222700000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 19.1133, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Foios', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 12.8701, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Alaquas', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 11, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 3.3274, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 5, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 27.4118, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Riba Roja', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 15.222700000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 6.1035, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 971.3665, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 10.5417, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 15.222700000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 16.0299, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 2.7334, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Benetusser', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 166.3646, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Elche', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 15.222700000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 4.2168, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sedaví', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 16.0299, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 15.2623, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 28.9272, 'Nombre de Pràctiques': 7, 'Punt de Destí': 'Rafelbunyol', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 16.0299, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 29.9449, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Guadassuar', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 62.168699999999994, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Gandía', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 62.168699999999994, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Gandía', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 10.5417, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 15.222700000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 10.182799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 370.0997, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Montcada i Reixac', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 15.222700000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 971.3665, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'Catarroja'})]</t>
+        </is>
+      </c>
+      <c r="L41" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Alumne': 'alumno40', 'Pràctica': 'Colegio San Antonio de Padua II(Pràctica 1)'})</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>alumno41</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>ASIR</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>Benifaio</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Auditor': '7', 'BD': '6', 'Ciberseguridad': '9', 'Consultor': '5', 'Hardware': '8', 'HelpDesk': '6', 'Monitorizador': '8', 'Redes': '5', 'Sistemas': '7'})</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr"/>
+      <c r="H42" t="inlineStr"/>
+      <c r="I42" t="inlineStr"/>
+      <c r="J42" t="inlineStr"/>
+      <c r="K42" t="inlineStr">
+        <is>
+          <t>[DefaultMunch(None, {'Distancia': 12.6061, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Benifaio'}), DefaultMunch(None, {'Distancia': 25.5705, 'Nombre de Pràctiques': 6, 'Punt de Destí': 'Valencia', 'Punt de Partida': 'Benifaio'}), DefaultMunch(None, {'Distancia': 18.1795, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Fortaleny', 'Punt de Partida': 'Benifaio'}), DefaultMunch(None, {'Distancia': 18.9632, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Massanassa', 'Punt de Partida': 'Benifaio'}), DefaultMunch(None, {'Distancia': 12.6061, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Benifaio'}), DefaultMunch(None, {'Distancia': 25.5705, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Valencia', 'Punt de Partida': 'Benifaio'}), DefaultMunch(None, {'Distancia': 32.8564, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Benifaio'}), DefaultMunch(None, {'Distancia': 18.834, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Albal', 'Punt de Partida': 'Benifaio'}), DefaultMunch(None, {'Distancia': 55.5541, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'Benifaio'}), DefaultMunch(None, {'Distancia': 18.146, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Benifaio'}), DefaultMunch(None, {'Distancia': 25.5705, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Benifaio'}), DefaultMunch(None, {'Distancia': 25.5705, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Benifaio'}), DefaultMunch(None, {'Distancia': 30.1654, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'Benifaio'}), DefaultMunch(None, {'Distancia': 18.146, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Benifaio'}), DefaultMunch(None, {'Distancia': 20.4481, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Benifaio'}), DefaultMunch(None, {'Distancia': 32.8564, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Benifaio'}), DefaultMunch(None, {'Distancia': 25.5705, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'València', 'Punt de Partida': 'Benifaio'}), DefaultMunch(None, {'Distancia': 22.915200000000002, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paiporta', 'Punt de Partida': 'Benifaio'}), DefaultMunch(None, {'Distancia': 25.5705, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Benifaio'}), DefaultMunch(None, {'Distancia': 18.146, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Benifaio'}), DefaultMunch(None, {'Distancia': 55.5541, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'Benifaio'}), DefaultMunch(None, {'Distancia': 25.5705, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Benifaio'}), DefaultMunch(None, {'Distancia': 30.1654, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'Benifaio'}), DefaultMunch(None, {'Distancia': 11.598700000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Algemesí', 'Punt de Partida': 'Benifaio'}), DefaultMunch(None, {'Distancia': 20.4481, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Benifaio'}), DefaultMunch(None, {'Distancia': 32.8564, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Benifaio'}), DefaultMunch(None, {'Distancia': 18.146, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Benifaio'}), DefaultMunch(None, {'Distancia': 378.8997, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Pozuelo de Alarcón', 'Punt de Partida': 'Benifaio'}), DefaultMunch(None, {'Distancia': 32.8564, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Benifaio'}), DefaultMunch(None, {'Distancia': 42.3677, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Xàtiva', 'Punt de Partida': 'Benifaio'}), DefaultMunch(None, {'Distancia': 14.1417, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Benifaio'}), DefaultMunch(None, {'Distancia': 25.5705, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Benifaio'}), DefaultMunch(None, {'Distancia': 14.1417, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Benifaio'}), DefaultMunch(None, {'Distancia': 25.5705, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Benifaio'}), DefaultMunch(None, {'Distancia': 54.7834, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Benisanó', 'Punt de Partida': 'Benifaio'}), DefaultMunch(None, {'Distancia': 16.487099999999998, 'Nombre de Pràctiques': 1, 'Punt de Destí': "L'Alcúdia", 'Punt de Partida': 'Benifaio'}), DefaultMunch(None, {'Distancia': 29.3107, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Mislata', 'Punt de Partida': 'Benifaio'}), DefaultMunch(None, {'Distancia': 23.954, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Benifaio'}), DefaultMunch(None, {'Distancia': 18.146, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Benifaio'}), DefaultMunch(None, {'Distancia': 32.8564, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Benifaio'}), DefaultMunch(None, {'Distancia': 32.8564, 'Nombre de Pràctiques': 5, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Benifaio'}), DefaultMunch(None, {'Distancia': 25.5705, 'Nombre de Pràctiques': 8, 'Punt de Destí': 'València', 'Punt de Partida': 'Benifaio'}), DefaultMunch(None, {'Distancia': 25.5705, 'Nombre de Pràctiques': 4, 'Punt de Destí': 'València', 'Punt de Partida': 'Benifaio'}), DefaultMunch(None, {'Distancia': 14.1417, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Benifaio'}), DefaultMunch(None, {'Distancia': 16.937900000000003, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sueca', 'Punt de Partida': 'Benifaio'}), DefaultMunch(None, {'Distancia': 20.4481, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Benifaio'}), DefaultMunch(None, {'Distancia': 34.1466, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Benifaio'}), DefaultMunch(None, {'Distancia': 32.8564, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Benifaio'}), DefaultMunch(None, {'Distancia': 35.1241, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Foios', 'Punt de Partida': 'Benifaio'}), DefaultMunch(None, {'Distancia': 26.423, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Alaquas', 'Punt de Partida': 'Benifaio'}), DefaultMunch(None, {'Distancia': 25.5705, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Benifaio'}), DefaultMunch(None, {'Distancia': 25.5705, 'Nombre de Pràctiques': 11, 'Punt de Destí': 'València', 'Punt de Partida': 'Benifaio'}), DefaultMunch(None, {'Distancia': 25.5705, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Benifaio'}), DefaultMunch(None, {'Distancia': 20.4481, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Benifaio'}), DefaultMunch(None, {'Distancia': 25.5705, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Benifaio'}), DefaultMunch(None, {'Distancia': 25.5705, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Benifaio'}), DefaultMunch(None, {'Distancia': 25.5705, 'Nombre de Pràctiques': 5, 'Punt de Destí': 'València', 'Punt de Partida': 'Benifaio'}), DefaultMunch(None, {'Distancia': 39.991, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Riba Roja', 'Punt de Partida': 'Benifaio'}), DefaultMunch(None, {'Distancia': 32.8564, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Benifaio'}), DefaultMunch(None, {'Distancia': 25.5705, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Benifaio'}), DefaultMunch(None, {'Distancia': 25.5705, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Benifaio'}), DefaultMunch(None, {'Distancia': 12.6061, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Benifaio'}), DefaultMunch(None, {'Distancia': 955.3668, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'Benifaio'}), DefaultMunch(None, {'Distancia': 23.954, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Benifaio'}), DefaultMunch(None, {'Distancia': 32.8564, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Benifaio'}), DefaultMunch(None, {'Distancia': 2.0896, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Benifaio'}), DefaultMunch(None, {'Distancia': 20.4964, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Benetusser', 'Punt de Partida': 'Benifaio'}), DefaultMunch(None, {'Distancia': 154.0524, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Elche', 'Punt de Partida': 'Benifaio'}), DefaultMunch(None, {'Distancia': 25.5705, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Benifaio'}), DefaultMunch(None, {'Distancia': 25.5705, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Benifaio'}), DefaultMunch(None, {'Distancia': 32.8564, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Benifaio'}), DefaultMunch(None, {'Distancia': 20.5733, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sedaví', 'Punt de Partida': 'Benifaio'}), DefaultMunch(None, {'Distancia': 25.5705, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Benifaio'}), DefaultMunch(None, {'Distancia': 25.5705, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Benifaio'}), DefaultMunch(None, {'Distancia': 25.5705, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Benifaio'}), DefaultMunch(None, {'Distancia': 25.5705, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Benifaio'}), DefaultMunch(None, {'Distancia': 25.5705, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Benifaio'}), DefaultMunch(None, {'Distancia': 2.0896, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Benifaio'}), DefaultMunch(None, {'Distancia': 34.1466, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Benifaio'}), DefaultMunch(None, {'Distancia': 54.688199999999995, 'Nombre de Pràctiques': 7, 'Punt de Destí': 'Rafelbunyol', 'Punt de Partida': 'Benifaio'}), DefaultMunch(None, {'Distancia': 25.5705, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Benifaio'}), DefaultMunch(None, {'Distancia': 2.0896, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Benifaio'}), DefaultMunch(None, {'Distancia': 16.2088, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Guadassuar', 'Punt de Partida': 'Benifaio'}), DefaultMunch(None, {'Distancia': 47.154, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Gandía', 'Punt de Partida': 'Benifaio'}), DefaultMunch(None, {'Distancia': 47.154, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Gandía', 'Punt de Partida': 'Benifaio'}), DefaultMunch(None, {'Distancia': 25.5705, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'València', 'Punt de Partida': 'Benifaio'}), DefaultMunch(None, {'Distancia': 25.5705, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Benifaio'}), DefaultMunch(None, {'Distancia': 23.954, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Benifaio'}), DefaultMunch(None, {'Distancia': 25.5705, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Benifaio'}), DefaultMunch(None, {'Distancia': 25.5705, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Benifaio'}), DefaultMunch(None, {'Distancia': 25.5705, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Benifaio'}), DefaultMunch(None, {'Distancia': 25.5705, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Benifaio'}), DefaultMunch(None, {'Distancia': 32.8564, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Benifaio'}), DefaultMunch(None, {'Distancia': 14.1417, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Benifaio'}), DefaultMunch(None, {'Distancia': 25.5705, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Benifaio'}), DefaultMunch(None, {'Distancia': 394.69759999999997, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Montcada i Reixac', 'Punt de Partida': 'Benifaio'}), DefaultMunch(None, {'Distancia': 32.8564, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Benifaio'}), DefaultMunch(None, {'Distancia': 955.3668, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'Benifaio'})]</t>
+        </is>
+      </c>
+      <c r="L42" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Alumne': 'alumno41', 'Pràctica': 'Val Automoción(Pràctica 2)'})</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="n">
+        <v>41</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>alumno42</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>ASIR</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>Albal</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>Si</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Auditor': '2', 'BD': '6', 'Ciberseguridad': '4', 'Consultor': '6', 'Hardware': '4', 'HelpDesk': '6', 'Monitorizador': '5', 'Redes': '4', 'Sistemas': '5'})</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr"/>
+      <c r="H43" t="inlineStr"/>
+      <c r="I43" t="inlineStr"/>
+      <c r="J43" t="inlineStr"/>
+      <c r="K43" t="inlineStr">
+        <is>
+          <t>[DefaultMunch(None, {'Distancia': 5.904, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 6, 'Punt de Destí': 'Valencia', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 31.4555, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Fortaleny', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 3.7565, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Massanassa', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 5.904, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Valencia', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 16.428099999999997, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Albal', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 36.9901, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 2.3773, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 13.7403, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 2.3773, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 5.59, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 16.428099999999997, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 6.3576999999999995, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paiporta', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 2.3773, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 36.9901, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 13.7403, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 28.3518, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Algemesí', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 5.59, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 16.428099999999997, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 2.3773, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 374.0283, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Pozuelo de Alarcón', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 16.428099999999997, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 54.4804, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Xàtiva', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 9.9833, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 9.9833, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 36.2194, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Benisanó', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 28.5998, 'Nombre de Pràctiques': 1, 'Punt de Destí': "L'Alcúdia", 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 12.8855, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Mislata', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 8.44, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 2.3773, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 16.428099999999997, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 16.428099999999997, 'Nombre de Pràctiques': 5, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 8, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 4, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 9.9833, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 30.2138, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sueca', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 5.59, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 16.4677, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 16.428099999999997, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 20.3187, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Foios', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.7685, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Alaquas', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 11, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 5.59, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 5, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 28.6172, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Riba Roja', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 16.428099999999997, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 5.904, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 972.572, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 8.44, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 16.428099999999997, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 15.8304, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 4.996, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Benetusser', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 166.1651, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Elche', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 16.428099999999997, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 7.253100000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sedaví', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 15.8304, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 16.4677, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 30.1327, 'Nombre de Pràctiques': 7, 'Punt de Destí': 'Rafelbunyol', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 15.8304, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 29.7454, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Guadassuar', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 61.969199999999994, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Gandía', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 61.969199999999994, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Gandía', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 8.44, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 16.428099999999997, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 9.9833, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 371.3051, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Montcada i Reixac', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 16.428099999999997, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 972.572, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'Albal'})]</t>
+        </is>
+      </c>
+      <c r="L43" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Alumne': 'alumno42', 'Pràctica': 'Media'})</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>alumno43</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>ASIR</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>Alginet</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Auditor': '10', 'BD': '8', 'Ciberseguridad': '9', 'Consultor': '3', 'Hardware': '5', 'HelpDesk': '6', 'Monitorizador': '7', 'Redes': '5', 'Sistemas': '5'})</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr"/>
+      <c r="H44" t="inlineStr"/>
+      <c r="I44" t="inlineStr"/>
+      <c r="J44" t="inlineStr"/>
+      <c r="K44" t="inlineStr">
+        <is>
+          <t>[DefaultMunch(None, {'Distancia': 13.950899999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 6, 'Punt de Destí': 'Valencia', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 23.9937, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Fortaleny', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 20.3081, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Massanassa', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 13.950899999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Valencia', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 34.2012, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 20.178900000000002, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Albal', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 57.2663, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 19.4909, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 31.5103, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 19.4909, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 21.792900000000003, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 34.2012, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 24.260099999999998, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paiporta', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 19.4909, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 57.2663, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 31.5103, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 10.4673, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Algemesí', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 21.792900000000003, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 34.2012, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 19.4909, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 380.61190000000005, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Pozuelo de Alarcón', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 34.2012, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 35.7939, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Xàtiva', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 15.867700000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 15.867700000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 56.495599999999996, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Benisanó', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 9.9133, 'Nombre de Pràctiques': 1, 'Punt de Destí': "L'Alcúdia", 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 30.6556, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Mislata', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 25.6662, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 19.4909, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 34.2012, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 34.2012, 'Nombre de Pràctiques': 5, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 8, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 4, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 15.867700000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 21.3029, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sueca', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 21.792900000000003, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 35.4914, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 34.2012, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 36.468900000000005, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Foios', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 28.135099999999998, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Alaquas', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 11, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 21.792900000000003, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 5, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 41.703199999999995, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Riba Roja', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 34.2012, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 13.950899999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 948.793, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 25.6662, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 34.2012, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 7.9038, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 21.8412, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Benetusser', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 147.4786, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Elche', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 34.2012, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 21.9181, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sedaví', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 7.9038, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 35.4914, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 56.400400000000005, 'Nombre de Pràctiques': 7, 'Punt de Destí': 'Rafelbunyol', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 7.9038, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 11.0588, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Guadassuar', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 48.4726, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Gandía', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 48.4726, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Gandía', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 25.6662, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 34.2012, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 15.867700000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 396.40979999999996, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Montcada i Reixac', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 34.2012, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 948.793, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'Alginet'})]</t>
+        </is>
+      </c>
+      <c r="L44" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Alumne': 'alumno43', 'Pràctica': 'Atmosfera Sport(Pràctica 1)'})</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="n">
+        <v>43</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>alumno44</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>ASIR</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>Valencia</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Auditor': '7', 'BD': '2', 'Ciberseguridad': '5', 'Consultor': '5', 'Hardware': '10', 'HelpDesk': '2', 'Monitorizador': '8', 'Redes': '7', 'Sistemas': '2'})</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr"/>
+      <c r="H45" t="inlineStr"/>
+      <c r="I45" t="inlineStr"/>
+      <c r="J45" t="inlineStr"/>
+      <c r="K45" t="inlineStr">
+        <is>
+          <t>[DefaultMunch(None, {'Distancia': 13.6585, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 6, 'Punt de Destí': 'Valencia', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 39.21, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Fortaleny', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 8.8391, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Massanassa', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 13.6585, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Valencia', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 11.0844, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Albal', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 28.0815, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.7637, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 8.0286, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.7637, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.937600000000001, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 8.2699, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paiporta', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.7637, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 28.0815, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 8.0286, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 36.1064, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Algemesí', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.937600000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.7637, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 367.69440000000003, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Pozuelo de Alarcón', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 62.235, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Xàtiva', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 17.7379, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 17.7379, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 27.3108, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Benisanó', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 36.3544, 'Nombre de Pràctiques': 1, 'Punt de Destí': "L'Alcúdia", 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 4.8457, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Mislata', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 10.663799999999998, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.7637, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 5, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 8, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 4, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 17.7379, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 37.9684, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sueca', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.937600000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.3887, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 10.3529, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Foios', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 10.22, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Alaquas', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 11, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.937600000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 5, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 22.5721, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Riba Roja', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 13.6585, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 966.2381, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 10.663799999999998, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 23.585, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.7878, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Benetusser', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 173.9197, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Elche', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 6.9288, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sedaví', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 23.585, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.3887, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 19.881400000000003, 'Nombre de Pràctiques': 7, 'Punt de Destí': 'Rafelbunyol', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 23.585, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 37.499900000000004, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Guadassuar', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 69.7237, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Gandía', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 69.7237, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Gandía', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 10.663799999999998, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 17.7379, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 361.05379999999997, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Montcada i Reixac', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 966.2381, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'Valencia'})]</t>
+        </is>
+      </c>
+      <c r="L45" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Alumne': 'alumno44', 'Pràctica': 'FRACTALYS, S.L.(Pràctica 1)'})</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="n">
+        <v>44</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>alumno45</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>ASIR</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>Valencia</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>Si</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Auditor': '10', 'BD': '6', 'Ciberseguridad': '3', 'Consultor': '10', 'Hardware': '9', 'HelpDesk': '3', 'Monitorizador': '8', 'Redes': '4', 'Sistemas': '2'})</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr"/>
+      <c r="H46" t="inlineStr"/>
+      <c r="I46" t="inlineStr"/>
+      <c r="J46" t="inlineStr"/>
+      <c r="K46" t="inlineStr">
+        <is>
+          <t>[DefaultMunch(None, {'Distancia': 13.6585, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 6, 'Punt de Destí': 'Valencia', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 39.21, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Fortaleny', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 8.8391, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Massanassa', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 13.6585, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Valencia', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 11.0844, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Albal', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 28.0815, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.7637, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 8.0286, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.7637, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.937600000000001, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 8.2699, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paiporta', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.7637, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 28.0815, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 8.0286, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 36.1064, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Algemesí', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.937600000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.7637, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 367.69440000000003, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Pozuelo de Alarcón', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 62.235, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Xàtiva', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 17.7379, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 17.7379, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 27.3108, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Benisanó', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 36.3544, 'Nombre de Pràctiques': 1, 'Punt de Destí': "L'Alcúdia", 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 4.8457, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Mislata', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 10.663799999999998, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.7637, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 5, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 8, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 4, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 17.7379, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 37.9684, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sueca', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.937600000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.3887, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 10.3529, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Foios', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 10.22, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Alaquas', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 11, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.937600000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 5, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 22.5721, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Riba Roja', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 13.6585, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 966.2381, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 10.663799999999998, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 23.585, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.7878, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Benetusser', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 173.9197, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Elche', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 6.9288, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sedaví', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 23.585, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.3887, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 19.881400000000003, 'Nombre de Pràctiques': 7, 'Punt de Destí': 'Rafelbunyol', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 23.585, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 37.499900000000004, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Guadassuar', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 69.7237, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Gandía', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 69.7237, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Gandía', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 10.663799999999998, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 17.7379, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 361.05379999999997, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Montcada i Reixac', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 966.2381, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'Valencia'})]</t>
+        </is>
+      </c>
+      <c r="L46" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Alumne': 'alumno45', 'Pràctica': 'CAPGEMINI(Pràctica 2)'})</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>alumno46</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>TSMR</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>Valencia</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>SÃ­</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Asesor': '5', 'HelpDesk': '2', 'Instalador': '2', 'Tecnico': '2'})</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr"/>
+      <c r="H47" t="inlineStr"/>
+      <c r="I47" t="inlineStr"/>
+      <c r="J47" t="inlineStr"/>
+      <c r="K47" t="inlineStr">
+        <is>
+          <t>[DefaultMunch(None, {'Distancia': 13.6585, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 6, 'Punt de Destí': 'Valencia', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 39.21, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Fortaleny', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 8.8391, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Massanassa', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 13.6585, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Valencia', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 11.0844, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Albal', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 28.0815, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.7637, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 8.0286, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.7637, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.937600000000001, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 8.2699, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paiporta', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.7637, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 28.0815, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 8.0286, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 36.1064, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Algemesí', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.937600000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.7637, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 367.69440000000003, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Pozuelo de Alarcón', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 62.235, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Xàtiva', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 17.7379, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 17.7379, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 27.3108, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Benisanó', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 36.3544, 'Nombre de Pràctiques': 1, 'Punt de Destí': "L'Alcúdia", 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 4.8457, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Mislata', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 10.663799999999998, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.7637, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 5, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 8, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 4, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 17.7379, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 37.9684, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sueca', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.937600000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.3887, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 10.3529, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Foios', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 10.22, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Alaquas', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 11, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.937600000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 5, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 22.5721, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Riba Roja', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 13.6585, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 966.2381, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 10.663799999999998, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 23.585, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.7878, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Benetusser', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 173.9197, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Elche', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 6.9288, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sedaví', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 23.585, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.3887, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 19.881400000000003, 'Nombre de Pràctiques': 7, 'Punt de Destí': 'Rafelbunyol', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 23.585, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 37.499900000000004, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Guadassuar', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 69.7237, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Gandía', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 69.7237, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Gandía', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 10.663799999999998, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 17.7379, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 361.05379999999997, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Montcada i Reixac', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 966.2381, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'Valencia'})]</t>
+        </is>
+      </c>
+      <c r="L47" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Alumne': 'alumno46', 'Pràctica': 'Uned(Pràctica 1)'})</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="1" t="n">
+        <v>46</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>alumno47</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>TSMR</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>Paiporta</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>SÃ­</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Asesor': '8', 'HelpDesk': '2', 'Instalador': '6', 'Tecnico': '6'})</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr"/>
+      <c r="H48" t="inlineStr"/>
+      <c r="I48" t="inlineStr"/>
+      <c r="J48" t="inlineStr"/>
+      <c r="K48" t="inlineStr">
+        <is>
+          <t>[DefaultMunch(None, {'Distancia': 10.6884, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 6, 'Punt de Destí': 'Valencia', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 36.2399, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Fortaleny', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 4.6883, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Massanassa', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 10.6884, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Valencia', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 12.6795, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 5.5664, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Albal', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 33.2415, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 5.6128, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 9.9916, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 5.6128, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 5.3247, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 12.6795, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'València', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paiporta', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 5.6128, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 33.2415, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 9.9916, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 33.136199999999995, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Algemesí', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 5.3247, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 12.6795, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 5.6128, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 370.2797, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Pozuelo de Alarcón', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 12.6795, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 59.2648, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Xàtiva', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 14.767700000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 14.767700000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 32.4708, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Benisanó', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 33.3842, 'Nombre de Pràctiques': 1, 'Punt de Destí': "L'Alcúdia", 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 9.136899999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Mislata', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 5.484100000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 5.6128, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 12.6795, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 12.6795, 'Nombre de Pràctiques': 5, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 8, 'Punt de Destí': 'València', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 4, 'Punt de Destí': 'València', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 14.767700000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 34.9983, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sueca', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 5.3247, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 12.3171, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 12.6795, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 17.250400000000003, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Foios', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 6.9689, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Alaquas', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 11, 'Punt de Destí': 'València', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 5.3247, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 5, 'Punt de Destí': 'València', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 24.8687, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Riba Roja', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 12.6795, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 10.6884, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 968.8234, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 5.484100000000001, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 12.6795, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 20.614900000000002, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 4.3557, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Benetusser', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 170.9496, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Elche', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 12.6795, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 4.7298, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sedaví', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 20.614900000000002, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 12.3171, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 27.6094, 'Nombre de Pràctiques': 7, 'Punt de Destí': 'Rafelbunyol', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 20.614900000000002, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 34.5298, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Guadassuar', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 66.7536, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Gandía', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 66.7536, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Gandía', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'València', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 5.484100000000001, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 12.6795, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 14.767700000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 7.974600000000001, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 374.057, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Montcada i Reixac', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 12.6795, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Paiporta'}), DefaultMunch(None, {'Distancia': 968.8234, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'Paiporta'})]</t>
+        </is>
+      </c>
+      <c r="L48" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Alumne': 'alumno47', 'Pràctica': 'pcmatica torrent(Pràctica 2)'})</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>alumno48</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>TSMR</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>Sollana</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>SÃ­</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Asesor': '1', 'HelpDesk': '6', 'Instalador': '5', 'Tecnico': '3'})</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr"/>
+      <c r="H49" t="inlineStr"/>
+      <c r="I49" t="inlineStr"/>
+      <c r="J49" t="inlineStr"/>
+      <c r="K49" t="inlineStr">
+        <is>
+          <t>[DefaultMunch(None, {'Distancia': 15.9393, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 28.9037, 'Nombre de Pràctiques': 6, 'Punt de Destí': 'Valencia', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 13.506, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Fortaleny', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 22.2965, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Massanassa', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 15.9393, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 28.9037, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Valencia', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 36.1896, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 22.1673, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Albal', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 59.2326, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 21.4793, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 28.9037, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 28.9037, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 33.4987, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 21.4793, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 23.781299999999998, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 36.1896, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 28.9037, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'València', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 26.2484, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paiporta', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 28.9037, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 21.4793, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 59.2326, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 28.9037, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 33.4987, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 15.0618, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Algemesí', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 23.781299999999998, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 36.1896, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 21.4793, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 382.57820000000004, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Pozuelo de Alarcón', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 36.1896, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 46.8598, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Xàtiva', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 17.8201, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 28.9037, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 17.8201, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 28.9037, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 58.4619, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Benisanó', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 20.979200000000002, 'Nombre de Pràctiques': 1, 'Punt de Destí': "L'Alcúdia", 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 32.6439, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Mislata', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 27.6325, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 21.4793, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 36.1896, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 36.1896, 'Nombre de Pràctiques': 5, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 28.9037, 'Nombre de Pràctiques': 8, 'Punt de Destí': 'València', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 28.9037, 'Nombre de Pràctiques': 4, 'Punt de Destí': 'València', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 17.8201, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 12.2644, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sueca', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 23.781299999999998, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 37.479800000000004, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 36.1896, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 38.457300000000004, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Foios', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 30.1014, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Alaquas', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 28.9037, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 28.9037, 'Nombre de Pràctiques': 11, 'Punt de Destí': 'València', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 28.9037, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 23.781299999999998, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 28.9037, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 28.9037, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 28.9037, 'Nombre de Pràctiques': 5, 'Punt de Destí': 'València', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 43.6695, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Riba Roja', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 36.1896, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 28.9037, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 28.9037, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 15.9393, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 981.1219, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 27.6325, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 36.1896, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 5.4293000000000005, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 23.8296, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Benetusser', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 158.5445, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Elche', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 28.9037, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 28.9037, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 36.1896, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 23.9065, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sedaví', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 28.9037, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 28.9037, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 28.9037, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 28.9037, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 28.9037, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 5.4293000000000005, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 37.479800000000004, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 58.366699999999994, 'Nombre de Pràctiques': 7, 'Punt de Destí': 'Rafelbunyol', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 28.9037, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 5.4293000000000005, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 19.6719, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Guadassuar', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 42.441199999999995, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Gandía', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 42.441199999999995, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Gandía', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 28.9037, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'València', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 28.9037, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 27.6325, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 28.9037, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 28.9037, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 28.9037, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 28.9037, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 36.1896, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 17.8201, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 28.9037, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 398.37609999999995, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Montcada i Reixac', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 36.1896, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Sollana'}), DefaultMunch(None, {'Distancia': 981.1219, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'Sollana'})]</t>
+        </is>
+      </c>
+      <c r="L49" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Alumne': 'alumno48', 'Pràctica': 'Val Automoción(Pràctica 1)'})</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="1" t="n">
+        <v>48</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>alumno49</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>TSMR</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>Alginet</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Asesor': '4', 'HelpDesk': '5', 'Instalador': '8', 'Tecnico': '5'})</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr"/>
+      <c r="H50" t="inlineStr"/>
+      <c r="I50" t="inlineStr"/>
+      <c r="J50" t="inlineStr"/>
+      <c r="K50" t="inlineStr">
+        <is>
+          <t>[DefaultMunch(None, {'Distancia': 13.950899999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 6, 'Punt de Destí': 'Valencia', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 23.9937, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Fortaleny', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 20.3081, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Massanassa', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 13.950899999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Valencia', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 34.2012, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 20.178900000000002, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Albal', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 57.2663, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 19.4909, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 31.5103, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 19.4909, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 21.792900000000003, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 34.2012, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 24.260099999999998, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paiporta', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 19.4909, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 57.2663, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 31.5103, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 10.4673, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Algemesí', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 21.792900000000003, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 34.2012, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 19.4909, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 380.61190000000005, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Pozuelo de Alarcón', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 34.2012, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 35.7939, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Xàtiva', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 15.867700000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 15.867700000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 56.495599999999996, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Benisanó', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 9.9133, 'Nombre de Pràctiques': 1, 'Punt de Destí': "L'Alcúdia", 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 30.6556, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Mislata', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 25.6662, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 19.4909, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 34.2012, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 34.2012, 'Nombre de Pràctiques': 5, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 8, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 4, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 15.867700000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 21.3029, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sueca', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 21.792900000000003, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 35.4914, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 34.2012, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 36.468900000000005, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Foios', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 28.135099999999998, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Alaquas', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 11, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 21.792900000000003, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 5, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 41.703199999999995, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Riba Roja', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 34.2012, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 13.950899999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 948.793, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 25.6662, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 34.2012, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 7.9038, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 21.8412, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Benetusser', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 147.4786, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Elche', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 34.2012, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 21.9181, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sedaví', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 7.9038, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 35.4914, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 56.400400000000005, 'Nombre de Pràctiques': 7, 'Punt de Destí': 'Rafelbunyol', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 7.9038, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 11.0588, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Guadassuar', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 48.4726, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Gandía', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 48.4726, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Gandía', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 25.6662, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 34.2012, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 15.867700000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 396.40979999999996, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Montcada i Reixac', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 34.2012, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 948.793, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'Alginet'})]</t>
+        </is>
+      </c>
+      <c r="L50" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Alumne': 'alumno49', 'Pràctica': 'INFASE MACHINES, S.L.(Pràctica 1)'})</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="1" t="n">
+        <v>49</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>alumno50</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>TSMR</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>Silla</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>SÃ­</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Asesor': '6', 'HelpDesk': '1', 'Instalador': '3', 'Tecnico': '2'})</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr"/>
+      <c r="H51" t="inlineStr"/>
+      <c r="I51" t="inlineStr"/>
+      <c r="J51" t="inlineStr"/>
+      <c r="K51" t="inlineStr">
+        <is>
+          <t>[DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 6, 'Punt de Destí': 'Valencia', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 27.0358, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Fortaleny', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 7.373, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Massanassa', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Valencia', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 21.266099999999998, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 6.5287, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Albal', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 41.8281, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 5.8407, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 18.575200000000002, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 5.8407, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 8.857899999999999, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 21.266099999999998, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 9.7786, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paiporta', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 5.8407, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 41.8281, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 18.575200000000002, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 23.9322, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Algemesí', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 8.857899999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 21.266099999999998, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 5.8407, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 371.7647, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Pozuelo de Alarcón', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 21.266099999999998, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 50.0608, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Xàtiva', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 5.144399999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 5.144399999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 41.0574, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Benisanó', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 24.1802, 'Nombre de Pràctiques': 1, 'Punt de Destí': "L'Alcúdia", 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 17.7205, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Mislata', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.2774, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 5.8407, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 21.266099999999998, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 21.266099999999998, 'Nombre de Pràctiques': 5, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 8, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 4, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 5.144399999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 25.7942, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sueca', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 8.857899999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 22.5564, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 21.266099999999998, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 23.533900000000003, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Foios', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 15.6059, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Alaquas', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 11, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 8.857899999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 5, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 32.856, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Riba Roja', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 21.266099999999998, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 970.3084, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.2774, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 21.266099999999998, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 11.4108, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 8.9062, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Benetusser', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 161.7455, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Elche', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 21.266099999999998, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 8.9831, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sedaví', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 11.4108, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 22.5564, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 32.553, 'Nombre de Pràctiques': 7, 'Punt de Destí': 'Rafelbunyol', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 11.4108, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 25.3257, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Guadassuar', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 57.5496, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Gandía', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 57.5496, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Gandía', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.2774, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 21.266099999999998, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 5.144399999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 373.7255, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Montcada i Reixac', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 21.266099999999998, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 970.3084, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'Silla'})]</t>
+        </is>
+      </c>
+      <c r="L51" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Alumne': 'alumno50', 'Pràctica': 'AEOL(Pràctica 1)'})</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>alumno51</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>TSMR</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>Silla</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Asesor': '1', 'HelpDesk': '8', 'Instalador': '4', 'Tecnico': '1'})</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr"/>
+      <c r="H52" t="inlineStr"/>
+      <c r="I52" t="inlineStr"/>
+      <c r="J52" t="inlineStr"/>
+      <c r="K52" t="inlineStr">
+        <is>
+          <t>[DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 6, 'Punt de Destí': 'Valencia', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 27.0358, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Fortaleny', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 7.373, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Massanassa', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Valencia', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 21.266099999999998, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 6.5287, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Albal', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 41.8281, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 5.8407, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 18.575200000000002, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 5.8407, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 8.857899999999999, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 21.266099999999998, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 9.7786, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paiporta', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 5.8407, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 41.8281, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 18.575200000000002, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 23.9322, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Algemesí', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 8.857899999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 21.266099999999998, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 5.8407, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 371.7647, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Pozuelo de Alarcón', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 21.266099999999998, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 50.0608, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Xàtiva', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 5.144399999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 5.144399999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 41.0574, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Benisanó', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 24.1802, 'Nombre de Pràctiques': 1, 'Punt de Destí': "L'Alcúdia", 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 17.7205, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Mislata', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.2774, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 5.8407, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 21.266099999999998, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 21.266099999999998, 'Nombre de Pràctiques': 5, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 8, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 4, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 5.144399999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 25.7942, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sueca', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 8.857899999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 22.5564, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 21.266099999999998, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 23.533900000000003, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Foios', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 15.6059, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Alaquas', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 11, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 8.857899999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 5, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 32.856, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Riba Roja', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 21.266099999999998, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 970.3084, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.2774, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 21.266099999999998, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 11.4108, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 8.9062, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Benetusser', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 161.7455, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Elche', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 21.266099999999998, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 8.9831, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sedaví', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 11.4108, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 22.5564, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 32.553, 'Nombre de Pràctiques': 7, 'Punt de Destí': 'Rafelbunyol', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 11.4108, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 25.3257, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Guadassuar', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 57.5496, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Gandía', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 57.5496, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Gandía', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.2774, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 21.266099999999998, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 5.144399999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 13.9803, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 373.7255, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Montcada i Reixac', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 21.266099999999998, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Silla'}), DefaultMunch(None, {'Distancia': 970.3084, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'Silla'})]</t>
+        </is>
+      </c>
+      <c r="L52" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Alumne': 'alumno51', 'Pràctica': 'AEOL(Pràctica 2)'})</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="1" t="n">
+        <v>51</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>alumno52</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>TSMR</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>Valencia</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>SÃ­</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Asesor': '6', 'HelpDesk': '3', 'Instalador': '3', 'Tecnico': '7'})</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr"/>
+      <c r="H53" t="inlineStr"/>
+      <c r="I53" t="inlineStr"/>
+      <c r="J53" t="inlineStr"/>
+      <c r="K53" t="inlineStr">
+        <is>
+          <t>[DefaultMunch(None, {'Distancia': 13.6585, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 6, 'Punt de Destí': 'Valencia', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 39.21, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Fortaleny', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 8.8391, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Massanassa', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 13.6585, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Valencia', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 11.0844, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Albal', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 28.0815, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.7637, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 8.0286, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.7637, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.937600000000001, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 8.2699, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paiporta', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.7637, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 28.0815, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 8.0286, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 36.1064, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Algemesí', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.937600000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.7637, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 367.69440000000003, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Pozuelo de Alarcón', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 62.235, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Xàtiva', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 17.7379, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 17.7379, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 27.3108, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Benisanó', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 36.3544, 'Nombre de Pràctiques': 1, 'Punt de Destí': "L'Alcúdia", 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 4.8457, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Mislata', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 10.663799999999998, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.7637, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 5, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 8, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 4, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 17.7379, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 37.9684, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sueca', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.937600000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.3887, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 10.3529, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Foios', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 10.22, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Alaquas', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 11, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.937600000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 5, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 22.5721, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Riba Roja', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 13.6585, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 966.2381, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 10.663799999999998, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 23.585, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.7878, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Benetusser', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 173.9197, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Elche', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 6.9288, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sedaví', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 23.585, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.3887, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 19.881400000000003, 'Nombre de Pràctiques': 7, 'Punt de Destí': 'Rafelbunyol', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 23.585, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 37.499900000000004, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Guadassuar', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 69.7237, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Gandía', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 69.7237, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Gandía', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 10.663799999999998, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 17.7379, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 361.05379999999997, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Montcada i Reixac', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 966.2381, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'Valencia'})]</t>
+        </is>
+      </c>
+      <c r="L53" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Alumne': 'alumno52', 'Pràctica': 'Laberit (proyecto academy)(Pràctica 3)'})</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="1" t="n">
+        <v>52</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>alumno53</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>TSMR</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>Valencia</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>SÃ­</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Asesor': '7', 'HelpDesk': '4', 'Instalador': '7', 'Tecnico': '8'})</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr"/>
+      <c r="H54" t="inlineStr"/>
+      <c r="I54" t="inlineStr"/>
+      <c r="J54" t="inlineStr"/>
+      <c r="K54" t="inlineStr">
+        <is>
+          <t>[DefaultMunch(None, {'Distancia': 13.6585, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 6, 'Punt de Destí': 'Valencia', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 39.21, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Fortaleny', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 8.8391, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Massanassa', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 13.6585, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Valencia', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 11.0844, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Albal', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 28.0815, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.7637, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 8.0286, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.7637, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.937600000000001, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 8.2699, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paiporta', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.7637, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 28.0815, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 8.0286, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 36.1064, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Algemesí', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.937600000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.7637, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 367.69440000000003, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Pozuelo de Alarcón', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 62.235, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Xàtiva', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 17.7379, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 17.7379, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 27.3108, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Benisanó', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 36.3544, 'Nombre de Pràctiques': 1, 'Punt de Destí': "L'Alcúdia", 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 4.8457, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Mislata', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 10.663799999999998, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.7637, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 5, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 8, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 4, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 17.7379, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 37.9684, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sueca', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.937600000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.3887, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 10.3529, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Foios', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 10.22, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Alaquas', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 11, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.937600000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 5, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 22.5721, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Riba Roja', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 13.6585, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 966.2381, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 10.663799999999998, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 23.585, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.7878, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Benetusser', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 173.9197, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Elche', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 6.9288, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sedaví', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 23.585, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.3887, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 19.881400000000003, 'Nombre de Pràctiques': 7, 'Punt de Destí': 'Rafelbunyol', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 23.585, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 37.499900000000004, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Guadassuar', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 69.7237, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Gandía', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 69.7237, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Gandía', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 10.663799999999998, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 17.7379, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 361.05379999999997, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Montcada i Reixac', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 966.2381, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'Valencia'})]</t>
+        </is>
+      </c>
+      <c r="L54" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Alumne': 'alumno53', 'Pràctica': 'Indenova(Pràctica 2)'})</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="1" t="n">
+        <v>53</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>alumno54</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>TSMR</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>Albal</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>SÃ­</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Asesor': '3', 'HelpDesk': '9', 'Instalador': '10', 'Tecnico': '5'})</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr"/>
+      <c r="H55" t="inlineStr"/>
+      <c r="I55" t="inlineStr"/>
+      <c r="J55" t="inlineStr"/>
+      <c r="K55" t="inlineStr">
+        <is>
+          <t>[DefaultMunch(None, {'Distancia': 5.904, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 6, 'Punt de Destí': 'Valencia', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 31.4555, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Fortaleny', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 3.7565, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Massanassa', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 5.904, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Valencia', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 16.428099999999997, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Albal', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 36.9901, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 2.3773, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 13.7403, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 2.3773, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 5.59, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 16.428099999999997, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 6.3576999999999995, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paiporta', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 2.3773, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 36.9901, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 13.7403, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 28.3518, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Algemesí', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 5.59, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 16.428099999999997, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 2.3773, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 374.0283, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Pozuelo de Alarcón', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 16.428099999999997, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 54.4804, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Xàtiva', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 9.9833, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 9.9833, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 36.2194, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Benisanó', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 28.5998, 'Nombre de Pràctiques': 1, 'Punt de Destí': "L'Alcúdia", 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 12.8855, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Mislata', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 8.44, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 2.3773, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 16.428099999999997, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 16.428099999999997, 'Nombre de Pràctiques': 5, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 8, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 4, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 9.9833, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 30.2138, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sueca', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 5.59, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 16.4677, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 16.428099999999997, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 20.3187, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Foios', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.7685, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Alaquas', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 11, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 5.59, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 5, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 28.6172, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Riba Roja', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 16.428099999999997, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 5.904, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 972.572, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 8.44, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 16.428099999999997, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 15.8304, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 4.996, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Benetusser', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 166.1651, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Elche', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 16.428099999999997, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 7.253100000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sedaví', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 15.8304, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 16.4677, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 30.1327, 'Nombre de Pràctiques': 7, 'Punt de Destí': 'Rafelbunyol', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 15.8304, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 29.7454, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Guadassuar', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 61.969199999999994, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Gandía', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 61.969199999999994, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Gandía', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 8.44, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 16.428099999999997, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 9.9833, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 371.3051, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Montcada i Reixac', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 16.428099999999997, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 972.572, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'Albal'})]</t>
+        </is>
+      </c>
+      <c r="L55" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Alumne': 'alumno54', 'Pràctica': 'Ayto Albal(Pràctica 1)'})</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="1" t="n">
+        <v>54</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>alumno55</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>TSMR</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>Valencia</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Asesor': '8', 'HelpDesk': '6', 'Instalador': '4', 'Tecnico': '9'})</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr"/>
+      <c r="H56" t="inlineStr"/>
+      <c r="I56" t="inlineStr"/>
+      <c r="J56" t="inlineStr"/>
+      <c r="K56" t="inlineStr">
+        <is>
+          <t>[DefaultMunch(None, {'Distancia': 13.6585, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 6, 'Punt de Destí': 'Valencia', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 39.21, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Fortaleny', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 8.8391, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Massanassa', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 13.6585, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Valencia', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 11.0844, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Albal', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 28.0815, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.7637, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 8.0286, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.7637, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.937600000000001, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 8.2699, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paiporta', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.7637, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 28.0815, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 8.0286, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 36.1064, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Algemesí', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.937600000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.7637, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 367.69440000000003, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Pozuelo de Alarcón', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 62.235, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Xàtiva', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 17.7379, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 17.7379, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 27.3108, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Benisanó', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 36.3544, 'Nombre de Pràctiques': 1, 'Punt de Destí': "L'Alcúdia", 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 4.8457, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Mislata', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 10.663799999999998, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.7637, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 5, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 8, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 4, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 17.7379, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 37.9684, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sueca', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.937600000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.3887, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 10.3529, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Foios', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 10.22, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Alaquas', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 11, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.937600000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 5, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 22.5721, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Riba Roja', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 13.6585, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 966.2381, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 10.663799999999998, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 23.585, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.7878, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Benetusser', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 173.9197, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Elche', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 6.9288, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sedaví', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 23.585, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.3887, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 19.881400000000003, 'Nombre de Pràctiques': 7, 'Punt de Destí': 'Rafelbunyol', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 23.585, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 37.499900000000004, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Guadassuar', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 69.7237, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Gandía', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 69.7237, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Gandía', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 10.663799999999998, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 17.7379, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 361.05379999999997, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Montcada i Reixac', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 966.2381, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'Valencia'})]</t>
+        </is>
+      </c>
+      <c r="L56" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Alumne': 'alumno55', 'Pràctica': 'COLBA TECHNOLOGIES(Pràctica 1)'})</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="1" t="n">
+        <v>55</v>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>alumno56</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>TSMR</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>Valencia</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>SÃ­</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Asesor': '10', 'HelpDesk': '10', 'Instalador': '4', 'Tecnico': '5'})</t>
+        </is>
+      </c>
+      <c r="G57" t="inlineStr"/>
+      <c r="H57" t="inlineStr"/>
+      <c r="I57" t="inlineStr"/>
+      <c r="J57" t="inlineStr"/>
+      <c r="K57" t="inlineStr">
+        <is>
+          <t>[DefaultMunch(None, {'Distancia': 13.6585, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 6, 'Punt de Destí': 'Valencia', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 39.21, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Fortaleny', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 8.8391, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Massanassa', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 13.6585, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Valencia', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 11.0844, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Albal', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 28.0815, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.7637, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 8.0286, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.7637, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.937600000000001, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 8.2699, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paiporta', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.7637, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 28.0815, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 8.0286, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 36.1064, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Algemesí', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.937600000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.7637, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 367.69440000000003, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Pozuelo de Alarcón', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 62.235, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Xàtiva', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 17.7379, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 17.7379, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 27.3108, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Benisanó', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 36.3544, 'Nombre de Pràctiques': 1, 'Punt de Destí': "L'Alcúdia", 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 4.8457, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Mislata', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 10.663799999999998, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.7637, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 5, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 8, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 4, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 17.7379, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 37.9684, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sueca', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.937600000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.3887, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 10.3529, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Foios', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 10.22, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Alaquas', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 11, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.937600000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 5, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 22.5721, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Riba Roja', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 13.6585, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 966.2381, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 10.663799999999998, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 23.585, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.7878, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Benetusser', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 173.9197, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Elche', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 6.9288, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sedaví', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 23.585, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 7.3887, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 19.881400000000003, 'Nombre de Pràctiques': 7, 'Punt de Destí': 'Rafelbunyol', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 23.585, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 37.499900000000004, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Guadassuar', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 69.7237, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Gandía', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 69.7237, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Gandía', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 10.663799999999998, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 17.7379, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 361.05379999999997, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Montcada i Reixac', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 9.560799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Valencia'}), DefaultMunch(None, {'Distancia': 966.2381, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'Valencia'})]</t>
+        </is>
+      </c>
+      <c r="L57" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Alumne': 'alumno56', 'Pràctica': 'Indenova(Pràctica 6)'})</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="1" t="n">
+        <v>56</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>alumno57</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>TSMR</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>Alginet</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Asesor': '5', 'HelpDesk': '3', 'Instalador': '5', 'Tecnico': '6'})</t>
+        </is>
+      </c>
+      <c r="G58" t="inlineStr"/>
+      <c r="H58" t="inlineStr"/>
+      <c r="I58" t="inlineStr"/>
+      <c r="J58" t="inlineStr"/>
+      <c r="K58" t="inlineStr">
+        <is>
+          <t>[DefaultMunch(None, {'Distancia': 13.950899999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 6, 'Punt de Destí': 'Valencia', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 23.9937, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Fortaleny', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 20.3081, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Massanassa', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 13.950899999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Valencia', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 34.2012, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 20.178900000000002, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Albal', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 57.2663, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 19.4909, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 31.5103, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 19.4909, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 21.792900000000003, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 34.2012, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 24.260099999999998, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paiporta', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 19.4909, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 57.2663, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 31.5103, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 10.4673, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Algemesí', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 21.792900000000003, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 34.2012, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 19.4909, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 380.61190000000005, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Pozuelo de Alarcón', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 34.2012, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 35.7939, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Xàtiva', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 15.867700000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 15.867700000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 56.495599999999996, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Benisanó', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 9.9133, 'Nombre de Pràctiques': 1, 'Punt de Destí': "L'Alcúdia", 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 30.6556, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Mislata', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 25.6662, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 19.4909, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 34.2012, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 34.2012, 'Nombre de Pràctiques': 5, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 8, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 4, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 15.867700000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 21.3029, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sueca', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 21.792900000000003, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 35.4914, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 34.2012, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 36.468900000000005, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Foios', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 28.135099999999998, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Alaquas', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 11, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 21.792900000000003, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 5, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 41.703199999999995, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Riba Roja', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 34.2012, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 13.950899999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 948.793, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 25.6662, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 34.2012, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 7.9038, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 21.8412, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Benetusser', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 147.4786, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Elche', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 34.2012, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 21.9181, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sedaví', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 7.9038, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 35.4914, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 56.400400000000005, 'Nombre de Pràctiques': 7, 'Punt de Destí': 'Rafelbunyol', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 7.9038, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 11.0588, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Guadassuar', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 48.4726, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Gandía', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 48.4726, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Gandía', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 25.6662, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 34.2012, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 15.867700000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 26.9154, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 396.40979999999996, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Montcada i Reixac', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 34.2012, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Alginet'}), DefaultMunch(None, {'Distancia': 948.793, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'Alginet'})]</t>
+        </is>
+      </c>
+      <c r="L58" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Alumne': 'alumno57', 'Pràctica': 'Red902(Pràctica 2)'})</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="1" t="n">
+        <v>57</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>alumno58</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>TSMR</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>Albal</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Asesor': '4', 'HelpDesk': '8', 'Instalador': '9', 'Tecnico': '9'})</t>
+        </is>
+      </c>
+      <c r="G59" t="inlineStr"/>
+      <c r="H59" t="inlineStr"/>
+      <c r="I59" t="inlineStr"/>
+      <c r="J59" t="inlineStr"/>
+      <c r="K59" t="inlineStr">
+        <is>
+          <t>[DefaultMunch(None, {'Distancia': 5.904, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 6, 'Punt de Destí': 'Valencia', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 31.4555, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Fortaleny', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 3.7565, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Massanassa', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 5.904, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Valencia', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 16.428099999999997, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Albal', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 36.9901, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 2.3773, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 13.7403, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 2.3773, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 5.59, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 16.428099999999997, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 6.3576999999999995, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paiporta', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 2.3773, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 36.9901, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 13.7403, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 28.3518, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Algemesí', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 5.59, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 16.428099999999997, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 2.3773, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 374.0283, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Pozuelo de Alarcón', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 16.428099999999997, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 54.4804, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Xàtiva', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 9.9833, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 9.9833, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 36.2194, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Benisanó', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 28.5998, 'Nombre de Pràctiques': 1, 'Punt de Destí': "L'Alcúdia", 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 12.8855, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Mislata', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 8.44, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 2.3773, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 16.428099999999997, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 16.428099999999997, 'Nombre de Pràctiques': 5, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 8, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 4, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 9.9833, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 30.2138, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sueca', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 5.59, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 16.4677, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 16.428099999999997, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 20.3187, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Foios', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.7685, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Alaquas', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 11, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 5.59, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 5, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 28.6172, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Riba Roja', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 16.428099999999997, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 5.904, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 972.572, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 8.44, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 16.428099999999997, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 15.8304, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 4.996, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Benetusser', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 166.1651, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Elche', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 16.428099999999997, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 7.253100000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sedaví', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 15.8304, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 16.4677, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 30.1327, 'Nombre de Pràctiques': 7, 'Punt de Destí': 'Rafelbunyol', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 15.8304, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 29.7454, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Guadassuar', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 61.969199999999994, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Gandía', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 61.969199999999994, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Gandía', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 8.44, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 16.428099999999997, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 9.9833, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 10.4979, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 371.3051, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Montcada i Reixac', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 16.428099999999997, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Albal'}), DefaultMunch(None, {'Distancia': 972.572, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'Albal'})]</t>
+        </is>
+      </c>
+      <c r="L59" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Alumne': 'alumno58', 'Pràctica': 'DYNAMIZATIC(Pràctica 1)'})</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="1" t="n">
+        <v>58</v>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>alumno59</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>TSMR</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>Picassent</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Asesor': '7', 'HelpDesk': '5', 'Instalador': '10', 'Tecnico': '6'})</t>
+        </is>
+      </c>
+      <c r="G60" t="inlineStr"/>
+      <c r="H60" t="inlineStr"/>
+      <c r="I60" t="inlineStr"/>
+      <c r="J60" t="inlineStr"/>
+      <c r="K60" t="inlineStr">
+        <is>
+          <t>[DefaultMunch(None, {'Distancia': 5.1371, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 18.2363, 'Nombre de Pràctiques': 6, 'Punt de Destí': 'Valencia', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 27.827099999999998, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Fortaleny', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 11.629100000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Massanassa', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 5.1371, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 18.2363, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Valencia', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 25.5222, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 9.295, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Albal', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 45.2917, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 8.607, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 18.2363, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 18.2363, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 22.8313, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 8.607, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 13.1139, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 25.5222, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 18.2363, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'València', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 12.5449, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paiporta', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 18.2363, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 8.607, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 45.2917, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 18.2363, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 22.8313, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 24.7234, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Algemesí', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 13.1139, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 25.5222, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 8.607, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 368.6373, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Pozuelo de Alarcón', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 25.5222, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 50.8544, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Xàtiva', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 18.2363, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 18.2363, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 44.521, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Benisanó', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 24.9738, 'Nombre de Pràctiques': 1, 'Punt de Destí': "L'Alcúdia", 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 21.9765, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Mislata', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 13.691600000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 8.607, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 25.5222, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 25.5222, 'Nombre de Pràctiques': 5, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 18.2363, 'Nombre de Pràctiques': 8, 'Punt de Destí': 'València', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 18.2363, 'Nombre de Pràctiques': 4, 'Punt de Destí': 'València', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 26.5854, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sueca', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 13.1139, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 26.8124, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 25.5222, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 27.789900000000003, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Foios', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 16.1605, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Alaquas', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 18.2363, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 18.2363, 'Nombre de Pràctiques': 11, 'Punt de Destí': 'València', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 18.2363, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 13.1139, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 18.2363, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 18.2363, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 18.2363, 'Nombre de Pràctiques': 5, 'Punt de Destí': 'València', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 29.7286, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Riba Roja', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 25.5222, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 18.2363, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 18.2363, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 5.1371, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 967.181, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 13.691600000000001, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 25.5222, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 12.2021, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 13.1622, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Benetusser', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 162.53910000000002, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Elche', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 18.2363, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 18.2363, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 25.5222, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 13.2391, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sedaví', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 18.2363, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 18.2363, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 18.2363, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 18.2363, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 18.2363, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 12.2021, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 26.8124, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 44.4258, 'Nombre de Pràctiques': 7, 'Punt de Destí': 'Rafelbunyol', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 18.2363, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 12.2021, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 26.1193, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Guadassuar', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 58.3408, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Gandía', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 58.3408, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Gandía', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 18.2363, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'València', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 18.2363, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 13.691600000000001, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 18.2363, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 18.2363, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 18.2363, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 18.2363, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 25.5222, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 18.2363, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 384.4352, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Montcada i Reixac', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 25.5222, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Picassent'}), DefaultMunch(None, {'Distancia': 967.181, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'Picassent'})]</t>
+        </is>
+      </c>
+      <c r="L60" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Alumne': 'alumno59', 'Pràctica': 'EtraMufrep(Pràctica 2)'})</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="1" t="n">
+        <v>59</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>alumno60</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>TSMR</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>Catarroja</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Asesor': '9', 'HelpDesk': '9', 'Instalador': '1', 'Tecnico': '4'})</t>
+        </is>
+      </c>
+      <c r="G61" t="inlineStr"/>
+      <c r="H61" t="inlineStr"/>
+      <c r="I61" t="inlineStr"/>
+      <c r="J61" t="inlineStr"/>
+      <c r="K61" t="inlineStr">
+        <is>
+          <t>[DefaultMunch(None, {'Distancia': 6.1035, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 6, 'Punt de Destí': 'Valencia', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 31.6549, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Fortaleny', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 1.2002000000000002, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Massanassa', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 6.1035, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Valencia', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 15.222700000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 2.0949, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Albal', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 35.7846, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 12.534799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 3.3274, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 15.222700000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 5.1522, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paiporta', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 35.7846, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Lliria', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 12.534799999999999, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Quart de Poblet', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 28.551299999999998, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Algemesí', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 3.3274, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 15.222700000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 372.8228, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Pozuelo de Alarcón', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 15.222700000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 54.6799, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Xàtiva', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 10.182799999999999, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 10.182799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 35.014, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Benisanó', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 28.7993, 'Nombre de Pràctiques': 1, 'Punt de Destí': "L'Alcúdia", 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 11.6801, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Mislata', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 10.5417, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 0.0, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Catarroja', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 15.222700000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 15.222700000000001, 'Nombre de Pràctiques': 5, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 8, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 4, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 10.182799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 30.4133, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sueca', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 3.3274, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 15.2623, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 15.222700000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 19.1133, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Foios', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 12.8701, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Alaquas', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 11, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 3.3274, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Alfafar', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 5, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 27.4118, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Riba Roja', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 15.222700000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 6.1035, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Silla', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 971.3665, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 10.5417, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 15.222700000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 16.0299, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 2.7334, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Benetusser', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 166.3646, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Elche', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 15.222700000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 4.2168, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Sedaví', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 16.0299, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 15.2623, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Burjassot', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 28.9272, 'Nombre de Pràctiques': 7, 'Punt de Destí': 'Rafelbunyol', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 16.0299, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Almussafes', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 29.9449, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Guadassuar', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 62.168699999999994, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Gandía', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 62.168699999999994, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Gandía', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 3, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 10.5417, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'Torrent', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 15.222700000000001, 'Nombre de Pràctiques': 2, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 10.182799999999999, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Picassent', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 9.2925, 'Nombre de Pràctiques': 0, 'Punt de Destí': 'València', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 370.0997, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Montcada i Reixac', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 15.222700000000001, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Paterna', 'Punt de Partida': 'Catarroja'}), DefaultMunch(None, {'Distancia': 971.3665, 'Nombre de Pràctiques': 1, 'Punt de Destí': 'Madrid', 'Punt de Partida': 'Catarroja'})]</t>
+        </is>
+      </c>
+      <c r="L61" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Alumne': 'alumno60', 'Pràctica': 'Arrocerias Pons(Pràctica 1)'})</t>
         </is>
       </c>
     </row>

</xml_diff>